<commit_message>
Add weather coloring and routes to main map
</commit_message>
<xml_diff>
--- a/io_in/city_list.xlsx
+++ b/io_in/city_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Coding/roadtrips/io_in/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DBA7F3-F3A8-5C43-BFF1-5C99FDED5194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81242CE6-15F6-224E-9E85-365D4CE20CF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="500" windowWidth="24000" windowHeight="21900" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
   </bookViews>
@@ -1275,13 +1275,6 @@
     <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1297,14 +1290,23 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1623,8 +1625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418BD67C-5132-6942-B406-D98F46E6A0BD}">
   <dimension ref="A1:M121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="G116" sqref="G116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1634,7 +1636,7 @@
     <col min="3" max="3" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.83203125" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="1"/>
-    <col min="6" max="6" width="5.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" style="24" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.1640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1" customWidth="1"/>
@@ -1661,7 +1663,7 @@
       <c r="E1" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="23" t="s">
         <v>217</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -1688,21 +1690,23 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <f>A1+1</f>
+        <f t="shared" ref="A2:A33" si="0">A1+1</f>
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>100</v>
       </c>
       <c r="C2" s="1" t="str">
-        <f>RIGHT(B2,2)</f>
+        <f t="shared" ref="C2:C33" si="1">RIGHT(B2,2)</f>
         <v>AK</v>
       </c>
       <c r="D2" s="5">
         <v>0</v>
       </c>
       <c r="E2" s="6"/>
-      <c r="F2" s="15"/>
+      <c r="F2" s="23">
+        <v>0</v>
+      </c>
       <c r="G2" s="5" t="s">
         <v>128</v>
       </c>
@@ -1721,21 +1725,23 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <f>A2+1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>126</v>
       </c>
       <c r="C3" s="1" t="str">
-        <f>RIGHT(B3,2)</f>
+        <f t="shared" si="1"/>
         <v>AK</v>
       </c>
       <c r="D3" s="5">
         <v>0</v>
       </c>
       <c r="E3" s="6"/>
-      <c r="F3" s="15"/>
+      <c r="F3" s="23">
+        <v>0</v>
+      </c>
       <c r="G3" s="5" t="s">
         <v>125</v>
       </c>
@@ -1754,14 +1760,14 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <f>A3+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>43</v>
       </c>
       <c r="C4" s="1" t="str">
-        <f>RIGHT(B4,2)</f>
+        <f t="shared" si="1"/>
         <v>AL</v>
       </c>
       <c r="D4" s="5">
@@ -1770,7 +1776,7 @@
       <c r="E4" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="F4" s="15"/>
+      <c r="F4" s="23"/>
       <c r="G4" s="5" t="s">
         <v>128</v>
       </c>
@@ -1790,14 +1796,14 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <f>A4+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C5" s="1" t="str">
-        <f>RIGHT(B5,2)</f>
+        <f t="shared" si="1"/>
         <v>AL</v>
       </c>
       <c r="D5" s="5">
@@ -1806,7 +1812,7 @@
       <c r="E5" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="F5" s="15"/>
+      <c r="F5" s="23"/>
       <c r="G5" s="5" t="s">
         <v>125</v>
       </c>
@@ -1823,21 +1829,23 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <f>A5+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>105</v>
       </c>
       <c r="C6" s="1" t="str">
-        <f>RIGHT(B6,2)</f>
+        <f t="shared" si="1"/>
         <v>AR</v>
       </c>
       <c r="D6" s="5">
         <v>0</v>
       </c>
       <c r="E6" s="6"/>
-      <c r="F6" s="15"/>
+      <c r="F6" s="23">
+        <v>0</v>
+      </c>
       <c r="G6" s="5" t="s">
         <v>125</v>
       </c>
@@ -1854,21 +1862,23 @@
     </row>
     <row r="7" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <f>A6+1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>211</v>
       </c>
       <c r="C7" s="1" t="str">
-        <f>RIGHT(B7,2)</f>
+        <f t="shared" si="1"/>
         <v>AZ</v>
       </c>
       <c r="D7" s="12">
         <v>0</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="16"/>
+      <c r="F7" s="24">
+        <v>0</v>
+      </c>
       <c r="G7" s="1" t="s">
         <v>240</v>
       </c>
@@ -1889,21 +1899,23 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <f>A7+1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>77</v>
       </c>
       <c r="C8" s="1" t="str">
-        <f>RIGHT(B8,2)</f>
+        <f t="shared" si="1"/>
         <v>AZ</v>
       </c>
       <c r="D8" s="5">
         <v>1</v>
       </c>
       <c r="E8" s="6"/>
-      <c r="F8" s="15"/>
+      <c r="F8" s="23">
+        <v>0</v>
+      </c>
       <c r="G8" s="5" t="s">
         <v>125</v>
       </c>
@@ -1923,21 +1935,23 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <f>A8+1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>78</v>
       </c>
       <c r="C9" s="1" t="str">
-        <f>RIGHT(B9,2)</f>
+        <f t="shared" si="1"/>
         <v>AZ</v>
       </c>
       <c r="D9" s="5">
         <v>0</v>
       </c>
       <c r="E9" s="6"/>
-      <c r="F9" s="15"/>
+      <c r="F9" s="23">
+        <v>0</v>
+      </c>
       <c r="G9" s="5" t="s">
         <v>128</v>
       </c>
@@ -1957,18 +1971,21 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <f>A9+1</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>212</v>
       </c>
       <c r="C10" s="1" t="str">
-        <f>RIGHT(B10,2)</f>
+        <f t="shared" si="1"/>
         <v>CA</v>
       </c>
       <c r="D10" s="12">
         <v>1</v>
+      </c>
+      <c r="F10" s="24">
+        <v>0</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>240</v>
@@ -1985,21 +2002,23 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <f>A10+1</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C11" s="1" t="str">
-        <f>RIGHT(B11,2)</f>
+        <f t="shared" si="1"/>
         <v>CA</v>
       </c>
       <c r="D11" s="5">
         <v>0</v>
       </c>
       <c r="E11" s="6"/>
-      <c r="F11" s="15"/>
+      <c r="F11" s="23">
+        <v>0</v>
+      </c>
       <c r="G11" s="1" t="s">
         <v>127</v>
       </c>
@@ -2019,14 +2038,14 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <f>A11+1</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C12" s="1" t="str">
-        <f>RIGHT(B12,2)</f>
+        <f t="shared" si="1"/>
         <v>CA</v>
       </c>
       <c r="D12" s="5">
@@ -2035,7 +2054,7 @@
       <c r="E12" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="23">
         <f>1.4+6.7+4.9+6.1+7.9</f>
         <v>27</v>
       </c>
@@ -2058,14 +2077,14 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <f>A12+1</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="1" t="str">
-        <f>RIGHT(B13,2)</f>
+        <f t="shared" si="1"/>
         <v>CA</v>
       </c>
       <c r="D13" s="5">
@@ -2074,7 +2093,7 @@
       <c r="E13" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="23">
         <v>3</v>
       </c>
       <c r="G13" s="1" t="s">
@@ -2096,21 +2115,23 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <f>A13+1</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>81</v>
       </c>
       <c r="C14" s="1" t="str">
-        <f>RIGHT(B14,2)</f>
+        <f t="shared" si="1"/>
         <v>CA</v>
       </c>
       <c r="D14" s="5">
         <v>1</v>
       </c>
       <c r="E14" s="6"/>
-      <c r="F14" s="15"/>
+      <c r="F14" s="23">
+        <v>0</v>
+      </c>
       <c r="G14" s="5" t="s">
         <v>125</v>
       </c>
@@ -2130,14 +2151,14 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <f>A14+1</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>82</v>
       </c>
       <c r="C15" s="1" t="str">
-        <f>RIGHT(B15,2)</f>
+        <f t="shared" si="1"/>
         <v>CA</v>
       </c>
       <c r="D15" s="5">
@@ -2146,9 +2167,9 @@
       <c r="E15" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="F15" s="15">
-        <f>5.2+16.1+9.75</f>
-        <v>31.05</v>
+      <c r="F15" s="23">
+        <f>5.2+16.1+9.8</f>
+        <v>31.1</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>127</v>
@@ -2169,21 +2190,23 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <f>A15+1</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>83</v>
       </c>
       <c r="C16" s="1" t="str">
-        <f>RIGHT(B16,2)</f>
+        <f t="shared" si="1"/>
         <v>CA</v>
       </c>
       <c r="D16" s="5">
         <v>1</v>
       </c>
       <c r="E16" s="6"/>
-      <c r="F16" s="15"/>
+      <c r="F16" s="23">
+        <v>0</v>
+      </c>
       <c r="G16" s="1" t="s">
         <v>127</v>
       </c>
@@ -2203,21 +2226,23 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <f>A16+1</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>84</v>
       </c>
       <c r="C17" s="1" t="str">
-        <f>RIGHT(B17,2)</f>
+        <f t="shared" si="1"/>
         <v>CA</v>
       </c>
       <c r="D17" s="5">
         <v>0</v>
       </c>
       <c r="E17" s="6"/>
-      <c r="F17" s="15"/>
+      <c r="F17" s="23">
+        <v>0</v>
+      </c>
       <c r="G17" s="1" t="s">
         <v>127</v>
       </c>
@@ -2237,17 +2262,20 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <f>A17+1</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>210</v>
       </c>
       <c r="C18" s="1" t="str">
-        <f>RIGHT(B18,2)</f>
+        <f t="shared" si="1"/>
         <v>CA</v>
       </c>
       <c r="D18" s="12">
+        <v>0</v>
+      </c>
+      <c r="F18" s="24">
         <v>0</v>
       </c>
       <c r="G18" s="1" t="s">
@@ -2265,17 +2293,20 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <f>A18+1</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>185</v>
       </c>
       <c r="C19" s="1" t="str">
-        <f>RIGHT(B19,2)</f>
+        <f t="shared" si="1"/>
         <v>CO</v>
       </c>
       <c r="D19" s="12">
+        <v>0</v>
+      </c>
+      <c r="F19" s="24">
         <v>0</v>
       </c>
       <c r="G19" s="1" t="s">
@@ -2293,21 +2324,23 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <f>A19+1</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>86</v>
       </c>
       <c r="C20" s="1" t="str">
-        <f>RIGHT(B20,2)</f>
+        <f t="shared" si="1"/>
         <v>CO</v>
       </c>
       <c r="D20" s="5">
         <v>0</v>
       </c>
       <c r="E20" s="6"/>
-      <c r="F20" s="15"/>
+      <c r="F20" s="23">
+        <v>0</v>
+      </c>
       <c r="G20" s="5" t="s">
         <v>125</v>
       </c>
@@ -2327,14 +2360,14 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <f>A20+1</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C21" s="1" t="str">
-        <f>RIGHT(B21,2)</f>
+        <f t="shared" si="1"/>
         <v>CT</v>
       </c>
       <c r="D21" s="5">
@@ -2343,7 +2376,7 @@
       <c r="E21" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F21" s="15"/>
+      <c r="F21" s="23"/>
       <c r="G21" s="5" t="s">
         <v>125</v>
       </c>
@@ -2363,14 +2396,14 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <f>A21+1</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>186</v>
       </c>
       <c r="C22" s="1" t="str">
-        <f>RIGHT(B22,2)</f>
+        <f t="shared" si="1"/>
         <v>CT</v>
       </c>
       <c r="D22" s="5">
@@ -2379,7 +2412,7 @@
       <c r="E22" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F22" s="15"/>
+      <c r="F22" s="23"/>
       <c r="G22" s="1" t="s">
         <v>128</v>
       </c>
@@ -2396,14 +2429,14 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <f>A22+1</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C23" s="1" t="str">
-        <f>RIGHT(B23,2)</f>
+        <f t="shared" si="1"/>
         <v>DC</v>
       </c>
       <c r="D23" s="5">
@@ -2412,7 +2445,7 @@
       <c r="E23" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="F23" s="15"/>
+      <c r="F23" s="23"/>
       <c r="G23" s="5" t="s">
         <v>125</v>
       </c>
@@ -2434,14 +2467,14 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <f>A23+1</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>47</v>
       </c>
       <c r="C24" s="1" t="str">
-        <f>RIGHT(B24,2)</f>
+        <f t="shared" si="1"/>
         <v>DE</v>
       </c>
       <c r="D24" s="5">
@@ -2450,7 +2483,7 @@
       <c r="E24" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="F24" s="15"/>
+      <c r="F24" s="23"/>
       <c r="G24" s="5" t="s">
         <v>125</v>
       </c>
@@ -2464,14 +2497,14 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <f>A24+1</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C25" s="1" t="str">
-        <f>RIGHT(B25,2)</f>
+        <f t="shared" si="1"/>
         <v>FL</v>
       </c>
       <c r="D25" s="5">
@@ -2480,7 +2513,7 @@
       <c r="E25" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="F25" s="15">
+      <c r="F25" s="23">
         <v>11.5</v>
       </c>
       <c r="G25" s="1" t="s">
@@ -2505,14 +2538,14 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <f>A25+1</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>207</v>
       </c>
       <c r="C26" s="1" t="str">
-        <f>RIGHT(B26,2)</f>
+        <f t="shared" si="1"/>
         <v>FL</v>
       </c>
       <c r="D26" s="5">
@@ -2521,7 +2554,7 @@
       <c r="E26" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="F26" s="15">
+      <c r="F26" s="23">
         <f>7.6+1.3</f>
         <v>8.9</v>
       </c>
@@ -2541,14 +2574,14 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <f>A26+1</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>49</v>
       </c>
       <c r="C27" s="1" t="str">
-        <f>RIGHT(B27,2)</f>
+        <f t="shared" si="1"/>
         <v>FL</v>
       </c>
       <c r="D27" s="5">
@@ -2557,7 +2590,7 @@
       <c r="E27" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="F27" s="15">
+      <c r="F27" s="23">
         <v>14.3</v>
       </c>
       <c r="G27" s="7" t="s">
@@ -2579,14 +2612,14 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <f>A27+1</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C28" s="1" t="str">
-        <f>RIGHT(B28,2)</f>
+        <f t="shared" si="1"/>
         <v>FL</v>
       </c>
       <c r="D28" s="5">
@@ -2595,7 +2628,7 @@
       <c r="E28" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="F28" s="15">
+      <c r="F28" s="23">
         <v>6.1</v>
       </c>
       <c r="G28" s="1" t="s">
@@ -2617,14 +2650,14 @@
     </row>
     <row r="29" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <f>A28+1</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>51</v>
       </c>
       <c r="C29" s="1" t="str">
-        <f>RIGHT(B29,2)</f>
+        <f t="shared" si="1"/>
         <v>FL</v>
       </c>
       <c r="D29" s="5">
@@ -2633,7 +2666,7 @@
       <c r="E29" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="F29" s="15">
+      <c r="F29" s="23">
         <v>5</v>
       </c>
       <c r="G29" s="5" t="s">
@@ -2652,14 +2685,14 @@
     </row>
     <row r="30" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <f>A29+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C30" s="1" t="str">
-        <f>RIGHT(B30,2)</f>
+        <f t="shared" si="1"/>
         <v>FL</v>
       </c>
       <c r="D30" s="5">
@@ -2668,7 +2701,7 @@
       <c r="E30" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="F30" s="15">
+      <c r="F30" s="23">
         <v>7.4</v>
       </c>
       <c r="G30" s="1" t="s">
@@ -2691,14 +2724,14 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <f>A30+1</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C31" s="1" t="str">
-        <f>RIGHT(B31,2)</f>
+        <f t="shared" si="1"/>
         <v>GA</v>
       </c>
       <c r="D31" s="5">
@@ -2707,7 +2740,7 @@
       <c r="E31" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="F31" s="15"/>
+      <c r="F31" s="23"/>
       <c r="G31" s="5" t="s">
         <v>125</v>
       </c>
@@ -2727,14 +2760,14 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <f>A31+1</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>54</v>
       </c>
       <c r="C32" s="1" t="str">
-        <f>RIGHT(B32,2)</f>
+        <f t="shared" si="1"/>
         <v>GA</v>
       </c>
       <c r="D32" s="5">
@@ -2743,7 +2776,7 @@
       <c r="E32" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="F32" s="15"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="5" t="s">
         <v>128</v>
       </c>
@@ -2760,21 +2793,23 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <f>A32+1</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>101</v>
       </c>
       <c r="C33" s="1" t="str">
-        <f>RIGHT(B33,2)</f>
+        <f t="shared" si="1"/>
         <v>HI</v>
       </c>
       <c r="D33" s="5">
         <v>0</v>
       </c>
-      <c r="E33" s="19"/>
-      <c r="F33" s="15"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="23">
+        <v>0</v>
+      </c>
       <c r="G33" s="5" t="s">
         <v>125</v>
       </c>
@@ -2796,14 +2831,14 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <f>A33+1</f>
+        <f t="shared" ref="A34:A65" si="2">A33+1</f>
         <v>33</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C34" s="1" t="str">
-        <f>RIGHT(B34,2)</f>
+        <f t="shared" ref="C34:C65" si="3">RIGHT(B34,2)</f>
         <v>IA</v>
       </c>
       <c r="D34" s="5">
@@ -2812,7 +2847,7 @@
       <c r="E34" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="F34" s="17"/>
+      <c r="F34" s="25"/>
       <c r="G34" s="5" t="s">
         <v>128</v>
       </c>
@@ -2829,14 +2864,14 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <f>A34+1</f>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>104</v>
       </c>
       <c r="C35" s="1" t="str">
-        <f>RIGHT(B35,2)</f>
+        <f t="shared" si="3"/>
         <v>IA</v>
       </c>
       <c r="D35" s="5">
@@ -2845,7 +2880,7 @@
       <c r="E35" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F35" s="15"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="5" t="s">
         <v>125</v>
       </c>
@@ -2862,21 +2897,23 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <f>A35+1</f>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>87</v>
       </c>
       <c r="C36" s="1" t="str">
-        <f>RIGHT(B36,2)</f>
+        <f t="shared" si="3"/>
         <v>ID</v>
       </c>
       <c r="D36" s="5">
         <v>0</v>
       </c>
       <c r="E36" s="6"/>
-      <c r="F36" s="15"/>
+      <c r="F36" s="23">
+        <v>0</v>
+      </c>
       <c r="G36" s="5" t="s">
         <v>125</v>
       </c>
@@ -2893,21 +2930,23 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <f>A36+1</f>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>189</v>
       </c>
       <c r="C37" s="1" t="str">
-        <f>RIGHT(B37,2)</f>
+        <f t="shared" si="3"/>
         <v>ID</v>
       </c>
       <c r="D37" s="5">
         <v>0</v>
       </c>
       <c r="E37" s="6"/>
-      <c r="F37" s="15"/>
+      <c r="F37" s="23">
+        <v>0</v>
+      </c>
       <c r="G37" s="1" t="s">
         <v>128</v>
       </c>
@@ -2921,14 +2960,14 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <f>A37+1</f>
+        <f t="shared" si="2"/>
         <v>37</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C38" s="1" t="str">
-        <f>RIGHT(B38,2)</f>
+        <f t="shared" si="3"/>
         <v>IL</v>
       </c>
       <c r="D38" s="5">
@@ -2937,7 +2976,7 @@
       <c r="E38" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="F38" s="15"/>
+      <c r="F38" s="23"/>
       <c r="G38" s="5" t="s">
         <v>128</v>
       </c>
@@ -2957,14 +2996,14 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <f>A38+1</f>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C39" s="1" t="str">
-        <f>RIGHT(B39,2)</f>
+        <f t="shared" si="3"/>
         <v>IL</v>
       </c>
       <c r="D39" s="5">
@@ -2973,7 +3012,7 @@
       <c r="E39" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F39" s="15"/>
+      <c r="F39" s="23"/>
       <c r="G39" s="5" t="s">
         <v>125</v>
       </c>
@@ -2990,14 +3029,14 @@
     </row>
     <row r="40" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <f>A39+1</f>
+        <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C40" s="1" t="str">
-        <f>RIGHT(B40,2)</f>
+        <f t="shared" si="3"/>
         <v>IN</v>
       </c>
       <c r="D40" s="5">
@@ -3006,7 +3045,7 @@
       <c r="E40" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F40" s="15"/>
+      <c r="F40" s="23"/>
       <c r="G40" s="5" t="s">
         <v>125</v>
       </c>
@@ -3027,14 +3066,14 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <f>A40+1</f>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C41" s="1" t="str">
-        <f>RIGHT(B41,2)</f>
+        <f t="shared" si="3"/>
         <v>KS</v>
       </c>
       <c r="D41" s="5">
@@ -3043,7 +3082,7 @@
       <c r="E41" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F41" s="15"/>
+      <c r="F41" s="23"/>
       <c r="G41" s="5" t="s">
         <v>125</v>
       </c>
@@ -3060,21 +3099,23 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <f>A41+1</f>
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C42" s="1" t="str">
-        <f>RIGHT(B42,2)</f>
+        <f t="shared" si="3"/>
         <v>KS</v>
       </c>
       <c r="D42" s="5">
         <v>0</v>
       </c>
       <c r="E42" s="6"/>
-      <c r="F42" s="15"/>
+      <c r="F42" s="23">
+        <v>0</v>
+      </c>
       <c r="G42" s="5" t="s">
         <v>128</v>
       </c>
@@ -3091,14 +3132,14 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <f>A42+1</f>
+        <f t="shared" si="2"/>
         <v>42</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C43" s="1" t="str">
-        <f>RIGHT(B43,2)</f>
+        <f t="shared" si="3"/>
         <v>KY</v>
       </c>
       <c r="D43" s="5">
@@ -3107,7 +3148,7 @@
       <c r="E43" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F43" s="15"/>
+      <c r="F43" s="23"/>
       <c r="G43" s="5" t="s">
         <v>125</v>
       </c>
@@ -3124,14 +3165,14 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <f>A43+1</f>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C44" s="1" t="str">
-        <f>RIGHT(B44,2)</f>
+        <f t="shared" si="3"/>
         <v>KY</v>
       </c>
       <c r="D44" s="5">
@@ -3140,7 +3181,7 @@
       <c r="E44" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F44" s="15"/>
+      <c r="F44" s="23"/>
       <c r="G44" s="5" t="s">
         <v>128</v>
       </c>
@@ -3160,21 +3201,23 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <f>A44+1</f>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>57</v>
       </c>
       <c r="C45" s="1" t="str">
-        <f>RIGHT(B45,2)</f>
+        <f t="shared" si="3"/>
         <v>LA</v>
       </c>
       <c r="D45" s="5">
         <v>1</v>
       </c>
       <c r="E45" s="6"/>
-      <c r="F45" s="15"/>
+      <c r="F45" s="23">
+        <v>0</v>
+      </c>
       <c r="G45" s="5" t="s">
         <v>125</v>
       </c>
@@ -3191,14 +3234,14 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <f>A45+1</f>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>58</v>
       </c>
       <c r="C46" s="1" t="str">
-        <f>RIGHT(B46,2)</f>
+        <f t="shared" si="3"/>
         <v>LA</v>
       </c>
       <c r="D46" s="5">
@@ -3207,7 +3250,7 @@
       <c r="E46" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="F46" s="15">
+      <c r="F46" s="23">
         <f>5.4+11+7.5</f>
         <v>23.9</v>
       </c>
@@ -3227,14 +3270,14 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <f>A46+1</f>
+        <f t="shared" si="2"/>
         <v>46</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C47" s="1" t="str">
-        <f>RIGHT(B47,2)</f>
+        <f t="shared" si="3"/>
         <v>MA</v>
       </c>
       <c r="D47" s="5">
@@ -3243,7 +3286,7 @@
       <c r="E47" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F47" s="15"/>
+      <c r="F47" s="23"/>
       <c r="G47" s="5" t="s">
         <v>125</v>
       </c>
@@ -3263,14 +3306,14 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <f>A47+1</f>
+        <f t="shared" si="2"/>
         <v>47</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C48" s="1" t="str">
-        <f>RIGHT(B48,2)</f>
+        <f t="shared" si="3"/>
         <v>MD</v>
       </c>
       <c r="D48" s="5">
@@ -3279,7 +3322,7 @@
       <c r="E48" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="F48" s="15"/>
+      <c r="F48" s="23"/>
       <c r="G48" s="5" t="s">
         <v>125</v>
       </c>
@@ -3296,14 +3339,14 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <f>A48+1</f>
+        <f t="shared" si="2"/>
         <v>48</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>60</v>
       </c>
       <c r="C49" s="1" t="str">
-        <f>RIGHT(B49,2)</f>
+        <f t="shared" si="3"/>
         <v>MD</v>
       </c>
       <c r="D49" s="5">
@@ -3312,7 +3355,7 @@
       <c r="E49" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="F49" s="15"/>
+      <c r="F49" s="23"/>
       <c r="G49" s="5" t="s">
         <v>128</v>
       </c>
@@ -3332,14 +3375,14 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <f>A49+1</f>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C50" s="1" t="str">
-        <f>RIGHT(B50,2)</f>
+        <f t="shared" si="3"/>
         <v>ME</v>
       </c>
       <c r="D50" s="5">
@@ -3348,7 +3391,7 @@
       <c r="E50" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F50" s="15"/>
+      <c r="F50" s="23"/>
       <c r="G50" s="5" t="s">
         <v>125</v>
       </c>
@@ -3365,14 +3408,14 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <f>A50+1</f>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C51" s="1" t="str">
-        <f>RIGHT(B51,2)</f>
+        <f t="shared" si="3"/>
         <v>ME</v>
       </c>
       <c r="D51" s="5">
@@ -3381,7 +3424,7 @@
       <c r="E51" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F51" s="15"/>
+      <c r="F51" s="23"/>
       <c r="G51" s="5" t="s">
         <v>128</v>
       </c>
@@ -3398,14 +3441,14 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <f>A51+1</f>
+        <f t="shared" si="2"/>
         <v>51</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C52" s="1" t="str">
-        <f>RIGHT(B52,2)</f>
+        <f t="shared" si="3"/>
         <v>MI</v>
       </c>
       <c r="D52" s="5">
@@ -3414,7 +3457,7 @@
       <c r="E52" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="F52" s="15"/>
+      <c r="F52" s="23"/>
       <c r="G52" s="5" t="s">
         <v>128</v>
       </c>
@@ -3434,14 +3477,14 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <f>A52+1</f>
+        <f t="shared" si="2"/>
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C53" s="1" t="str">
-        <f>RIGHT(B53,2)</f>
+        <f t="shared" si="3"/>
         <v>MI</v>
       </c>
       <c r="D53" s="5">
@@ -3450,7 +3493,7 @@
       <c r="E53" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="F53" s="15"/>
+      <c r="F53" s="23"/>
       <c r="G53" s="1" t="s">
         <v>127</v>
       </c>
@@ -3470,14 +3513,14 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
-        <f>A53+1</f>
+        <f t="shared" si="2"/>
         <v>53</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C54" s="1" t="str">
-        <f>RIGHT(B54,2)</f>
+        <f t="shared" si="3"/>
         <v>MI</v>
       </c>
       <c r="D54" s="5">
@@ -3486,7 +3529,7 @@
       <c r="E54" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="F54" s="15"/>
+      <c r="F54" s="23"/>
       <c r="G54" s="5" t="s">
         <v>125</v>
       </c>
@@ -3503,17 +3546,20 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <f>A54+1</f>
+        <f t="shared" si="2"/>
         <v>54</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C55" s="1" t="str">
-        <f>RIGHT(B55,2)</f>
+        <f t="shared" si="3"/>
         <v>MN</v>
       </c>
       <c r="D55" s="12">
+        <v>0</v>
+      </c>
+      <c r="F55" s="24">
         <v>0</v>
       </c>
       <c r="G55" s="1" t="s">
@@ -3531,21 +3577,23 @@
     </row>
     <row r="56" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <f>A55+1</f>
+        <f t="shared" si="2"/>
         <v>55</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C56" s="1" t="str">
-        <f>RIGHT(B56,2)</f>
+        <f t="shared" si="3"/>
         <v>MN</v>
       </c>
       <c r="D56" s="5">
         <v>0</v>
       </c>
       <c r="E56" s="6"/>
-      <c r="F56" s="15"/>
+      <c r="F56" s="23">
+        <v>0</v>
+      </c>
       <c r="G56" s="5" t="s">
         <v>125</v>
       </c>
@@ -3566,14 +3614,14 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
-        <f>A56+1</f>
+        <f t="shared" si="2"/>
         <v>56</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C57" s="1" t="str">
-        <f>RIGHT(B57,2)</f>
+        <f t="shared" si="3"/>
         <v>MO</v>
       </c>
       <c r="D57" s="5">
@@ -3582,7 +3630,7 @@
       <c r="E57" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F57" s="15"/>
+      <c r="F57" s="23"/>
       <c r="G57" s="5" t="s">
         <v>125</v>
       </c>
@@ -3599,14 +3647,14 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
-        <f>A57+1</f>
+        <f t="shared" si="2"/>
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C58" s="1" t="str">
-        <f>RIGHT(B58,2)</f>
+        <f t="shared" si="3"/>
         <v>MO</v>
       </c>
       <c r="D58" s="5">
@@ -3615,7 +3663,7 @@
       <c r="E58" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F58" s="15"/>
+      <c r="F58" s="23"/>
       <c r="G58" s="1" t="s">
         <v>127</v>
       </c>
@@ -3635,14 +3683,14 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
-        <f>A58+1</f>
+        <f t="shared" si="2"/>
         <v>58</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C59" s="1" t="str">
-        <f>RIGHT(B59,2)</f>
+        <f t="shared" si="3"/>
         <v>MO</v>
       </c>
       <c r="D59" s="5">
@@ -3667,28 +3715,30 @@
       <c r="K59" s="13">
         <v>38.627002500000003</v>
       </c>
-      <c r="L59" s="27"/>
+      <c r="L59" s="22"/>
       <c r="M59" s="1" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
-        <f>A59+1</f>
+        <f t="shared" si="2"/>
         <v>59</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>61</v>
       </c>
       <c r="C60" s="1" t="str">
-        <f>RIGHT(B60,2)</f>
+        <f t="shared" si="3"/>
         <v>MS</v>
       </c>
       <c r="D60" s="5">
         <v>1</v>
       </c>
       <c r="E60" s="6"/>
-      <c r="F60" s="15"/>
+      <c r="F60" s="23">
+        <v>0</v>
+      </c>
       <c r="G60" s="5" t="s">
         <v>125</v>
       </c>
@@ -3705,21 +3755,23 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
-        <f>A60+1</f>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>88</v>
       </c>
       <c r="C61" s="1" t="str">
-        <f>RIGHT(B61,2)</f>
+        <f t="shared" si="3"/>
         <v>MT</v>
       </c>
       <c r="D61" s="5">
         <v>0</v>
       </c>
       <c r="E61" s="6"/>
-      <c r="F61" s="15"/>
+      <c r="F61" s="23">
+        <v>0</v>
+      </c>
       <c r="G61" s="5" t="s">
         <v>128</v>
       </c>
@@ -3736,17 +3788,20 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
-        <f>A61+1</f>
+        <f t="shared" si="2"/>
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>213</v>
       </c>
       <c r="C62" s="1" t="str">
-        <f>RIGHT(B62,2)</f>
+        <f t="shared" si="3"/>
         <v>MT</v>
       </c>
       <c r="D62" s="12">
+        <v>0</v>
+      </c>
+      <c r="F62" s="24">
         <v>0</v>
       </c>
       <c r="G62" s="1" t="s">
@@ -3764,21 +3819,23 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
-        <f>A62+1</f>
+        <f t="shared" si="2"/>
         <v>62</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>89</v>
       </c>
       <c r="C63" s="1" t="str">
-        <f>RIGHT(B63,2)</f>
+        <f t="shared" si="3"/>
         <v>MT</v>
       </c>
       <c r="D63" s="5">
         <v>0</v>
       </c>
       <c r="E63" s="6"/>
-      <c r="F63" s="15"/>
+      <c r="F63" s="23">
+        <v>0</v>
+      </c>
       <c r="G63" s="5" t="s">
         <v>125</v>
       </c>
@@ -3795,14 +3852,14 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
-        <f>A63+1</f>
+        <f t="shared" si="2"/>
         <v>63</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>63</v>
       </c>
       <c r="C64" s="1" t="str">
-        <f>RIGHT(B64,2)</f>
+        <f t="shared" si="3"/>
         <v>NC</v>
       </c>
       <c r="D64" s="5">
@@ -3811,7 +3868,7 @@
       <c r="E64" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="F64" s="15"/>
+      <c r="F64" s="23"/>
       <c r="G64" s="5" t="s">
         <v>128</v>
       </c>
@@ -3831,14 +3888,14 @@
     </row>
     <row r="65" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
-        <f>A64+1</f>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>62</v>
       </c>
       <c r="C65" s="1" t="str">
-        <f>RIGHT(B65,2)</f>
+        <f t="shared" si="3"/>
         <v>NC</v>
       </c>
       <c r="D65" s="5">
@@ -3847,7 +3904,7 @@
       <c r="E65" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="F65" s="15"/>
+      <c r="F65" s="23"/>
       <c r="G65" s="5" t="s">
         <v>125</v>
       </c>
@@ -3868,21 +3925,23 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
-        <f>A65+1</f>
+        <f t="shared" ref="A66:A97" si="4">A65+1</f>
         <v>65</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C66" s="1" t="str">
-        <f>RIGHT(B66,2)</f>
+        <f t="shared" ref="C66:C97" si="5">RIGHT(B66,2)</f>
         <v>ND</v>
       </c>
       <c r="D66" s="5">
         <v>0</v>
       </c>
       <c r="E66" s="6"/>
-      <c r="F66" s="15"/>
+      <c r="F66" s="23">
+        <v>0</v>
+      </c>
       <c r="G66" s="5" t="s">
         <v>125</v>
       </c>
@@ -3899,21 +3958,23 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
-        <f>A66+1</f>
+        <f t="shared" si="4"/>
         <v>66</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C67" s="1" t="str">
-        <f>RIGHT(B67,2)</f>
+        <f t="shared" si="5"/>
         <v>ND</v>
       </c>
       <c r="D67" s="5">
         <v>0</v>
       </c>
       <c r="E67" s="6"/>
-      <c r="F67" s="15"/>
+      <c r="F67" s="23">
+        <v>0</v>
+      </c>
       <c r="G67" s="5" t="s">
         <v>128</v>
       </c>
@@ -3930,14 +3991,14 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
-        <f>A67+1</f>
+        <f t="shared" si="4"/>
         <v>67</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C68" s="1" t="str">
-        <f>RIGHT(B68,2)</f>
+        <f t="shared" si="5"/>
         <v>NE</v>
       </c>
       <c r="D68" s="5">
@@ -3946,7 +4007,7 @@
       <c r="E68" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F68" s="15"/>
+      <c r="F68" s="23"/>
       <c r="G68" s="5" t="s">
         <v>125</v>
       </c>
@@ -3963,14 +4024,14 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
-        <f>A68+1</f>
+        <f t="shared" si="4"/>
         <v>68</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C69" s="1" t="str">
-        <f>RIGHT(B69,2)</f>
+        <f t="shared" si="5"/>
         <v>NE</v>
       </c>
       <c r="D69" s="5">
@@ -3979,7 +4040,7 @@
       <c r="E69" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F69" s="15"/>
+      <c r="F69" s="23"/>
       <c r="G69" s="5" t="s">
         <v>128</v>
       </c>
@@ -3996,14 +4057,14 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
-        <f>A69+1</f>
+        <f t="shared" si="4"/>
         <v>69</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C70" s="1" t="str">
-        <f>RIGHT(B70,2)</f>
+        <f t="shared" si="5"/>
         <v>NH</v>
       </c>
       <c r="D70" s="5">
@@ -4012,7 +4073,7 @@
       <c r="E70" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F70" s="15"/>
+      <c r="F70" s="23"/>
       <c r="G70" s="5" t="s">
         <v>125</v>
       </c>
@@ -4029,14 +4090,14 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
-        <f>A70+1</f>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>129</v>
       </c>
       <c r="C71" s="1" t="str">
-        <f>RIGHT(B71,2)</f>
+        <f t="shared" si="5"/>
         <v>NH</v>
       </c>
       <c r="D71" s="5">
@@ -4045,7 +4106,7 @@
       <c r="E71" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F71" s="15"/>
+      <c r="F71" s="23"/>
       <c r="G71" s="1" t="s">
         <v>128</v>
       </c>
@@ -4059,21 +4120,23 @@
     </row>
     <row r="72" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
-        <f>A71+1</f>
+        <f t="shared" si="4"/>
         <v>71</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>182</v>
       </c>
       <c r="C72" s="1" t="str">
-        <f>RIGHT(B72,2)</f>
+        <f t="shared" si="5"/>
         <v>NJ</v>
       </c>
       <c r="D72" s="5">
         <v>0</v>
       </c>
       <c r="E72" s="6"/>
-      <c r="F72" s="15"/>
+      <c r="F72" s="23">
+        <v>0</v>
+      </c>
       <c r="G72" s="1" t="s">
         <v>128</v>
       </c>
@@ -4092,14 +4155,14 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
-        <f>A72+1</f>
+        <f t="shared" si="4"/>
         <v>72</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C73" s="1" t="str">
-        <f>RIGHT(B73,2)</f>
+        <f t="shared" si="5"/>
         <v>NJ</v>
       </c>
       <c r="D73" s="5">
@@ -4108,7 +4171,7 @@
       <c r="E73" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F73" s="15"/>
+      <c r="F73" s="23"/>
       <c r="G73" s="5" t="s">
         <v>125</v>
       </c>
@@ -4125,14 +4188,14 @@
     </row>
     <row r="74" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
-        <f>A73+1</f>
+        <f t="shared" si="4"/>
         <v>73</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>90</v>
       </c>
       <c r="C74" s="1" t="str">
-        <f>RIGHT(B74,2)</f>
+        <f t="shared" si="5"/>
         <v>NM</v>
       </c>
       <c r="D74" s="5">
@@ -4141,7 +4204,7 @@
       <c r="E74" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="F74" s="15"/>
+      <c r="F74" s="23"/>
       <c r="G74" s="5" t="s">
         <v>128</v>
       </c>
@@ -4160,14 +4223,14 @@
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
-        <f>A74+1</f>
+        <f t="shared" si="4"/>
         <v>74</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>106</v>
       </c>
       <c r="C75" s="1" t="str">
-        <f>RIGHT(B75,2)</f>
+        <f t="shared" si="5"/>
         <v>NM</v>
       </c>
       <c r="D75" s="5">
@@ -4176,7 +4239,7 @@
       <c r="E75" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="F75" s="15"/>
+      <c r="F75" s="23"/>
       <c r="G75" s="5" t="s">
         <v>125</v>
       </c>
@@ -4193,14 +4256,14 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
-        <f>A75+1</f>
+        <f t="shared" si="4"/>
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>123</v>
       </c>
       <c r="C76" s="1" t="str">
-        <f>RIGHT(B76,2)</f>
+        <f t="shared" si="5"/>
         <v>NM</v>
       </c>
       <c r="D76" s="5">
@@ -4209,7 +4272,7 @@
       <c r="E76" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="F76" s="15"/>
+      <c r="F76" s="23"/>
       <c r="G76" s="1" t="s">
         <v>240</v>
       </c>
@@ -4223,21 +4286,23 @@
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
-        <f>A76+1</f>
+        <f t="shared" si="4"/>
         <v>76</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>92</v>
       </c>
       <c r="C77" s="1" t="str">
-        <f>RIGHT(B77,2)</f>
+        <f t="shared" si="5"/>
         <v>NV</v>
       </c>
       <c r="D77" s="5">
         <v>0</v>
       </c>
       <c r="E77" s="6"/>
-      <c r="F77" s="15"/>
+      <c r="F77" s="23">
+        <v>0</v>
+      </c>
       <c r="G77" s="5" t="s">
         <v>125</v>
       </c>
@@ -4254,14 +4319,14 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
-        <f>A77+1</f>
+        <f t="shared" si="4"/>
         <v>77</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>91</v>
       </c>
       <c r="C78" s="1" t="str">
-        <f>RIGHT(B78,2)</f>
+        <f t="shared" si="5"/>
         <v>NV</v>
       </c>
       <c r="D78" s="5">
@@ -4270,7 +4335,7 @@
       <c r="E78" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="F78" s="15"/>
+      <c r="F78" s="23"/>
       <c r="G78" s="5" t="s">
         <v>128</v>
       </c>
@@ -4290,14 +4355,14 @@
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
-        <f>A78+1</f>
+        <f t="shared" si="4"/>
         <v>78</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C79" s="1" t="str">
-        <f>RIGHT(B79,2)</f>
+        <f t="shared" si="5"/>
         <v>NY</v>
       </c>
       <c r="D79" s="5">
@@ -4306,7 +4371,7 @@
       <c r="E79" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F79" s="15"/>
+      <c r="F79" s="23"/>
       <c r="G79" s="5" t="s">
         <v>125</v>
       </c>
@@ -4323,14 +4388,14 @@
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
-        <f>A79+1</f>
+        <f t="shared" si="4"/>
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C80" s="1" t="str">
-        <f>RIGHT(B80,2)</f>
+        <f t="shared" si="5"/>
         <v>NY</v>
       </c>
       <c r="D80" s="5">
@@ -4339,7 +4404,7 @@
       <c r="E80" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F80" s="15"/>
+      <c r="F80" s="23"/>
       <c r="G80" s="1" t="s">
         <v>127</v>
       </c>
@@ -4359,14 +4424,14 @@
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
-        <f>A80+1</f>
+        <f t="shared" si="4"/>
         <v>80</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>103</v>
       </c>
       <c r="C81" s="1" t="str">
-        <f>RIGHT(B81,2)</f>
+        <f t="shared" si="5"/>
         <v>NY</v>
       </c>
       <c r="D81" s="5">
@@ -4375,7 +4440,7 @@
       <c r="E81" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="F81" s="15">
+      <c r="F81" s="23">
         <f>7.4+8.9+9.2+6.7+11.6+11.5+1.6</f>
         <v>56.900000000000006</v>
       </c>
@@ -4401,14 +4466,14 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
-        <f>A81+1</f>
+        <f t="shared" si="4"/>
         <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C82" s="1" t="str">
-        <f>RIGHT(B82,2)</f>
+        <f t="shared" si="5"/>
         <v>NY</v>
       </c>
       <c r="D82" s="5">
@@ -4417,7 +4482,7 @@
       <c r="E82" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F82" s="15"/>
+      <c r="F82" s="23"/>
       <c r="G82" s="1" t="s">
         <v>127</v>
       </c>
@@ -4437,14 +4502,14 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
-        <f>A82+1</f>
+        <f t="shared" si="4"/>
         <v>82</v>
       </c>
       <c r="B83" s="5" t="s">
         <v>35</v>
       </c>
       <c r="C83" s="1" t="str">
-        <f>RIGHT(B83,2)</f>
+        <f t="shared" si="5"/>
         <v>OH</v>
       </c>
       <c r="D83" s="5">
@@ -4453,7 +4518,7 @@
       <c r="E83" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F83" s="15"/>
+      <c r="F83" s="23"/>
       <c r="G83" s="5" t="s">
         <v>128</v>
       </c>
@@ -4473,14 +4538,14 @@
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
-        <f>A83+1</f>
+        <f t="shared" si="4"/>
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C84" s="1" t="str">
-        <f>RIGHT(B84,2)</f>
+        <f t="shared" si="5"/>
         <v>OH</v>
       </c>
       <c r="D84" s="5">
@@ -4489,7 +4554,7 @@
       <c r="E84" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="F84" s="15"/>
+      <c r="F84" s="23"/>
       <c r="G84" s="1" t="s">
         <v>127</v>
       </c>
@@ -4509,14 +4574,14 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
-        <f>A84+1</f>
+        <f t="shared" si="4"/>
         <v>84</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C85" s="1" t="str">
-        <f>RIGHT(B85,2)</f>
+        <f t="shared" si="5"/>
         <v>OH</v>
       </c>
       <c r="D85" s="5">
@@ -4525,7 +4590,7 @@
       <c r="E85" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F85" s="15"/>
+      <c r="F85" s="23"/>
       <c r="G85" s="5" t="s">
         <v>125</v>
       </c>
@@ -4545,21 +4610,23 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
-        <f>A85+1</f>
+        <f t="shared" si="4"/>
         <v>85</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C86" s="1" t="str">
-        <f>RIGHT(B86,2)</f>
+        <f t="shared" si="5"/>
         <v>OK</v>
       </c>
       <c r="D86" s="5">
         <v>0</v>
       </c>
       <c r="E86" s="6"/>
-      <c r="F86" s="15"/>
+      <c r="F86" s="23">
+        <v>0</v>
+      </c>
       <c r="G86" s="5" t="s">
         <v>125</v>
       </c>
@@ -4579,21 +4646,23 @@
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
-        <f>A86+1</f>
+        <f t="shared" si="4"/>
         <v>86</v>
       </c>
       <c r="B87" s="5" t="s">
         <v>41</v>
       </c>
       <c r="C87" s="1" t="str">
-        <f>RIGHT(B87,2)</f>
+        <f t="shared" si="5"/>
         <v>OK</v>
       </c>
       <c r="D87" s="5">
         <v>0</v>
       </c>
       <c r="E87" s="6"/>
-      <c r="F87" s="15"/>
+      <c r="F87" s="23">
+        <v>0</v>
+      </c>
       <c r="G87" s="5" t="s">
         <v>128</v>
       </c>
@@ -4613,21 +4682,23 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
-        <f>A87+1</f>
+        <f t="shared" si="4"/>
         <v>87</v>
       </c>
       <c r="B88" s="5" t="s">
         <v>94</v>
       </c>
       <c r="C88" s="1" t="str">
-        <f>RIGHT(B88,2)</f>
+        <f t="shared" si="5"/>
         <v>OR</v>
       </c>
       <c r="D88" s="5">
         <v>1</v>
       </c>
       <c r="E88" s="6"/>
-      <c r="F88" s="15"/>
+      <c r="F88" s="23">
+        <v>0</v>
+      </c>
       <c r="G88" s="5" t="s">
         <v>128</v>
       </c>
@@ -4647,21 +4718,23 @@
     </row>
     <row r="89" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
-        <f>A88+1</f>
+        <f t="shared" si="4"/>
         <v>88</v>
       </c>
       <c r="B89" s="5" t="s">
         <v>93</v>
       </c>
       <c r="C89" s="1" t="str">
-        <f>RIGHT(B89,2)</f>
+        <f t="shared" si="5"/>
         <v>OR</v>
       </c>
       <c r="D89" s="5">
         <v>0</v>
       </c>
       <c r="E89" s="6"/>
-      <c r="F89" s="15"/>
+      <c r="F89" s="23">
+        <v>0</v>
+      </c>
       <c r="G89" s="5" t="s">
         <v>125</v>
       </c>
@@ -4680,14 +4753,14 @@
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
-        <f>A89+1</f>
+        <f t="shared" si="4"/>
         <v>89</v>
       </c>
       <c r="B90" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C90" s="1" t="str">
-        <f>RIGHT(B90,2)</f>
+        <f t="shared" si="5"/>
         <v>PA</v>
       </c>
       <c r="D90" s="5">
@@ -4696,7 +4769,7 @@
       <c r="E90" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F90" s="15"/>
+      <c r="F90" s="23"/>
       <c r="G90" s="5" t="s">
         <v>125</v>
       </c>
@@ -4713,14 +4786,14 @@
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
-        <f>A90+1</f>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
       <c r="B91" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C91" s="1" t="str">
-        <f>RIGHT(B91,2)</f>
+        <f t="shared" si="5"/>
         <v>PA</v>
       </c>
       <c r="D91" s="5">
@@ -4729,7 +4802,7 @@
       <c r="E91" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F91" s="15"/>
+      <c r="F91" s="23"/>
       <c r="G91" s="5" t="s">
         <v>128</v>
       </c>
@@ -4752,14 +4825,14 @@
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
-        <f>A91+1</f>
+        <f t="shared" si="4"/>
         <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C92" s="1" t="str">
-        <f>RIGHT(B92,2)</f>
+        <f t="shared" si="5"/>
         <v>PA</v>
       </c>
       <c r="D92" s="5">
@@ -4768,7 +4841,7 @@
       <c r="E92" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="F92" s="15"/>
+      <c r="F92" s="23"/>
       <c r="G92" s="1" t="s">
         <v>127</v>
       </c>
@@ -4788,21 +4861,23 @@
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
-        <f>A92+1</f>
+        <f t="shared" si="4"/>
         <v>92</v>
       </c>
       <c r="B93" s="5" t="s">
         <v>102</v>
       </c>
       <c r="C93" s="1" t="str">
-        <f>RIGHT(B93,2)</f>
+        <f t="shared" si="5"/>
         <v>PR</v>
       </c>
       <c r="D93" s="5">
         <v>1</v>
       </c>
       <c r="E93" s="6"/>
-      <c r="F93" s="15"/>
+      <c r="F93" s="23">
+        <v>0</v>
+      </c>
       <c r="G93" s="5" t="s">
         <v>125</v>
       </c>
@@ -4824,14 +4899,14 @@
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
-        <f>A93+1</f>
+        <f t="shared" si="4"/>
         <v>93</v>
       </c>
       <c r="B94" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C94" s="1" t="str">
-        <f>RIGHT(B94,2)</f>
+        <f t="shared" si="5"/>
         <v>RI</v>
       </c>
       <c r="D94" s="5">
@@ -4840,7 +4915,7 @@
       <c r="E94" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F94" s="15"/>
+      <c r="F94" s="23"/>
       <c r="G94" s="5" t="s">
         <v>125</v>
       </c>
@@ -4860,14 +4935,14 @@
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
-        <f>A94+1</f>
+        <f t="shared" si="4"/>
         <v>94</v>
       </c>
       <c r="B95" s="5" t="s">
         <v>65</v>
       </c>
       <c r="C95" s="1" t="str">
-        <f>RIGHT(B95,2)</f>
+        <f t="shared" si="5"/>
         <v>SC</v>
       </c>
       <c r="D95" s="5">
@@ -4876,7 +4951,7 @@
       <c r="E95" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="F95" s="15"/>
+      <c r="F95" s="23"/>
       <c r="G95" s="5" t="s">
         <v>128</v>
       </c>
@@ -4893,14 +4968,14 @@
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
-        <f>A95+1</f>
+        <f t="shared" si="4"/>
         <v>95</v>
       </c>
       <c r="B96" s="5" t="s">
         <v>66</v>
       </c>
       <c r="C96" s="1" t="str">
-        <f>RIGHT(B96,2)</f>
+        <f t="shared" si="5"/>
         <v>SC</v>
       </c>
       <c r="D96" s="5">
@@ -4909,7 +4984,7 @@
       <c r="E96" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="F96" s="15"/>
+      <c r="F96" s="23"/>
       <c r="G96" s="5" t="s">
         <v>125</v>
       </c>
@@ -4926,21 +5001,23 @@
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
-        <f>A96+1</f>
+        <f t="shared" si="4"/>
         <v>96</v>
       </c>
       <c r="B97" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C97" s="1" t="str">
-        <f>RIGHT(B97,2)</f>
+        <f t="shared" si="5"/>
         <v>SD</v>
       </c>
       <c r="D97" s="5">
         <v>0</v>
       </c>
       <c r="E97" s="6"/>
-      <c r="F97" s="15"/>
+      <c r="F97" s="23">
+        <v>0</v>
+      </c>
       <c r="G97" s="5" t="s">
         <v>125</v>
       </c>
@@ -4957,21 +5034,23 @@
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
-        <f>A97+1</f>
+        <f t="shared" ref="A98:A121" si="6">A97+1</f>
         <v>97</v>
       </c>
       <c r="B98" s="5" t="s">
         <v>38</v>
       </c>
       <c r="C98" s="1" t="str">
-        <f>RIGHT(B98,2)</f>
+        <f t="shared" ref="C98:C121" si="7">RIGHT(B98,2)</f>
         <v>SD</v>
       </c>
       <c r="D98" s="5">
         <v>0</v>
       </c>
       <c r="E98" s="6"/>
-      <c r="F98" s="15"/>
+      <c r="F98" s="23">
+        <v>0</v>
+      </c>
       <c r="G98" s="5" t="s">
         <v>128</v>
       </c>
@@ -4988,14 +5067,14 @@
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
-        <f>A98+1</f>
+        <f t="shared" si="6"/>
         <v>98</v>
       </c>
       <c r="B99" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C99" s="1" t="str">
-        <f>RIGHT(B99,2)</f>
+        <f t="shared" si="7"/>
         <v>TN</v>
       </c>
       <c r="D99" s="5">
@@ -5004,7 +5083,7 @@
       <c r="E99" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="F99" s="15"/>
+      <c r="F99" s="23"/>
       <c r="G99" s="1" t="s">
         <v>240</v>
       </c>
@@ -5024,21 +5103,23 @@
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
-        <f>A99+1</f>
+        <f t="shared" si="6"/>
         <v>99</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>68</v>
       </c>
       <c r="C100" s="1" t="str">
-        <f>RIGHT(B100,2)</f>
+        <f t="shared" si="7"/>
         <v>TN</v>
       </c>
       <c r="D100" s="5">
         <v>0</v>
       </c>
       <c r="E100" s="6"/>
-      <c r="F100" s="15"/>
+      <c r="F100" s="23">
+        <v>0</v>
+      </c>
       <c r="G100" s="1" t="s">
         <v>128</v>
       </c>
@@ -5058,14 +5139,14 @@
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
-        <f>A100+1</f>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="B101" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C101" s="1" t="str">
-        <f>RIGHT(B101,2)</f>
+        <f t="shared" si="7"/>
         <v>TN</v>
       </c>
       <c r="D101" s="5">
@@ -5074,7 +5155,7 @@
       <c r="E101" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="F101" s="15"/>
+      <c r="F101" s="23"/>
       <c r="G101" s="5" t="s">
         <v>125</v>
       </c>
@@ -5094,21 +5175,23 @@
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
-        <f>A101+1</f>
+        <f t="shared" si="6"/>
         <v>101</v>
       </c>
       <c r="B102" s="5" t="s">
         <v>69</v>
       </c>
       <c r="C102" s="1" t="str">
-        <f>RIGHT(B102,2)</f>
+        <f t="shared" si="7"/>
         <v>TX</v>
       </c>
       <c r="D102" s="5">
         <v>1</v>
       </c>
       <c r="E102" s="6"/>
-      <c r="F102" s="15"/>
+      <c r="F102" s="23">
+        <v>0</v>
+      </c>
       <c r="G102" s="5" t="s">
         <v>125</v>
       </c>
@@ -5128,21 +5211,23 @@
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
-        <f>A102+1</f>
+        <f t="shared" si="6"/>
         <v>102</v>
       </c>
       <c r="B103" s="5" t="s">
         <v>70</v>
       </c>
       <c r="C103" s="1" t="str">
-        <f>RIGHT(B103,2)</f>
+        <f t="shared" si="7"/>
         <v>TX</v>
       </c>
       <c r="D103" s="5">
         <v>1</v>
       </c>
       <c r="E103" s="6"/>
-      <c r="F103" s="15"/>
+      <c r="F103" s="23">
+        <v>0</v>
+      </c>
       <c r="G103" s="5" t="s">
         <v>128</v>
       </c>
@@ -5162,21 +5247,23 @@
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
-        <f>A103+1</f>
+        <f t="shared" si="6"/>
         <v>103</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C104" s="1" t="str">
-        <f>RIGHT(B104,2)</f>
+        <f t="shared" si="7"/>
         <v>TX</v>
       </c>
       <c r="D104" s="5">
         <v>1</v>
       </c>
       <c r="E104" s="6"/>
-      <c r="F104" s="15"/>
+      <c r="F104" s="23">
+        <v>0</v>
+      </c>
       <c r="G104" s="1" t="s">
         <v>127</v>
       </c>
@@ -5196,21 +5283,23 @@
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
-        <f>A104+1</f>
+        <f t="shared" si="6"/>
         <v>104</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C105" s="1" t="str">
-        <f>RIGHT(B105,2)</f>
+        <f t="shared" si="7"/>
         <v>TX</v>
       </c>
       <c r="D105" s="5">
         <v>1</v>
       </c>
       <c r="E105" s="6"/>
-      <c r="F105" s="15"/>
+      <c r="F105" s="23">
+        <v>0</v>
+      </c>
       <c r="G105" s="1" t="s">
         <v>127</v>
       </c>
@@ -5233,21 +5322,23 @@
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
-        <f>A105+1</f>
+        <f t="shared" si="6"/>
         <v>105</v>
       </c>
       <c r="B106" s="5" t="s">
         <v>187</v>
       </c>
       <c r="C106" s="1" t="str">
-        <f>RIGHT(B106,2)</f>
+        <f t="shared" si="7"/>
         <v>UT</v>
       </c>
       <c r="D106" s="5">
         <v>0</v>
       </c>
       <c r="E106" s="6"/>
-      <c r="F106" s="15"/>
+      <c r="F106" s="23">
+        <v>0</v>
+      </c>
       <c r="G106" s="1" t="s">
         <v>128</v>
       </c>
@@ -5261,21 +5352,23 @@
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
-        <f>A106+1</f>
+        <f t="shared" si="6"/>
         <v>106</v>
       </c>
       <c r="B107" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C107" s="1" t="str">
-        <f>RIGHT(B107,2)</f>
+        <f t="shared" si="7"/>
         <v>UT</v>
       </c>
       <c r="D107" s="5">
         <v>0</v>
       </c>
       <c r="E107" s="6"/>
-      <c r="F107" s="15"/>
+      <c r="F107" s="23">
+        <v>0</v>
+      </c>
       <c r="G107" s="5" t="s">
         <v>125</v>
       </c>
@@ -5295,14 +5388,14 @@
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
-        <f>A107+1</f>
+        <f t="shared" si="6"/>
         <v>107</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C108" s="1" t="str">
-        <f>RIGHT(B108,2)</f>
+        <f t="shared" si="7"/>
         <v>VA</v>
       </c>
       <c r="D108" s="5">
@@ -5311,7 +5404,7 @@
       <c r="E108" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F108" s="15"/>
+      <c r="F108" s="23"/>
       <c r="G108" s="1" t="s">
         <v>240</v>
       </c>
@@ -5331,14 +5424,14 @@
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
-        <f>A108+1</f>
+        <f t="shared" si="6"/>
         <v>108</v>
       </c>
       <c r="B109" s="5" t="s">
         <v>75</v>
       </c>
       <c r="C109" s="1" t="str">
-        <f>RIGHT(B109,2)</f>
+        <f t="shared" si="7"/>
         <v>VA</v>
       </c>
       <c r="D109" s="5">
@@ -5347,7 +5440,7 @@
       <c r="E109" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="F109" s="15"/>
+      <c r="F109" s="23"/>
       <c r="G109" s="5" t="s">
         <v>128</v>
       </c>
@@ -5367,14 +5460,14 @@
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
-        <f>A109+1</f>
+        <f t="shared" si="6"/>
         <v>109</v>
       </c>
       <c r="B110" s="5" t="s">
         <v>74</v>
       </c>
       <c r="C110" s="1" t="str">
-        <f>RIGHT(B110,2)</f>
+        <f t="shared" si="7"/>
         <v>VA</v>
       </c>
       <c r="D110" s="5">
@@ -5383,7 +5476,7 @@
       <c r="E110" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F110" s="15"/>
+      <c r="F110" s="23"/>
       <c r="G110" s="5" t="s">
         <v>125</v>
       </c>
@@ -5406,14 +5499,14 @@
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
-        <f>A110+1</f>
+        <f t="shared" si="6"/>
         <v>110</v>
       </c>
       <c r="B111" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C111" s="1" t="str">
-        <f>RIGHT(B111,2)</f>
+        <f t="shared" si="7"/>
         <v>VT</v>
       </c>
       <c r="D111" s="5">
@@ -5422,7 +5515,7 @@
       <c r="E111" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F111" s="15"/>
+      <c r="F111" s="23"/>
       <c r="G111" s="5" t="s">
         <v>128</v>
       </c>
@@ -5439,14 +5532,14 @@
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
-        <f>A111+1</f>
+        <f t="shared" si="6"/>
         <v>111</v>
       </c>
       <c r="B112" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C112" s="1" t="str">
-        <f>RIGHT(B112,2)</f>
+        <f t="shared" si="7"/>
         <v>VT</v>
       </c>
       <c r="D112" s="5">
@@ -5455,7 +5548,7 @@
       <c r="E112" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F112" s="15"/>
+      <c r="F112" s="23"/>
       <c r="G112" s="5" t="s">
         <v>125</v>
       </c>
@@ -5469,21 +5562,23 @@
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
-        <f>A112+1</f>
+        <f t="shared" si="6"/>
         <v>112</v>
       </c>
       <c r="B113" s="5" t="s">
         <v>96</v>
       </c>
       <c r="C113" s="1" t="str">
-        <f>RIGHT(B113,2)</f>
+        <f t="shared" si="7"/>
         <v>WA</v>
       </c>
       <c r="D113" s="5">
         <v>0</v>
       </c>
       <c r="E113" s="6"/>
-      <c r="F113" s="15"/>
+      <c r="F113" s="23">
+        <v>0</v>
+      </c>
       <c r="G113" s="5" t="s">
         <v>125</v>
       </c>
@@ -5500,17 +5595,20 @@
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
-        <f>A113+1</f>
+        <f t="shared" si="6"/>
         <v>113</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>208</v>
       </c>
       <c r="C114" s="1" t="str">
-        <f>RIGHT(B114,2)</f>
+        <f t="shared" si="7"/>
         <v>WA</v>
       </c>
       <c r="D114" s="12">
+        <v>0</v>
+      </c>
+      <c r="F114" s="24">
         <v>0</v>
       </c>
       <c r="G114" s="1" t="s">
@@ -5522,21 +5620,23 @@
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
-        <f>A114+1</f>
+        <f t="shared" si="6"/>
         <v>114</v>
       </c>
       <c r="B115" s="5" t="s">
         <v>97</v>
       </c>
       <c r="C115" s="1" t="str">
-        <f>RIGHT(B115,2)</f>
+        <f t="shared" si="7"/>
         <v>WA</v>
       </c>
       <c r="D115" s="5">
         <v>1</v>
       </c>
       <c r="E115" s="6"/>
-      <c r="F115" s="15"/>
+      <c r="F115" s="23">
+        <v>0</v>
+      </c>
       <c r="G115" s="5" t="s">
         <v>128</v>
       </c>
@@ -5556,14 +5656,14 @@
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
-        <f>A115+1</f>
+        <f t="shared" si="6"/>
         <v>115</v>
       </c>
       <c r="B116" s="5" t="s">
         <v>36</v>
       </c>
       <c r="C116" s="1" t="str">
-        <f>RIGHT(B116,2)</f>
+        <f t="shared" si="7"/>
         <v>WI</v>
       </c>
       <c r="D116" s="5">
@@ -5572,7 +5672,7 @@
       <c r="E116" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="F116" s="15"/>
+      <c r="F116" s="23"/>
       <c r="G116" s="5" t="s">
         <v>125</v>
       </c>
@@ -5589,14 +5689,14 @@
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
-        <f>A116+1</f>
+        <f t="shared" si="6"/>
         <v>116</v>
       </c>
       <c r="B117" s="5" t="s">
         <v>37</v>
       </c>
       <c r="C117" s="1" t="str">
-        <f>RIGHT(B117,2)</f>
+        <f t="shared" si="7"/>
         <v>WI</v>
       </c>
       <c r="D117" s="5">
@@ -5605,7 +5705,7 @@
       <c r="E117" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="F117" s="15"/>
+      <c r="F117" s="23"/>
       <c r="G117" s="5" t="s">
         <v>128</v>
       </c>
@@ -5625,14 +5725,14 @@
     </row>
     <row r="118" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
-        <f>A117+1</f>
+        <f t="shared" si="6"/>
         <v>117</v>
       </c>
       <c r="B118" s="5" t="s">
         <v>76</v>
       </c>
       <c r="C118" s="1" t="str">
-        <f>RIGHT(B118,2)</f>
+        <f t="shared" si="7"/>
         <v>WV</v>
       </c>
       <c r="D118" s="5">
@@ -5641,7 +5741,7 @@
       <c r="E118" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F118" s="15"/>
+      <c r="F118" s="23"/>
       <c r="G118" s="5" t="s">
         <v>125</v>
       </c>
@@ -5660,14 +5760,14 @@
     </row>
     <row r="119" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
-        <f>A118+1</f>
+        <f t="shared" si="6"/>
         <v>118</v>
       </c>
       <c r="B119" s="5" t="s">
         <v>190</v>
       </c>
       <c r="C119" s="1" t="str">
-        <f>RIGHT(B119,2)</f>
+        <f t="shared" si="7"/>
         <v>WV</v>
       </c>
       <c r="D119" s="5">
@@ -5676,7 +5776,7 @@
       <c r="E119" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F119" s="15"/>
+      <c r="F119" s="23"/>
       <c r="G119" s="1" t="s">
         <v>128</v>
       </c>
@@ -5691,21 +5791,23 @@
     </row>
     <row r="120" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
-        <f>A119+1</f>
+        <f t="shared" si="6"/>
         <v>119</v>
       </c>
       <c r="B120" s="5" t="s">
         <v>98</v>
       </c>
       <c r="C120" s="1" t="str">
-        <f>RIGHT(B120,2)</f>
+        <f t="shared" si="7"/>
         <v>WY</v>
       </c>
       <c r="D120" s="5">
         <v>0</v>
       </c>
       <c r="E120" s="6"/>
-      <c r="F120" s="15"/>
+      <c r="F120" s="23">
+        <v>0</v>
+      </c>
       <c r="G120" s="5" t="s">
         <v>128</v>
       </c>
@@ -5724,21 +5826,23 @@
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
-        <f>A120+1</f>
+        <f t="shared" si="6"/>
         <v>120</v>
       </c>
       <c r="B121" s="5" t="s">
         <v>99</v>
       </c>
       <c r="C121" s="1" t="str">
-        <f>RIGHT(B121,2)</f>
+        <f t="shared" si="7"/>
         <v>WY</v>
       </c>
       <c r="D121" s="5">
         <v>0</v>
       </c>
       <c r="E121" s="6"/>
-      <c r="F121" s="15"/>
+      <c r="F121" s="23">
+        <v>0</v>
+      </c>
       <c r="G121" s="5" t="s">
         <v>125</v>
       </c>
@@ -5778,7 +5882,7 @@
     <col min="4" max="4" width="5.5" style="2" customWidth="1"/>
     <col min="5" max="5" width="5.5" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" style="15" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
@@ -5801,7 +5905,7 @@
       <c r="F1" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="15" t="s">
         <v>224</v>
       </c>
       <c r="H1" s="2" t="s">
@@ -5825,7 +5929,7 @@
       <c r="F2" s="2">
         <v>33</v>
       </c>
-      <c r="G2" s="18">
+      <c r="G2" s="15">
         <f>MOD(E2*F2+(F2/2)+H$2,360)</f>
         <v>241.5</v>
       </c>
@@ -5853,7 +5957,7 @@
       <c r="F3" s="2">
         <v>33</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="15">
         <f t="shared" ref="G3:G53" si="1">MOD(E3*F3+(F3/2)+H$2,360)</f>
         <v>241.5</v>
       </c>
@@ -5875,7 +5979,7 @@
       <c r="F4" s="2">
         <v>33</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="15">
         <f t="shared" si="1"/>
         <v>13.5</v>
       </c>
@@ -5897,7 +6001,7 @@
       <c r="F5" s="2">
         <v>33</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="15">
         <f t="shared" si="1"/>
         <v>13.5</v>
       </c>
@@ -5919,7 +6023,7 @@
       <c r="F6" s="2">
         <v>33</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="15">
         <f t="shared" si="1"/>
         <v>13.5</v>
       </c>
@@ -5941,7 +6045,7 @@
       <c r="F7" s="2">
         <v>33</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="15">
         <f t="shared" si="1"/>
         <v>13.5</v>
       </c>
@@ -5963,7 +6067,7 @@
       <c r="F8" s="2">
         <v>33</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="15">
         <f t="shared" si="1"/>
         <v>13.5</v>
       </c>
@@ -5985,7 +6089,7 @@
       <c r="F9" s="2">
         <v>33</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="15">
         <f t="shared" si="1"/>
         <v>13.5</v>
       </c>
@@ -6007,7 +6111,7 @@
       <c r="F10" s="2">
         <v>33</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="15">
         <f t="shared" si="1"/>
         <v>307.5</v>
       </c>
@@ -6029,7 +6133,7 @@
       <c r="F11" s="2">
         <v>33</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="15">
         <f t="shared" si="1"/>
         <v>307.5</v>
       </c>
@@ -6051,7 +6155,7 @@
       <c r="F12" s="2">
         <v>33</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="15">
         <f t="shared" si="1"/>
         <v>307.5</v>
       </c>
@@ -6073,7 +6177,7 @@
       <c r="F13" s="2">
         <v>33</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="15">
         <f t="shared" si="1"/>
         <v>307.5</v>
       </c>
@@ -6095,7 +6199,7 @@
       <c r="F14" s="2">
         <v>33</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G14" s="15">
         <f t="shared" si="1"/>
         <v>307.5</v>
       </c>
@@ -6117,7 +6221,7 @@
       <c r="F15" s="2">
         <v>33</v>
       </c>
-      <c r="G15" s="18">
+      <c r="G15" s="15">
         <f t="shared" si="1"/>
         <v>79.5</v>
       </c>
@@ -6139,7 +6243,7 @@
       <c r="F16" s="2">
         <v>33</v>
       </c>
-      <c r="G16" s="18">
+      <c r="G16" s="15">
         <f t="shared" si="1"/>
         <v>79.5</v>
       </c>
@@ -6161,7 +6265,7 @@
       <c r="F17" s="2">
         <v>33</v>
       </c>
-      <c r="G17" s="18">
+      <c r="G17" s="15">
         <f t="shared" si="1"/>
         <v>79.5</v>
       </c>
@@ -6186,7 +6290,7 @@
       <c r="F18" s="2">
         <v>33</v>
       </c>
-      <c r="G18" s="18">
+      <c r="G18" s="15">
         <f t="shared" si="1"/>
         <v>79.5</v>
       </c>
@@ -6208,7 +6312,7 @@
       <c r="F19" s="2">
         <v>33</v>
       </c>
-      <c r="G19" s="18">
+      <c r="G19" s="15">
         <f t="shared" si="1"/>
         <v>175.5</v>
       </c>
@@ -6230,7 +6334,7 @@
       <c r="F20" s="2">
         <v>33</v>
       </c>
-      <c r="G20" s="18">
+      <c r="G20" s="15">
         <f t="shared" si="1"/>
         <v>175.5</v>
       </c>
@@ -6252,7 +6356,7 @@
       <c r="F21" s="2">
         <v>33</v>
       </c>
-      <c r="G21" s="18">
+      <c r="G21" s="15">
         <f t="shared" si="1"/>
         <v>175.5</v>
       </c>
@@ -6274,7 +6378,7 @@
       <c r="F22" s="2">
         <v>33</v>
       </c>
-      <c r="G22" s="18">
+      <c r="G22" s="15">
         <f t="shared" si="1"/>
         <v>175.5</v>
       </c>
@@ -6296,7 +6400,7 @@
       <c r="F23" s="2">
         <v>33</v>
       </c>
-      <c r="G23" s="18">
+      <c r="G23" s="15">
         <f t="shared" si="1"/>
         <v>175.5</v>
       </c>
@@ -6318,7 +6422,7 @@
       <c r="F24" s="2">
         <v>33</v>
       </c>
-      <c r="G24" s="18">
+      <c r="G24" s="15">
         <f t="shared" si="1"/>
         <v>175.5</v>
       </c>
@@ -6340,7 +6444,7 @@
       <c r="F25" s="2">
         <v>33</v>
       </c>
-      <c r="G25" s="18">
+      <c r="G25" s="15">
         <f t="shared" si="1"/>
         <v>46.5</v>
       </c>
@@ -6362,7 +6466,7 @@
       <c r="F26" s="2">
         <v>33</v>
       </c>
-      <c r="G26" s="18">
+      <c r="G26" s="15">
         <f t="shared" si="1"/>
         <v>46.5</v>
       </c>
@@ -6384,7 +6488,7 @@
       <c r="F27" s="2">
         <v>33</v>
       </c>
-      <c r="G27" s="18">
+      <c r="G27" s="15">
         <f t="shared" si="1"/>
         <v>46.5</v>
       </c>
@@ -6406,7 +6510,7 @@
       <c r="F28" s="2">
         <v>33</v>
       </c>
-      <c r="G28" s="18">
+      <c r="G28" s="15">
         <f t="shared" si="1"/>
         <v>46.5</v>
       </c>
@@ -6428,7 +6532,7 @@
       <c r="F29" s="2">
         <v>33</v>
       </c>
-      <c r="G29" s="18">
+      <c r="G29" s="15">
         <f t="shared" si="1"/>
         <v>46.5</v>
       </c>
@@ -6450,7 +6554,7 @@
       <c r="F30" s="2">
         <v>33</v>
       </c>
-      <c r="G30" s="18">
+      <c r="G30" s="15">
         <f t="shared" si="1"/>
         <v>46.5</v>
       </c>
@@ -6475,7 +6579,7 @@
       <c r="F31" s="2">
         <v>33</v>
       </c>
-      <c r="G31" s="18">
+      <c r="G31" s="15">
         <f t="shared" si="1"/>
         <v>274.5</v>
       </c>
@@ -6497,7 +6601,7 @@
       <c r="F32" s="2">
         <v>33</v>
       </c>
-      <c r="G32" s="18">
+      <c r="G32" s="15">
         <f t="shared" si="1"/>
         <v>274.5</v>
       </c>
@@ -6519,7 +6623,7 @@
       <c r="F33" s="2">
         <v>33</v>
       </c>
-      <c r="G33" s="18">
+      <c r="G33" s="15">
         <f t="shared" si="1"/>
         <v>274.5</v>
       </c>
@@ -6541,7 +6645,7 @@
       <c r="F34" s="2">
         <v>33</v>
       </c>
-      <c r="G34" s="18">
+      <c r="G34" s="15">
         <f t="shared" si="1"/>
         <v>274.5</v>
       </c>
@@ -6563,7 +6667,7 @@
       <c r="F35" s="2">
         <v>33</v>
       </c>
-      <c r="G35" s="18">
+      <c r="G35" s="15">
         <f t="shared" si="1"/>
         <v>274.5</v>
       </c>
@@ -6585,7 +6689,7 @@
       <c r="F36" s="2">
         <v>33</v>
       </c>
-      <c r="G36" s="18">
+      <c r="G36" s="15">
         <f t="shared" si="1"/>
         <v>142.5</v>
       </c>
@@ -6607,7 +6711,7 @@
       <c r="F37" s="2">
         <v>33</v>
       </c>
-      <c r="G37" s="18">
+      <c r="G37" s="15">
         <f t="shared" si="1"/>
         <v>142.5</v>
       </c>
@@ -6629,7 +6733,7 @@
       <c r="F38" s="2">
         <v>33</v>
       </c>
-      <c r="G38" s="18">
+      <c r="G38" s="15">
         <f t="shared" si="1"/>
         <v>142.5</v>
       </c>
@@ -6651,7 +6755,7 @@
       <c r="F39" s="2">
         <v>33</v>
       </c>
-      <c r="G39" s="18">
+      <c r="G39" s="15">
         <f t="shared" si="1"/>
         <v>208.5</v>
       </c>
@@ -6673,7 +6777,7 @@
       <c r="F40" s="2">
         <v>33</v>
       </c>
-      <c r="G40" s="18">
+      <c r="G40" s="15">
         <f t="shared" si="1"/>
         <v>208.5</v>
       </c>
@@ -6695,7 +6799,7 @@
       <c r="F41" s="2">
         <v>33</v>
       </c>
-      <c r="G41" s="18">
+      <c r="G41" s="15">
         <f t="shared" si="1"/>
         <v>208.5</v>
       </c>
@@ -6717,7 +6821,7 @@
       <c r="F42" s="2">
         <v>33</v>
       </c>
-      <c r="G42" s="18">
+      <c r="G42" s="15">
         <f t="shared" si="1"/>
         <v>208.5</v>
       </c>
@@ -6742,7 +6846,7 @@
       <c r="F43" s="2">
         <v>33</v>
       </c>
-      <c r="G43" s="18">
+      <c r="G43" s="15">
         <f t="shared" si="1"/>
         <v>112.5</v>
       </c>
@@ -6764,7 +6868,7 @@
       <c r="F44" s="2">
         <v>33</v>
       </c>
-      <c r="G44" s="18">
+      <c r="G44" s="15">
         <f t="shared" si="1"/>
         <v>112.5</v>
       </c>
@@ -6786,7 +6890,7 @@
       <c r="F45" s="2">
         <v>33</v>
       </c>
-      <c r="G45" s="18">
+      <c r="G45" s="15">
         <f t="shared" si="1"/>
         <v>112.5</v>
       </c>
@@ -6808,7 +6912,7 @@
       <c r="F46" s="2">
         <v>33</v>
       </c>
-      <c r="G46" s="18">
+      <c r="G46" s="15">
         <f t="shared" si="1"/>
         <v>112.5</v>
       </c>
@@ -6830,7 +6934,7 @@
       <c r="F47" s="2">
         <v>33</v>
       </c>
-      <c r="G47" s="18">
+      <c r="G47" s="15">
         <f t="shared" si="1"/>
         <v>112.5</v>
       </c>
@@ -6852,7 +6956,7 @@
       <c r="F48" s="2">
         <v>33</v>
       </c>
-      <c r="G48" s="18">
+      <c r="G48" s="15">
         <f t="shared" si="1"/>
         <v>112.5</v>
       </c>
@@ -6874,7 +6978,7 @@
       <c r="F49" s="2">
         <v>33</v>
       </c>
-      <c r="G49" s="18">
+      <c r="G49" s="15">
         <f t="shared" si="1"/>
         <v>340.5</v>
       </c>
@@ -6896,7 +7000,7 @@
       <c r="F50" s="2">
         <v>33</v>
       </c>
-      <c r="G50" s="18">
+      <c r="G50" s="15">
         <f t="shared" si="1"/>
         <v>340.5</v>
       </c>
@@ -6918,7 +7022,7 @@
       <c r="F51" s="2">
         <v>33</v>
       </c>
-      <c r="G51" s="18">
+      <c r="G51" s="15">
         <f t="shared" si="1"/>
         <v>340.5</v>
       </c>
@@ -6940,7 +7044,7 @@
       <c r="F52" s="2">
         <v>33</v>
       </c>
-      <c r="G52" s="18">
+      <c r="G52" s="15">
         <f t="shared" si="1"/>
         <v>340.5</v>
       </c>
@@ -6962,7 +7066,7 @@
       <c r="F53" s="2">
         <v>33</v>
       </c>
-      <c r="G53" s="18">
+      <c r="G53" s="15">
         <f t="shared" si="1"/>
         <v>340.5</v>
       </c>
@@ -6987,152 +7091,152 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.6640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" style="20" customWidth="1"/>
-    <col min="5" max="10" width="10.83203125" style="20"/>
-    <col min="11" max="11" width="11.5" style="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="20"/>
+    <col min="1" max="1" width="13.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" style="17" customWidth="1"/>
+    <col min="5" max="10" width="10.83203125" style="17"/>
+    <col min="11" max="11" width="11.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="E2" s="22"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="23"/>
+      <c r="E2" s="19"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="20"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="E3" s="22"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="23"/>
+      <c r="E3" s="19"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="20"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="22"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="23"/>
+      <c r="E4" s="19"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="20"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="18" t="s">
         <v>183</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="23"/>
+      <c r="E5" s="19"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="20"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="22"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="23"/>
+      <c r="E6" s="19"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="20"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="27" t="s">
         <v>219</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="17" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="17" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="27" t="s">
         <v>241</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="17" t="s">
         <v>242</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="17" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="17" t="s">
         <v>244</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="17" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="17" t="s">
         <v>245</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="17" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="17" t="s">
         <v>190</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improve proximity panel, adjust color scheme
</commit_message>
<xml_diff>
--- a/io_in/city_list.xlsx
+++ b/io_in/city_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Coding/roadtrips/io_in/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26609A3C-AF03-8B42-8A8F-85B530F16CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BF5E93-8869-DF41-83AA-A11964A34AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17560" yWindow="500" windowWidth="24000" windowHeight="21900" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
+    <workbookView xWindow="11840" yWindow="500" windowWidth="24000" windowHeight="21900" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="9" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="355">
   <si>
     <t>Boston MA</t>
   </si>
@@ -795,9 +795,6 @@
     <t>USW00013963</t>
   </si>
   <si>
-    <t>USW00003103</t>
-  </si>
-  <si>
     <t>USW00023183</t>
   </si>
   <si>
@@ -831,24 +828,12 @@
     <t>USW00093822</t>
   </si>
   <si>
-    <t>USW00053842</t>
-  </si>
-  <si>
     <t>USW00013920</t>
   </si>
   <si>
-    <t>USW00053841</t>
-  </si>
-  <si>
-    <t>USW00013970</t>
-  </si>
-  <si>
     <t>USW00014739</t>
   </si>
   <si>
-    <t>USW00013752</t>
-  </si>
-  <si>
     <t>USW00014605</t>
   </si>
   <si>
@@ -858,9 +843,6 @@
     <t>USW00014922</t>
   </si>
   <si>
-    <t>USW00003963</t>
-  </si>
-  <si>
     <t>USW00003940</t>
   </si>
   <si>
@@ -879,12 +861,6 @@
     <t>USW00014745</t>
   </si>
   <si>
-    <t>USW00014792</t>
-  </si>
-  <si>
-    <t>USW00023049</t>
-  </si>
-  <si>
     <t>USW00014735</t>
   </si>
   <si>
@@ -897,27 +873,15 @@
     <t>USW00024232</t>
   </si>
   <si>
-    <t>USW00014751</t>
-  </si>
-  <si>
-    <t>RQW00011641</t>
-  </si>
-  <si>
     <t>USW00014765</t>
   </si>
   <si>
     <t>USW00013883</t>
   </si>
   <si>
-    <t>USW00024025</t>
-  </si>
-  <si>
     <t>USW00013897</t>
   </si>
   <si>
-    <t>USW00013904</t>
-  </si>
-  <si>
     <t>USW00024127</t>
   </si>
   <si>
@@ -999,18 +963,12 @@
     <t>USW00094823</t>
   </si>
   <si>
-    <t>USW00013841</t>
-  </si>
-  <si>
     <t>USW00003947</t>
   </si>
   <si>
     <t>USW00014820</t>
   </si>
   <si>
-    <t>USW00023293</t>
-  </si>
-  <si>
     <t>USW00013737</t>
   </si>
   <si>
@@ -1038,9 +996,6 @@
     <t>USW00013968</t>
   </si>
   <si>
-    <t>USW00003171</t>
-  </si>
-  <si>
     <t>USW00013743</t>
   </si>
   <si>
@@ -1065,9 +1020,6 @@
     <t>USW00024089</t>
   </si>
   <si>
-    <t>USW00014758</t>
-  </si>
-  <si>
     <t>USW00003822</t>
   </si>
   <si>
@@ -1098,10 +1050,58 @@
     <t>USW00013736</t>
   </si>
   <si>
-    <t>USW00094982</t>
-  </si>
-  <si>
-    <t>USW00093736</t>
+    <t>USW00023157</t>
+  </si>
+  <si>
+    <t>USW00024225</t>
+  </si>
+  <si>
+    <t>USW00013707</t>
+  </si>
+  <si>
+    <t>USW00012836</t>
+  </si>
+  <si>
+    <t>USW00093805</t>
+  </si>
+  <si>
+    <t>USW00024157</t>
+  </si>
+  <si>
+    <t>USW00003945</t>
+  </si>
+  <si>
+    <t>USW00024132</t>
+  </si>
+  <si>
+    <t>USW00014710</t>
+  </si>
+  <si>
+    <t>USW00024090</t>
+  </si>
+  <si>
+    <t>USW00093812</t>
+  </si>
+  <si>
+    <t>USW00013976</t>
+  </si>
+  <si>
+    <t>USW00013810</t>
+  </si>
+  <si>
+    <t>USW00014737</t>
+  </si>
+  <si>
+    <t>USW00093819</t>
+  </si>
+  <si>
+    <t>USW00013733</t>
+  </si>
+  <si>
+    <t>USW00014706</t>
+  </si>
+  <si>
+    <t>USW00014990</t>
   </si>
 </sst>
 </file>
@@ -1164,7 +1164,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1193,6 +1193,12 @@
       <patternFill patternType="solid">
         <fgColor theme="3" tint="-0.499984740745262"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1239,7 +1245,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1308,6 +1314,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1625,8 +1632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418BD67C-5132-6942-B406-D98F46E6A0BD}">
   <dimension ref="A1:M121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1893,7 +1900,7 @@
         <v>35.180556000000003</v>
       </c>
       <c r="L7" s="1"/>
-      <c r="M7" s="1" t="s">
+      <c r="M7" s="28" t="s">
         <v>252</v>
       </c>
     </row>
@@ -1930,7 +1937,7 @@
       </c>
       <c r="L8" s="5"/>
       <c r="M8" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -1966,7 +1973,7 @@
       </c>
       <c r="L9" s="5"/>
       <c r="M9" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -1999,6 +2006,9 @@
       <c r="K10" s="14">
         <v>40.801943999999999</v>
       </c>
+      <c r="M10" s="28" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -2033,7 +2043,7 @@
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -2072,7 +2082,7 @@
       </c>
       <c r="L12" s="5"/>
       <c r="M12" s="1" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -2109,8 +2119,8 @@
         <v>33.980600500000001</v>
       </c>
       <c r="L13" s="5"/>
-      <c r="M13" s="1" t="s">
-        <v>333</v>
+      <c r="M13" s="28" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -2146,7 +2156,7 @@
       </c>
       <c r="L14" s="5"/>
       <c r="M14" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -2185,7 +2195,7 @@
       </c>
       <c r="L15" s="5"/>
       <c r="M15" s="1" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -2221,7 +2231,7 @@
       </c>
       <c r="L16" s="5"/>
       <c r="M16" s="1" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -2256,8 +2266,8 @@
         <v>37.338208199999997</v>
       </c>
       <c r="L17" s="5"/>
-      <c r="M17" s="1" t="s">
-        <v>323</v>
+      <c r="M17" s="28" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -2290,6 +2300,9 @@
       <c r="K18" s="14">
         <v>37.984444000000003</v>
       </c>
+      <c r="M18" s="28" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
@@ -2319,7 +2332,7 @@
         <v>38.833888999999999</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
@@ -2355,7 +2368,7 @@
       </c>
       <c r="L20" s="5"/>
       <c r="M20" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -2391,7 +2404,7 @@
       </c>
       <c r="L21" s="5"/>
       <c r="M21" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
@@ -2423,8 +2436,8 @@
         <v>41.31</v>
       </c>
       <c r="L22" s="5"/>
-      <c r="M22" s="1" t="s">
-        <v>342</v>
+      <c r="M22" s="28" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
@@ -2462,7 +2475,7 @@
         <v>128</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
@@ -2494,6 +2507,9 @@
         <v>39.158168000000003</v>
       </c>
       <c r="L24" s="5"/>
+      <c r="M24" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
@@ -2533,7 +2549,7 @@
       </c>
       <c r="L25" s="5"/>
       <c r="M25" s="1" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
@@ -2571,6 +2587,9 @@
         <v>24.555</v>
       </c>
       <c r="L26" s="5"/>
+      <c r="M26" s="1" t="s">
+        <v>340</v>
+      </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
@@ -2607,7 +2626,7 @@
       </c>
       <c r="L27" s="5"/>
       <c r="M27" s="1" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
@@ -2645,7 +2664,7 @@
       </c>
       <c r="L28" s="5"/>
       <c r="M28" s="1" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
     </row>
     <row r="29" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2681,7 +2700,9 @@
         <v>30.438255900000001</v>
       </c>
       <c r="L29" s="5"/>
-      <c r="M29" s="1"/>
+      <c r="M29" s="1" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="30" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
@@ -2719,7 +2740,7 @@
       </c>
       <c r="L30" s="5"/>
       <c r="M30" s="1" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
@@ -2755,7 +2776,7 @@
       </c>
       <c r="L31" s="5"/>
       <c r="M31" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
@@ -2788,7 +2809,7 @@
       </c>
       <c r="L32" s="5"/>
       <c r="M32" s="1" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
@@ -2826,7 +2847,7 @@
         <v>209</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
@@ -2858,8 +2879,8 @@
         <v>41.523643700000001</v>
       </c>
       <c r="L34" s="5"/>
-      <c r="M34" s="1" t="s">
-        <v>353</v>
+      <c r="M34" s="28" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
@@ -2892,7 +2913,7 @@
       </c>
       <c r="L35" s="5"/>
       <c r="M35" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
@@ -2925,7 +2946,7 @@
       </c>
       <c r="L36" s="5"/>
       <c r="M36" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
@@ -2957,6 +2978,9 @@
         <v>47.692777999999997</v>
       </c>
       <c r="L37" s="5"/>
+      <c r="M37" s="28" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
@@ -2991,7 +3015,7 @@
       </c>
       <c r="L38" s="5"/>
       <c r="M38" s="1" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
@@ -3024,7 +3048,7 @@
       </c>
       <c r="L39" s="5"/>
       <c r="M39" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="40" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -3061,7 +3085,7 @@
       </c>
       <c r="L40" s="5"/>
       <c r="M40" s="1" t="s">
-        <v>264</v>
+        <v>351</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
@@ -3094,7 +3118,7 @@
       </c>
       <c r="L41" s="5"/>
       <c r="M41" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
@@ -3127,7 +3151,7 @@
       </c>
       <c r="L42" s="5"/>
       <c r="M42" s="1" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
@@ -3159,8 +3183,8 @@
         <v>38.200905499999998</v>
       </c>
       <c r="L43" s="5"/>
-      <c r="M43" s="1" t="s">
-        <v>266</v>
+      <c r="M43" s="28" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
@@ -3196,7 +3220,7 @@
       </c>
       <c r="L44" s="5"/>
       <c r="M44" s="1" t="s">
-        <v>327</v>
+        <v>313</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
@@ -3228,8 +3252,8 @@
         <v>30.451467699999998</v>
       </c>
       <c r="L45" s="5"/>
-      <c r="M45" s="1" t="s">
-        <v>267</v>
+      <c r="M45" s="28" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
@@ -3265,7 +3289,7 @@
       </c>
       <c r="L46" s="5"/>
       <c r="M46" s="1" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
@@ -3301,7 +3325,7 @@
       </c>
       <c r="L47" s="5"/>
       <c r="M47" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
@@ -3333,8 +3357,8 @@
         <v>38.978445299999997</v>
       </c>
       <c r="L48" s="5"/>
-      <c r="M48" s="1" t="s">
-        <v>269</v>
+      <c r="M48" s="28" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
@@ -3370,7 +3394,7 @@
       </c>
       <c r="L49" s="5"/>
       <c r="M49" s="1" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
@@ -3403,7 +3427,7 @@
       </c>
       <c r="L50" s="5"/>
       <c r="M50" s="1" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
@@ -3436,7 +3460,7 @@
       </c>
       <c r="L51" s="5"/>
       <c r="M51" s="1" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
@@ -3472,7 +3496,7 @@
       </c>
       <c r="L52" s="5"/>
       <c r="M52" s="1" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
@@ -3508,7 +3532,7 @@
       </c>
       <c r="L53" s="5"/>
       <c r="M53" s="1" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
@@ -3541,7 +3565,7 @@
       </c>
       <c r="L54" s="5"/>
       <c r="M54" s="1" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
@@ -3572,7 +3596,7 @@
         <v>46.786943999999998</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>347</v>
+        <v>331</v>
       </c>
     </row>
     <row r="56" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -3609,7 +3633,7 @@
       </c>
       <c r="L56" s="5"/>
       <c r="M56" s="1" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
@@ -3641,8 +3665,8 @@
         <v>38.576701700000001</v>
       </c>
       <c r="L57" s="5"/>
-      <c r="M57" s="1" t="s">
-        <v>273</v>
+      <c r="M57" s="28" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
@@ -3678,7 +3702,7 @@
       </c>
       <c r="L58" s="5"/>
       <c r="M58" s="1" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
@@ -3717,7 +3741,7 @@
       </c>
       <c r="L59" s="22"/>
       <c r="M59" s="1" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
@@ -3750,7 +3774,7 @@
       </c>
       <c r="L60" s="5"/>
       <c r="M60" s="1" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
@@ -3783,7 +3807,7 @@
       </c>
       <c r="L61" s="5"/>
       <c r="M61" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.2">
@@ -3816,6 +3840,9 @@
       <c r="K62" s="14">
         <v>45.677778000000004</v>
       </c>
+      <c r="M62" s="1" t="s">
+        <v>344</v>
+      </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
@@ -3847,7 +3874,7 @@
       </c>
       <c r="L63" s="5"/>
       <c r="M63" s="1" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
@@ -3883,7 +3910,7 @@
       </c>
       <c r="L64" s="5"/>
       <c r="M64" s="1" t="s">
-        <v>316</v>
+        <v>304</v>
       </c>
     </row>
     <row r="65" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -3920,7 +3947,7 @@
       </c>
       <c r="L65" s="5"/>
       <c r="M65" s="1" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.2">
@@ -3953,7 +3980,7 @@
       </c>
       <c r="L66" s="5"/>
       <c r="M66" s="1" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.2">
@@ -3986,7 +4013,7 @@
       </c>
       <c r="L67" s="5"/>
       <c r="M67" s="1" t="s">
-        <v>348</v>
+        <v>332</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
@@ -4019,7 +4046,7 @@
       </c>
       <c r="L68" s="5"/>
       <c r="M68" s="1" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.2">
@@ -4052,7 +4079,7 @@
       </c>
       <c r="L69" s="5"/>
       <c r="M69" s="1" t="s">
-        <v>349</v>
+        <v>333</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.2">
@@ -4085,7 +4112,7 @@
       </c>
       <c r="L70" s="5"/>
       <c r="M70" s="1" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.2">
@@ -4117,6 +4144,9 @@
         <v>42.990833000000002</v>
       </c>
       <c r="L71" s="5"/>
+      <c r="M71" s="1" t="s">
+        <v>345</v>
+      </c>
     </row>
     <row r="72" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
@@ -4150,7 +4180,7 @@
       </c>
       <c r="L72" s="5"/>
       <c r="M72" s="1" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.2">
@@ -4182,8 +4212,8 @@
         <v>40.220582399999998</v>
       </c>
       <c r="L73" s="5"/>
-      <c r="M73" s="1" t="s">
-        <v>280</v>
+      <c r="M73" s="28" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="74" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -4218,7 +4248,7 @@
       </c>
       <c r="L74" s="5"/>
       <c r="M74" s="1" t="s">
-        <v>350</v>
+        <v>334</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.2">
@@ -4250,8 +4280,8 @@
         <v>35.686975199999999</v>
       </c>
       <c r="L75" s="5"/>
-      <c r="M75" s="1" t="s">
-        <v>281</v>
+      <c r="M75" s="28" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.2">
@@ -4283,6 +4313,9 @@
         <v>36.393889000000001</v>
       </c>
       <c r="L76" s="5"/>
+      <c r="M76" s="28" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
@@ -4314,7 +4347,7 @@
       </c>
       <c r="L77" s="5"/>
       <c r="M77" s="1" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.2">
@@ -4350,7 +4383,7 @@
       </c>
       <c r="L78" s="5"/>
       <c r="M78" s="1" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.2">
@@ -4383,7 +4416,7 @@
       </c>
       <c r="L79" s="5"/>
       <c r="M79" s="1" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.2">
@@ -4419,7 +4452,7 @@
       </c>
       <c r="L80" s="5"/>
       <c r="M80" s="1" t="s">
-        <v>329</v>
+        <v>315</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.2">
@@ -4461,7 +4494,7 @@
       </c>
       <c r="L81" s="5"/>
       <c r="M81" s="1" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.2">
@@ -4497,7 +4530,7 @@
       </c>
       <c r="L82" s="5"/>
       <c r="M82" s="1" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.2">
@@ -4532,8 +4565,8 @@
         <v>39.103118199999997</v>
       </c>
       <c r="L83" s="5"/>
-      <c r="M83" s="1" t="s">
-        <v>320</v>
+      <c r="M83" s="28" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.2">
@@ -4569,7 +4602,7 @@
       </c>
       <c r="L84" s="5"/>
       <c r="M84" s="1" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
@@ -4605,7 +4638,7 @@
       </c>
       <c r="L85" s="5"/>
       <c r="M85" s="1" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.2">
@@ -4641,7 +4674,7 @@
       </c>
       <c r="L86" s="5"/>
       <c r="M86" s="1" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.2">
@@ -4677,7 +4710,7 @@
       </c>
       <c r="L87" s="5"/>
       <c r="M87" s="1" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.2">
@@ -4713,7 +4746,7 @@
       </c>
       <c r="L88" s="5"/>
       <c r="M88" s="1" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
     </row>
     <row r="89" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -4748,7 +4781,7 @@
       </c>
       <c r="L89" s="5"/>
       <c r="M89" s="1" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.2">
@@ -4780,8 +4813,8 @@
         <v>40.273191099999998</v>
       </c>
       <c r="L90" s="5"/>
-      <c r="M90" s="1" t="s">
-        <v>286</v>
+      <c r="M90" s="28" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.2">
@@ -4820,7 +4853,7 @@
       </c>
       <c r="L91" s="5"/>
       <c r="M91" s="1" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.2">
@@ -4856,7 +4889,7 @@
       </c>
       <c r="L92" s="5"/>
       <c r="M92" s="1" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.2">
@@ -4893,8 +4926,8 @@
       <c r="L93" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="M93" s="1" t="s">
-        <v>287</v>
+      <c r="M93" s="28" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.2">
@@ -4930,7 +4963,7 @@
       </c>
       <c r="L94" s="5"/>
       <c r="M94" s="1" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.2">
@@ -4963,7 +4996,7 @@
       </c>
       <c r="L95" s="5"/>
       <c r="M95" s="1" t="s">
-        <v>351</v>
+        <v>335</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">
@@ -4996,7 +5029,7 @@
       </c>
       <c r="L96" s="5"/>
       <c r="M96" s="1" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.2">
@@ -5028,8 +5061,8 @@
         <v>44.366787600000002</v>
       </c>
       <c r="L97" s="5"/>
-      <c r="M97" s="1" t="s">
-        <v>290</v>
+      <c r="M97" s="28" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.2">
@@ -5062,7 +5095,7 @@
       </c>
       <c r="L98" s="5"/>
       <c r="M98" s="1" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.2">
@@ -5098,7 +5131,7 @@
       </c>
       <c r="L99" s="5"/>
       <c r="M99" s="1" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.2">
@@ -5134,7 +5167,7 @@
       </c>
       <c r="L100" s="5"/>
       <c r="M100" s="1" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.2">
@@ -5170,7 +5203,7 @@
       </c>
       <c r="L101" s="5"/>
       <c r="M101" s="1" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.2">
@@ -5205,8 +5238,8 @@
         <v>30.267153</v>
       </c>
       <c r="L102" s="5"/>
-      <c r="M102" s="1" t="s">
-        <v>292</v>
+      <c r="M102" s="28" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.2">
@@ -5242,7 +5275,7 @@
       </c>
       <c r="L103" s="5"/>
       <c r="M103" s="1" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.2">
@@ -5278,7 +5311,7 @@
       </c>
       <c r="L104" s="5"/>
       <c r="M104" s="1" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.2">
@@ -5317,7 +5350,7 @@
       </c>
       <c r="L105" s="5"/>
       <c r="M105" s="1" t="s">
-        <v>317</v>
+        <v>305</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.2">
@@ -5349,6 +5382,9 @@
         <v>40.244444000000001</v>
       </c>
       <c r="L106" s="5"/>
+      <c r="M106" s="28" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
@@ -5383,7 +5419,7 @@
       </c>
       <c r="L107" s="5"/>
       <c r="M107" s="1" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.2">
@@ -5418,8 +5454,8 @@
         <v>38.029305899999997</v>
       </c>
       <c r="L108" s="5"/>
-      <c r="M108" s="1" t="s">
-        <v>354</v>
+      <c r="M108" s="28" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.2">
@@ -5455,7 +5491,7 @@
       </c>
       <c r="L109" s="5"/>
       <c r="M109" s="1" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.2">
@@ -5494,7 +5530,7 @@
       </c>
       <c r="L110" s="5"/>
       <c r="M110" s="1" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.2">
@@ -5527,7 +5563,7 @@
       </c>
       <c r="L111" s="5"/>
       <c r="M111" s="1" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.2">
@@ -5559,6 +5595,9 @@
         <v>44.260059300000002</v>
       </c>
       <c r="L112" s="5"/>
+      <c r="M112" s="28" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
@@ -5590,7 +5629,7 @@
       </c>
       <c r="L113" s="5"/>
       <c r="M113" s="1" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.2">
@@ -5623,6 +5662,9 @@
       <c r="K114" s="14">
         <v>48.113056</v>
       </c>
+      <c r="M114" s="28" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
@@ -5657,7 +5699,7 @@
       </c>
       <c r="L115" s="5"/>
       <c r="M115" s="1" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.2">
@@ -5690,7 +5732,7 @@
       </c>
       <c r="L116" s="5"/>
       <c r="M116" s="1" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.2">
@@ -5726,7 +5768,7 @@
       </c>
       <c r="L117" s="5"/>
       <c r="M117" s="1" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
     </row>
     <row r="118" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -5761,7 +5803,7 @@
       </c>
       <c r="L118" s="5"/>
       <c r="M118" s="1" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
     </row>
     <row r="119" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -5796,7 +5838,7 @@
       </c>
       <c r="L119" s="5"/>
       <c r="M119" s="1" t="s">
-        <v>352</v>
+        <v>336</v>
       </c>
     </row>
     <row r="120" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -5831,7 +5873,7 @@
       </c>
       <c r="L120" s="5"/>
       <c r="M120" s="1" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.2">
@@ -5864,7 +5906,7 @@
       </c>
       <c r="L121" s="5"/>
       <c r="M121" s="1" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fill in explanatory text, improve weather hovertext
</commit_message>
<xml_diff>
--- a/io_in/city_list.xlsx
+++ b/io_in/city_list.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Coding/roadtrips/io_in/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC74EE3-1C4A-C048-88C1-44BBB6172508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FA3764-7EAC-BE45-BC13-A42C6D031F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11840" yWindow="500" windowWidth="24000" windowHeight="21900" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
+    <workbookView xWindow="13500" yWindow="500" windowWidth="30020" windowHeight="21900" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="9" r:id="rId1"/>
-    <sheet name="Regions" sheetId="8" r:id="rId2"/>
-    <sheet name="Omissions" sheetId="4" r:id="rId3"/>
+    <sheet name="Climate" sheetId="10" r:id="rId2"/>
+    <sheet name="Regions" sheetId="8" r:id="rId3"/>
+    <sheet name="Omissions" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="423">
   <si>
     <t>Boston MA</t>
   </si>
@@ -1102,6 +1103,210 @@
   </si>
   <si>
     <t>USW00014990</t>
+  </si>
+  <si>
+    <t>koppen</t>
+  </si>
+  <si>
+    <t>Tropical Savanna</t>
+  </si>
+  <si>
+    <t>Tropical Monsoon</t>
+  </si>
+  <si>
+    <t>Dfc</t>
+  </si>
+  <si>
+    <t>Abbrev</t>
+  </si>
+  <si>
+    <t>Climate</t>
+  </si>
+  <si>
+    <t>Cfa</t>
+  </si>
+  <si>
+    <t>BSk</t>
+  </si>
+  <si>
+    <t>BWh</t>
+  </si>
+  <si>
+    <t>Csb</t>
+  </si>
+  <si>
+    <t>BSh</t>
+  </si>
+  <si>
+    <t>Csa</t>
+  </si>
+  <si>
+    <t>Dfa</t>
+  </si>
+  <si>
+    <t>Aw</t>
+  </si>
+  <si>
+    <t>Am</t>
+  </si>
+  <si>
+    <t>Dsb</t>
+  </si>
+  <si>
+    <t>Dfb</t>
+  </si>
+  <si>
+    <t>Bsk</t>
+  </si>
+  <si>
+    <t>Af</t>
+  </si>
+  <si>
+    <t>BWk</t>
+  </si>
+  <si>
+    <t>As</t>
+  </si>
+  <si>
+    <t>Csc</t>
+  </si>
+  <si>
+    <t>Cwa</t>
+  </si>
+  <si>
+    <t>Cwb</t>
+  </si>
+  <si>
+    <t>Cwc</t>
+  </si>
+  <si>
+    <t>Cfb</t>
+  </si>
+  <si>
+    <t>Cfc</t>
+  </si>
+  <si>
+    <t>Dsa</t>
+  </si>
+  <si>
+    <t>Dsc</t>
+  </si>
+  <si>
+    <t>Dsd</t>
+  </si>
+  <si>
+    <t>Dwa</t>
+  </si>
+  <si>
+    <t>Dwb</t>
+  </si>
+  <si>
+    <t>Dwc</t>
+  </si>
+  <si>
+    <t>Dwd</t>
+  </si>
+  <si>
+    <t>Dfd</t>
+  </si>
+  <si>
+    <t>ET</t>
+  </si>
+  <si>
+    <t>EF</t>
+  </si>
+  <si>
+    <t>Tropical Rainforest</t>
+  </si>
+  <si>
+    <t>Arid Hot</t>
+  </si>
+  <si>
+    <t>Arid Cold</t>
+  </si>
+  <si>
+    <t>Desert Hot</t>
+  </si>
+  <si>
+    <t>Desert Cold</t>
+  </si>
+  <si>
+    <t>Temperate</t>
+  </si>
+  <si>
+    <t>Polar Tundra</t>
+  </si>
+  <si>
+    <t>Polar Ice</t>
+  </si>
+  <si>
+    <t>climate_major</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Data Pending</t>
+  </si>
+  <si>
+    <t>XZ</t>
+  </si>
+  <si>
+    <t>climate_summer</t>
+  </si>
+  <si>
+    <t>Continental</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>Dry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dry </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hot </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cold </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dry, Hot </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dry, Warm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dry, Cold </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dry, Very Cold </t>
+  </si>
+  <si>
+    <t>Wet</t>
+  </si>
+  <si>
+    <t>Hot, Wet</t>
+  </si>
+  <si>
+    <t>Warm, Wet</t>
+  </si>
+  <si>
+    <t>Cold, Wet</t>
+  </si>
+  <si>
+    <t>Very Cold, Wet</t>
+  </si>
+  <si>
+    <t>climate_winter</t>
   </si>
 </sst>
 </file>
@@ -1245,7 +1450,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1315,6 +1520,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1630,10 +1836,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418BD67C-5132-6942-B406-D98F46E6A0BD}">
-  <dimension ref="A1:M121"/>
+  <dimension ref="A1:Q121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="H97" sqref="H97"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1651,10 +1857,14 @@
     <col min="11" max="11" width="5.6640625" style="14" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.5" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="10.83203125" style="1"/>
+    <col min="14" max="14" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>-1</v>
       </c>
@@ -1694,8 +1904,20 @@
       <c r="M1" s="1" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <f t="shared" ref="A2:A33" si="0">A1+1</f>
         <v>0</v>
@@ -1729,8 +1951,23 @@
       <c r="M2" s="1" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="O2" s="1" t="str">
+        <f>LOOKUP(N2,Climate!A:A,Climate!B:B)</f>
+        <v>Continental</v>
+      </c>
+      <c r="P2" s="1" t="str">
+        <f>LOOKUP(N2,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q2" s="1" t="str">
+        <f>LOOKUP(N2,Climate!A:A,Climate!C:C)</f>
+        <v>Cold, Wet</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1764,8 +2001,23 @@
       <c r="M3" s="1" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="O3" s="1" t="str">
+        <f>LOOKUP(N3,Climate!A:A,Climate!B:B)</f>
+        <v>Continental</v>
+      </c>
+      <c r="P3" s="1" t="str">
+        <f>LOOKUP(N3,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q3" s="1" t="str">
+        <f>LOOKUP(N3,Climate!A:A,Climate!C:C)</f>
+        <v>Cold, Wet</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -1800,8 +2052,23 @@
       <c r="M4" s="1" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="O4" s="1" t="str">
+        <f>LOOKUP(N4,Climate!A:A,Climate!B:B)</f>
+        <v>Temperate</v>
+      </c>
+      <c r="P4" s="1" t="str">
+        <f>LOOKUP(N4,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q4" s="1" t="str">
+        <f>LOOKUP(N4,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1833,8 +2100,23 @@
       <c r="M5" s="1" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="O5" s="1" t="str">
+        <f>LOOKUP(N5,Climate!A:A,Climate!B:B)</f>
+        <v>Temperate</v>
+      </c>
+      <c r="P5" s="1" t="str">
+        <f>LOOKUP(N5,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q5" s="1" t="str">
+        <f>LOOKUP(N5,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1866,8 +2148,23 @@
       <c r="M6" s="1" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N6" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="O6" s="1" t="str">
+        <f>LOOKUP(N6,Climate!A:A,Climate!B:B)</f>
+        <v>Temperate</v>
+      </c>
+      <c r="P6" s="1" t="str">
+        <f>LOOKUP(N6,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q6" s="1" t="str">
+        <f>LOOKUP(N6,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1903,8 +2200,23 @@
       <c r="M7" s="27" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N7" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="O7" s="1" t="str">
+        <f>LOOKUP(N7,Climate!A:A,Climate!B:B)</f>
+        <v>Arid Cold</v>
+      </c>
+      <c r="P7" s="1" t="str">
+        <f>LOOKUP(N7,Climate!A:A,Climate!D:D)</f>
+        <v>Dry</v>
+      </c>
+      <c r="Q7" s="1" t="str">
+        <f>LOOKUP(N7,Climate!A:A,Climate!C:C)</f>
+        <v>Dry</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1939,8 +2251,23 @@
       <c r="M8" s="1" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N8" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="O8" s="1" t="str">
+        <f>LOOKUP(N8,Climate!A:A,Climate!B:B)</f>
+        <v>Desert Hot</v>
+      </c>
+      <c r="P8" s="1" t="str">
+        <f>LOOKUP(N8,Climate!A:A,Climate!D:D)</f>
+        <v>Dry</v>
+      </c>
+      <c r="Q8" s="1" t="str">
+        <f>LOOKUP(N8,Climate!A:A,Climate!C:C)</f>
+        <v>Dry</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1975,8 +2302,23 @@
       <c r="M9" s="1" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N9" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="O9" s="1" t="str">
+        <f>LOOKUP(N9,Climate!A:A,Climate!B:B)</f>
+        <v>Desert Hot</v>
+      </c>
+      <c r="P9" s="1" t="str">
+        <f>LOOKUP(N9,Climate!A:A,Climate!D:D)</f>
+        <v>Dry</v>
+      </c>
+      <c r="Q9" s="1" t="str">
+        <f>LOOKUP(N9,Climate!A:A,Climate!C:C)</f>
+        <v>Dry</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2009,8 +2351,23 @@
       <c r="M10" s="27" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N10" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="O10" s="1" t="str">
+        <f>LOOKUP(N10,Climate!A:A,Climate!B:B)</f>
+        <v>Temperate</v>
+      </c>
+      <c r="P10" s="1" t="str">
+        <f>LOOKUP(N10,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q10" s="1" t="str">
+        <f>LOOKUP(N10,Climate!A:A,Climate!C:C)</f>
+        <v xml:space="preserve">Dry, Warm </v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2045,8 +2402,23 @@
       <c r="M11" s="1" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N11" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="O11" s="1" t="str">
+        <f>LOOKUP(N11,Climate!A:A,Climate!B:B)</f>
+        <v>Arid Hot</v>
+      </c>
+      <c r="P11" s="1" t="str">
+        <f>LOOKUP(N11,Climate!A:A,Climate!D:D)</f>
+        <v>Dry</v>
+      </c>
+      <c r="Q11" s="1" t="str">
+        <f>LOOKUP(N11,Climate!A:A,Climate!C:C)</f>
+        <v>Dry</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2084,8 +2456,23 @@
       <c r="M12" s="1" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N12" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="O12" s="1" t="str">
+        <f>LOOKUP(N12,Climate!A:A,Climate!B:B)</f>
+        <v>Temperate</v>
+      </c>
+      <c r="P12" s="1" t="str">
+        <f>LOOKUP(N12,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q12" s="1" t="str">
+        <f>LOOKUP(N12,Climate!A:A,Climate!C:C)</f>
+        <v xml:space="preserve">Dry, Hot </v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2122,8 +2509,23 @@
       <c r="M13" s="27" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N13" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="O13" s="1" t="str">
+        <f>LOOKUP(N13,Climate!A:A,Climate!B:B)</f>
+        <v>Arid Hot</v>
+      </c>
+      <c r="P13" s="1" t="str">
+        <f>LOOKUP(N13,Climate!A:A,Climate!D:D)</f>
+        <v>Dry</v>
+      </c>
+      <c r="Q13" s="1" t="str">
+        <f>LOOKUP(N13,Climate!A:A,Climate!C:C)</f>
+        <v>Dry</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2158,8 +2560,23 @@
       <c r="M14" s="1" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N14" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="O14" s="1" t="str">
+        <f>LOOKUP(N14,Climate!A:A,Climate!B:B)</f>
+        <v>Temperate</v>
+      </c>
+      <c r="P14" s="1" t="str">
+        <f>LOOKUP(N14,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q14" s="1" t="str">
+        <f>LOOKUP(N14,Climate!A:A,Climate!C:C)</f>
+        <v xml:space="preserve">Dry, Hot </v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2197,8 +2614,23 @@
       <c r="M15" s="1" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N15" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="O15" s="1" t="str">
+        <f>LOOKUP(N15,Climate!A:A,Climate!B:B)</f>
+        <v>Arid Hot</v>
+      </c>
+      <c r="P15" s="1" t="str">
+        <f>LOOKUP(N15,Climate!A:A,Climate!D:D)</f>
+        <v>Dry</v>
+      </c>
+      <c r="Q15" s="1" t="str">
+        <f>LOOKUP(N15,Climate!A:A,Climate!C:C)</f>
+        <v>Dry</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2233,8 +2665,23 @@
       <c r="M16" s="1" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N16" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="O16" s="1" t="str">
+        <f>LOOKUP(N16,Climate!A:A,Climate!B:B)</f>
+        <v>Temperate</v>
+      </c>
+      <c r="P16" s="1" t="str">
+        <f>LOOKUP(N16,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q16" s="1" t="str">
+        <f>LOOKUP(N16,Climate!A:A,Climate!C:C)</f>
+        <v xml:space="preserve">Dry, Warm </v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2269,8 +2716,23 @@
       <c r="M17" s="27" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N17" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="O17" s="1" t="str">
+        <f>LOOKUP(N17,Climate!A:A,Climate!B:B)</f>
+        <v>Temperate</v>
+      </c>
+      <c r="P17" s="1" t="str">
+        <f>LOOKUP(N17,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q17" s="1" t="str">
+        <f>LOOKUP(N17,Climate!A:A,Climate!C:C)</f>
+        <v xml:space="preserve">Dry, Hot </v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2303,8 +2765,23 @@
       <c r="M18" s="27" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N18" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="O18" s="1" t="str">
+        <f>LOOKUP(N18,Climate!A:A,Climate!B:B)</f>
+        <v>Temperate</v>
+      </c>
+      <c r="P18" s="1" t="str">
+        <f>LOOKUP(N18,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q18" s="1" t="str">
+        <f>LOOKUP(N18,Climate!A:A,Climate!C:C)</f>
+        <v xml:space="preserve">Dry, Hot </v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2334,8 +2811,23 @@
       <c r="M19" s="1" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N19" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="O19" s="1" t="str">
+        <f>LOOKUP(N19,Climate!A:A,Climate!B:B)</f>
+        <v>Arid Cold</v>
+      </c>
+      <c r="P19" s="1" t="str">
+        <f>LOOKUP(N19,Climate!A:A,Climate!D:D)</f>
+        <v>Dry</v>
+      </c>
+      <c r="Q19" s="1" t="str">
+        <f>LOOKUP(N19,Climate!A:A,Climate!C:C)</f>
+        <v>Dry</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2370,8 +2862,23 @@
       <c r="M20" s="1" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N20" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="O20" s="1" t="str">
+        <f>LOOKUP(N20,Climate!A:A,Climate!B:B)</f>
+        <v>Arid Cold</v>
+      </c>
+      <c r="P20" s="1" t="str">
+        <f>LOOKUP(N20,Climate!A:A,Climate!D:D)</f>
+        <v>Dry</v>
+      </c>
+      <c r="Q20" s="1" t="str">
+        <f>LOOKUP(N20,Climate!A:A,Climate!C:C)</f>
+        <v>Dry</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2406,8 +2913,23 @@
       <c r="M21" s="1" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N21" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="O21" s="1" t="str">
+        <f>LOOKUP(N21,Climate!A:A,Climate!B:B)</f>
+        <v>Continental</v>
+      </c>
+      <c r="P21" s="1" t="str">
+        <f>LOOKUP(N21,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q21" s="1" t="str">
+        <f>LOOKUP(N21,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2439,8 +2961,23 @@
       <c r="M22" s="27" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N22" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="O22" s="1" t="str">
+        <f>LOOKUP(N22,Climate!A:A,Climate!B:B)</f>
+        <v>Temperate</v>
+      </c>
+      <c r="P22" s="1" t="str">
+        <f>LOOKUP(N22,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q22" s="1" t="str">
+        <f>LOOKUP(N22,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2477,8 +3014,23 @@
       <c r="M23" s="1" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N23" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="O23" s="1" t="str">
+        <f>LOOKUP(N23,Climate!A:A,Climate!B:B)</f>
+        <v>Temperate</v>
+      </c>
+      <c r="P23" s="1" t="str">
+        <f>LOOKUP(N23,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q23" s="1" t="str">
+        <f>LOOKUP(N23,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2510,8 +3062,23 @@
       <c r="M24" s="1" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N24" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="O24" s="1" t="str">
+        <f>LOOKUP(N24,Climate!A:A,Climate!B:B)</f>
+        <v>Temperate</v>
+      </c>
+      <c r="P24" s="1" t="str">
+        <f>LOOKUP(N24,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q24" s="1" t="str">
+        <f>LOOKUP(N24,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2551,8 +3118,23 @@
       <c r="M25" s="1" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N25" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="O25" s="1" t="str">
+        <f>LOOKUP(N25,Climate!A:A,Climate!B:B)</f>
+        <v>Temperate</v>
+      </c>
+      <c r="P25" s="1" t="str">
+        <f>LOOKUP(N25,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q25" s="1" t="str">
+        <f>LOOKUP(N25,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2590,8 +3172,23 @@
       <c r="M26" s="1" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N26" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="O26" s="1" t="str">
+        <f>LOOKUP(N26,Climate!A:A,Climate!B:B)</f>
+        <v>Tropical Savanna</v>
+      </c>
+      <c r="P26" s="1" t="str">
+        <f>LOOKUP(N26,Climate!A:A,Climate!D:D)</f>
+        <v>Dry</v>
+      </c>
+      <c r="Q26" s="1" t="str">
+        <f>LOOKUP(N26,Climate!A:A,Climate!C:C)</f>
+        <v>Wet</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2628,8 +3225,23 @@
       <c r="M27" s="1" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N27" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="O27" s="1" t="str">
+        <f>LOOKUP(N27,Climate!A:A,Climate!B:B)</f>
+        <v>Tropical Monsoon</v>
+      </c>
+      <c r="P27" s="1" t="str">
+        <f>LOOKUP(N27,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q27" s="1" t="str">
+        <f>LOOKUP(N27,Climate!A:A,Climate!C:C)</f>
+        <v>Wet</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2666,8 +3278,23 @@
       <c r="M28" s="1" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N28" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="O28" s="1" t="str">
+        <f>LOOKUP(N28,Climate!A:A,Climate!B:B)</f>
+        <v>Temperate</v>
+      </c>
+      <c r="P28" s="1" t="str">
+        <f>LOOKUP(N28,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q28" s="1" t="str">
+        <f>LOOKUP(N28,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -2703,8 +3330,23 @@
       <c r="M29" s="1" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N29" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="O29" s="1" t="str">
+        <f>LOOKUP(N29,Climate!A:A,Climate!B:B)</f>
+        <v>Temperate</v>
+      </c>
+      <c r="P29" s="1" t="str">
+        <f>LOOKUP(N29,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q29" s="1" t="str">
+        <f>LOOKUP(N29,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -2742,8 +3384,23 @@
       <c r="M30" s="1" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N30" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="O30" s="1" t="str">
+        <f>LOOKUP(N30,Climate!A:A,Climate!B:B)</f>
+        <v>Temperate</v>
+      </c>
+      <c r="P30" s="1" t="str">
+        <f>LOOKUP(N30,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q30" s="1" t="str">
+        <f>LOOKUP(N30,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -2778,8 +3435,23 @@
       <c r="M31" s="1" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N31" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="O31" s="1" t="str">
+        <f>LOOKUP(N31,Climate!A:A,Climate!B:B)</f>
+        <v>Temperate</v>
+      </c>
+      <c r="P31" s="1" t="str">
+        <f>LOOKUP(N31,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q31" s="1" t="str">
+        <f>LOOKUP(N31,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2811,8 +3483,23 @@
       <c r="M32" s="1" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N32" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="O32" s="1" t="str">
+        <f>LOOKUP(N32,Climate!A:A,Climate!B:B)</f>
+        <v>Temperate</v>
+      </c>
+      <c r="P32" s="1" t="str">
+        <f>LOOKUP(N32,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q32" s="1" t="str">
+        <f>LOOKUP(N32,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2849,8 +3536,23 @@
       <c r="M33" s="1" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N33" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="O33" s="1" t="str">
+        <f>LOOKUP(N33,Climate!A:A,Climate!B:B)</f>
+        <v>Arid Hot</v>
+      </c>
+      <c r="P33" s="1" t="str">
+        <f>LOOKUP(N33,Climate!A:A,Climate!D:D)</f>
+        <v>Dry</v>
+      </c>
+      <c r="Q33" s="1" t="str">
+        <f>LOOKUP(N33,Climate!A:A,Climate!C:C)</f>
+        <v>Dry</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <f t="shared" ref="A34:A65" si="2">A33+1</f>
         <v>32</v>
@@ -2882,8 +3584,23 @@
       <c r="M34" s="27" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N34" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="O34" s="1" t="str">
+        <f>LOOKUP(N34,Climate!A:A,Climate!B:B)</f>
+        <v>Continental</v>
+      </c>
+      <c r="P34" s="1" t="str">
+        <f>LOOKUP(N34,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q34" s="1" t="str">
+        <f>LOOKUP(N34,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -2915,8 +3632,23 @@
       <c r="M35" s="1" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N35" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="O35" s="1" t="str">
+        <f>LOOKUP(N35,Climate!A:A,Climate!B:B)</f>
+        <v>Continental</v>
+      </c>
+      <c r="P35" s="1" t="str">
+        <f>LOOKUP(N35,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q35" s="1" t="str">
+        <f>LOOKUP(N35,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -2948,8 +3680,23 @@
       <c r="M36" s="1" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N36" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="O36" s="1" t="str">
+        <f>LOOKUP(N36,Climate!A:A,Climate!B:B)</f>
+        <v>Arid Cold</v>
+      </c>
+      <c r="P36" s="1" t="str">
+        <f>LOOKUP(N36,Climate!A:A,Climate!D:D)</f>
+        <v>Dry</v>
+      </c>
+      <c r="Q36" s="1" t="str">
+        <f>LOOKUP(N36,Climate!A:A,Climate!C:C)</f>
+        <v>Dry</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -2981,8 +3728,23 @@
       <c r="M37" s="27" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N37" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="O37" s="1" t="str">
+        <f>LOOKUP(N37,Climate!A:A,Climate!B:B)</f>
+        <v>Continental</v>
+      </c>
+      <c r="P37" s="1" t="str">
+        <f>LOOKUP(N37,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q37" s="1" t="str">
+        <f>LOOKUP(N37,Climate!A:A,Climate!C:C)</f>
+        <v xml:space="preserve">Dry, Warm </v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -3017,8 +3779,23 @@
       <c r="M38" s="1" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N38" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="O38" s="1" t="str">
+        <f>LOOKUP(N38,Climate!A:A,Climate!B:B)</f>
+        <v>Continental</v>
+      </c>
+      <c r="P38" s="1" t="str">
+        <f>LOOKUP(N38,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q38" s="1" t="str">
+        <f>LOOKUP(N38,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <f t="shared" si="2"/>
         <v>37</v>
@@ -3050,8 +3827,23 @@
       <c r="M39" s="1" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N39" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="O39" s="1" t="str">
+        <f>LOOKUP(N39,Climate!A:A,Climate!B:B)</f>
+        <v>Continental</v>
+      </c>
+      <c r="P39" s="1" t="str">
+        <f>LOOKUP(N39,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q39" s="1" t="str">
+        <f>LOOKUP(N39,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -3087,8 +3879,23 @@
       <c r="M40" s="1" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N40" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="O40" s="1" t="str">
+        <f>LOOKUP(N40,Climate!A:A,Climate!B:B)</f>
+        <v>Continental</v>
+      </c>
+      <c r="P40" s="1" t="str">
+        <f>LOOKUP(N40,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q40" s="1" t="str">
+        <f>LOOKUP(N40,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -3120,8 +3927,23 @@
       <c r="M41" s="1" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N41" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="O41" s="1" t="str">
+        <f>LOOKUP(N41,Climate!A:A,Climate!B:B)</f>
+        <v>Continental</v>
+      </c>
+      <c r="P41" s="1" t="str">
+        <f>LOOKUP(N41,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q41" s="1" t="str">
+        <f>LOOKUP(N41,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -3153,8 +3975,23 @@
       <c r="M42" s="1" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N42" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="O42" s="1" t="str">
+        <f>LOOKUP(N42,Climate!A:A,Climate!B:B)</f>
+        <v>Temperate</v>
+      </c>
+      <c r="P42" s="1" t="str">
+        <f>LOOKUP(N42,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q42" s="1" t="str">
+        <f>LOOKUP(N42,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -3186,8 +4023,23 @@
       <c r="M43" s="27" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N43" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="O43" s="1" t="str">
+        <f>LOOKUP(N43,Climate!A:A,Climate!B:B)</f>
+        <v>Temperate</v>
+      </c>
+      <c r="P43" s="1" t="str">
+        <f>LOOKUP(N43,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q43" s="1" t="str">
+        <f>LOOKUP(N43,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -3222,8 +4074,23 @@
       <c r="M44" s="1" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N44" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="O44" s="1" t="str">
+        <f>LOOKUP(N44,Climate!A:A,Climate!B:B)</f>
+        <v>Temperate</v>
+      </c>
+      <c r="P44" s="1" t="str">
+        <f>LOOKUP(N44,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q44" s="1" t="str">
+        <f>LOOKUP(N44,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -3255,8 +4122,23 @@
       <c r="M45" s="27" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N45" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="O45" s="1" t="str">
+        <f>LOOKUP(N45,Climate!A:A,Climate!B:B)</f>
+        <v>Temperate</v>
+      </c>
+      <c r="P45" s="1" t="str">
+        <f>LOOKUP(N45,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q45" s="1" t="str">
+        <f>LOOKUP(N45,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -3291,8 +4173,23 @@
       <c r="M46" s="1" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N46" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="O46" s="1" t="str">
+        <f>LOOKUP(N46,Climate!A:A,Climate!B:B)</f>
+        <v>Temperate</v>
+      </c>
+      <c r="P46" s="1" t="str">
+        <f>LOOKUP(N46,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q46" s="1" t="str">
+        <f>LOOKUP(N46,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -3327,8 +4224,23 @@
       <c r="M47" s="1" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N47" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="O47" s="1" t="str">
+        <f>LOOKUP(N47,Climate!A:A,Climate!B:B)</f>
+        <v>Continental</v>
+      </c>
+      <c r="P47" s="1" t="str">
+        <f>LOOKUP(N47,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q47" s="1" t="str">
+        <f>LOOKUP(N47,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -3360,8 +4272,23 @@
       <c r="M48" s="27" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N48" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="O48" s="1" t="str">
+        <f>LOOKUP(N48,Climate!A:A,Climate!B:B)</f>
+        <v>Temperate</v>
+      </c>
+      <c r="P48" s="1" t="str">
+        <f>LOOKUP(N48,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q48" s="1" t="str">
+        <f>LOOKUP(N48,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <f t="shared" si="2"/>
         <v>47</v>
@@ -3396,8 +4323,23 @@
       <c r="M49" s="1" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N49" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="O49" s="1" t="str">
+        <f>LOOKUP(N49,Climate!A:A,Climate!B:B)</f>
+        <v>Temperate</v>
+      </c>
+      <c r="P49" s="1" t="str">
+        <f>LOOKUP(N49,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q49" s="1" t="str">
+        <f>LOOKUP(N49,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <f t="shared" si="2"/>
         <v>48</v>
@@ -3429,8 +4371,23 @@
       <c r="M50" s="1" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N50" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="O50" s="1" t="str">
+        <f>LOOKUP(N50,Climate!A:A,Climate!B:B)</f>
+        <v>Continental</v>
+      </c>
+      <c r="P50" s="1" t="str">
+        <f>LOOKUP(N50,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q50" s="1" t="str">
+        <f>LOOKUP(N50,Climate!A:A,Climate!C:C)</f>
+        <v>Warm, Wet</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <f t="shared" si="2"/>
         <v>49</v>
@@ -3462,8 +4419,23 @@
       <c r="M51" s="1" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N51" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="O51" s="1" t="str">
+        <f>LOOKUP(N51,Climate!A:A,Climate!B:B)</f>
+        <v>Continental</v>
+      </c>
+      <c r="P51" s="1" t="str">
+        <f>LOOKUP(N51,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q51" s="1" t="str">
+        <f>LOOKUP(N51,Climate!A:A,Climate!C:C)</f>
+        <v>Warm, Wet</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <f t="shared" si="2"/>
         <v>50</v>
@@ -3498,8 +4470,23 @@
       <c r="M52" s="1" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N52" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="O52" s="1" t="str">
+        <f>LOOKUP(N52,Climate!A:A,Climate!B:B)</f>
+        <v>Continental</v>
+      </c>
+      <c r="P52" s="1" t="str">
+        <f>LOOKUP(N52,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q52" s="1" t="str">
+        <f>LOOKUP(N52,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <f t="shared" si="2"/>
         <v>51</v>
@@ -3534,8 +4521,23 @@
       <c r="M53" s="1" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N53" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="O53" s="1" t="str">
+        <f>LOOKUP(N53,Climate!A:A,Climate!B:B)</f>
+        <v>Continental</v>
+      </c>
+      <c r="P53" s="1" t="str">
+        <f>LOOKUP(N53,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q53" s="1" t="str">
+        <f>LOOKUP(N53,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <f t="shared" si="2"/>
         <v>52</v>
@@ -3567,8 +4569,23 @@
       <c r="M54" s="1" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N54" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="O54" s="1" t="str">
+        <f>LOOKUP(N54,Climate!A:A,Climate!B:B)</f>
+        <v>Continental</v>
+      </c>
+      <c r="P54" s="1" t="str">
+        <f>LOOKUP(N54,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q54" s="1" t="str">
+        <f>LOOKUP(N54,Climate!A:A,Climate!C:C)</f>
+        <v>Warm, Wet</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <f t="shared" si="2"/>
         <v>53</v>
@@ -3598,8 +4615,23 @@
       <c r="M55" s="1" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N55" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="O55" s="1" t="str">
+        <f>LOOKUP(N55,Climate!A:A,Climate!B:B)</f>
+        <v>Continental</v>
+      </c>
+      <c r="P55" s="1" t="str">
+        <f>LOOKUP(N55,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q55" s="1" t="str">
+        <f>LOOKUP(N55,Climate!A:A,Climate!C:C)</f>
+        <v>Warm, Wet</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <f t="shared" si="2"/>
         <v>54</v>
@@ -3635,8 +4667,23 @@
       <c r="M56" s="1" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N56" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="O56" s="1" t="str">
+        <f>LOOKUP(N56,Climate!A:A,Climate!B:B)</f>
+        <v>Continental</v>
+      </c>
+      <c r="P56" s="1" t="str">
+        <f>LOOKUP(N56,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q56" s="1" t="str">
+        <f>LOOKUP(N56,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <f t="shared" si="2"/>
         <v>55</v>
@@ -3668,8 +4715,23 @@
       <c r="M57" s="27" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N57" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="O57" s="1" t="str">
+        <f>LOOKUP(N57,Climate!A:A,Climate!B:B)</f>
+        <v>Continental</v>
+      </c>
+      <c r="P57" s="1" t="str">
+        <f>LOOKUP(N57,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q57" s="1" t="str">
+        <f>LOOKUP(N57,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <f t="shared" si="2"/>
         <v>56</v>
@@ -3704,8 +4766,23 @@
       <c r="M58" s="1" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N58" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="O58" s="1" t="str">
+        <f>LOOKUP(N58,Climate!A:A,Climate!B:B)</f>
+        <v>Continental</v>
+      </c>
+      <c r="P58" s="1" t="str">
+        <f>LOOKUP(N58,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q58" s="1" t="str">
+        <f>LOOKUP(N58,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <f t="shared" si="2"/>
         <v>57</v>
@@ -3743,8 +4820,23 @@
       <c r="M59" s="1" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N59" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="O59" s="1" t="str">
+        <f>LOOKUP(N59,Climate!A:A,Climate!B:B)</f>
+        <v>Temperate</v>
+      </c>
+      <c r="P59" s="1" t="str">
+        <f>LOOKUP(N59,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q59" s="1" t="str">
+        <f>LOOKUP(N59,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <f t="shared" si="2"/>
         <v>58</v>
@@ -3776,8 +4868,23 @@
       <c r="M60" s="1" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N60" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="O60" s="1" t="str">
+        <f>LOOKUP(N60,Climate!A:A,Climate!B:B)</f>
+        <v>Temperate</v>
+      </c>
+      <c r="P60" s="1" t="str">
+        <f>LOOKUP(N60,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q60" s="1" t="str">
+        <f>LOOKUP(N60,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <f t="shared" si="2"/>
         <v>59</v>
@@ -3809,8 +4916,23 @@
       <c r="M61" s="1" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N61" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="O61" s="1" t="str">
+        <f>LOOKUP(N61,Climate!A:A,Climate!B:B)</f>
+        <v>Arid Cold</v>
+      </c>
+      <c r="P61" s="1" t="str">
+        <f>LOOKUP(N61,Climate!A:A,Climate!D:D)</f>
+        <v>Dry</v>
+      </c>
+      <c r="Q61" s="1" t="str">
+        <f>LOOKUP(N61,Climate!A:A,Climate!C:C)</f>
+        <v>Dry</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <f t="shared" si="2"/>
         <v>60</v>
@@ -3843,8 +4965,23 @@
       <c r="M62" s="1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N62" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="O62" s="1" t="str">
+        <f>LOOKUP(N62,Climate!A:A,Climate!B:B)</f>
+        <v>Continental</v>
+      </c>
+      <c r="P62" s="1" t="str">
+        <f>LOOKUP(N62,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q62" s="1" t="str">
+        <f>LOOKUP(N62,Climate!A:A,Climate!C:C)</f>
+        <v>Warm, Wet</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <f t="shared" si="2"/>
         <v>61</v>
@@ -3876,8 +5013,23 @@
       <c r="M63" s="1" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N63" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="O63" s="1" t="str">
+        <f>LOOKUP(N63,Climate!A:A,Climate!B:B)</f>
+        <v>Arid Cold</v>
+      </c>
+      <c r="P63" s="1" t="str">
+        <f>LOOKUP(N63,Climate!A:A,Climate!D:D)</f>
+        <v>Dry</v>
+      </c>
+      <c r="Q63" s="1" t="str">
+        <f>LOOKUP(N63,Climate!A:A,Climate!C:C)</f>
+        <v>Dry</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <f t="shared" si="2"/>
         <v>62</v>
@@ -3912,8 +5064,23 @@
       <c r="M64" s="1" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="65" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N64" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="O64" s="1" t="str">
+        <f>LOOKUP(N64,Climate!A:A,Climate!B:B)</f>
+        <v>Temperate</v>
+      </c>
+      <c r="P64" s="1" t="str">
+        <f>LOOKUP(N64,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q64" s="1" t="str">
+        <f>LOOKUP(N64,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <f t="shared" si="2"/>
         <v>63</v>
@@ -3949,8 +5116,23 @@
       <c r="M65" s="1" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N65" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="O65" s="1" t="str">
+        <f>LOOKUP(N65,Climate!A:A,Climate!B:B)</f>
+        <v>Temperate</v>
+      </c>
+      <c r="P65" s="1" t="str">
+        <f>LOOKUP(N65,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q65" s="1" t="str">
+        <f>LOOKUP(N65,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <f t="shared" ref="A66:A97" si="4">A65+1</f>
         <v>64</v>
@@ -3982,8 +5164,23 @@
       <c r="M66" s="1" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N66" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="O66" s="1" t="str">
+        <f>LOOKUP(N66,Climate!A:A,Climate!B:B)</f>
+        <v>Continental</v>
+      </c>
+      <c r="P66" s="1" t="str">
+        <f>LOOKUP(N66,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q66" s="1" t="str">
+        <f>LOOKUP(N66,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <f t="shared" si="4"/>
         <v>65</v>
@@ -4015,8 +5212,23 @@
       <c r="M67" s="1" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N67" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="O67" s="1" t="str">
+        <f>LOOKUP(N67,Climate!A:A,Climate!B:B)</f>
+        <v>Continental</v>
+      </c>
+      <c r="P67" s="1" t="str">
+        <f>LOOKUP(N67,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q67" s="1" t="str">
+        <f>LOOKUP(N67,Climate!A:A,Climate!C:C)</f>
+        <v>Warm, Wet</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <f t="shared" si="4"/>
         <v>66</v>
@@ -4048,8 +5260,23 @@
       <c r="M68" s="1" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N68" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="O68" s="1" t="str">
+        <f>LOOKUP(N68,Climate!A:A,Climate!B:B)</f>
+        <v>Continental</v>
+      </c>
+      <c r="P68" s="1" t="str">
+        <f>LOOKUP(N68,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q68" s="1" t="str">
+        <f>LOOKUP(N68,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <f t="shared" si="4"/>
         <v>67</v>
@@ -4081,8 +5308,23 @@
       <c r="M69" s="1" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N69" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="O69" s="1" t="str">
+        <f>LOOKUP(N69,Climate!A:A,Climate!B:B)</f>
+        <v>Continental</v>
+      </c>
+      <c r="P69" s="1" t="str">
+        <f>LOOKUP(N69,Climate!A:A,Climate!D:D)</f>
+        <v>Wet</v>
+      </c>
+      <c r="Q69" s="1" t="str">
+        <f>LOOKUP(N69,Climate!A:A,Climate!C:C)</f>
+        <v>Hot, Wet</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <f t="shared" si="4"/>
         <v>68</v>
@@ -4114,8 +5356,23 @@
       <c r="M70" s="1" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N70" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O70" s="1" t="str">
+        <f>LOOKUP(N70,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P70" s="1" t="str">
+        <f>LOOKUP(N70,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q70" s="1" t="str">
+        <f>LOOKUP(N70,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <f t="shared" si="4"/>
         <v>69</v>
@@ -4147,8 +5404,23 @@
       <c r="M71" s="1" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="72" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N71" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O71" s="1" t="str">
+        <f>LOOKUP(N71,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P71" s="1" t="str">
+        <f>LOOKUP(N71,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q71" s="1" t="str">
+        <f>LOOKUP(N71,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <f t="shared" si="4"/>
         <v>70</v>
@@ -4182,8 +5454,23 @@
       <c r="M72" s="1" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N72" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O72" s="1" t="str">
+        <f>LOOKUP(N72,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P72" s="1" t="str">
+        <f>LOOKUP(N72,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q72" s="1" t="str">
+        <f>LOOKUP(N72,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <f t="shared" si="4"/>
         <v>71</v>
@@ -4215,8 +5502,23 @@
       <c r="M73" s="27" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="74" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N73" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O73" s="1" t="str">
+        <f>LOOKUP(N73,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P73" s="1" t="str">
+        <f>LOOKUP(N73,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q73" s="1" t="str">
+        <f>LOOKUP(N73,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -4250,8 +5552,23 @@
       <c r="M74" s="1" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N74" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O74" s="1" t="str">
+        <f>LOOKUP(N74,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P74" s="1" t="str">
+        <f>LOOKUP(N74,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q74" s="1" t="str">
+        <f>LOOKUP(N74,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <f t="shared" si="4"/>
         <v>73</v>
@@ -4283,8 +5600,23 @@
       <c r="M75" s="27" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N75" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O75" s="1" t="str">
+        <f>LOOKUP(N75,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P75" s="1" t="str">
+        <f>LOOKUP(N75,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q75" s="1" t="str">
+        <f>LOOKUP(N75,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <f t="shared" si="4"/>
         <v>74</v>
@@ -4316,8 +5648,23 @@
       <c r="M76" s="27" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N76" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O76" s="1" t="str">
+        <f>LOOKUP(N76,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P76" s="1" t="str">
+        <f>LOOKUP(N76,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q76" s="1" t="str">
+        <f>LOOKUP(N76,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <f t="shared" si="4"/>
         <v>75</v>
@@ -4349,8 +5696,23 @@
       <c r="M77" s="1" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N77" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O77" s="1" t="str">
+        <f>LOOKUP(N77,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P77" s="1" t="str">
+        <f>LOOKUP(N77,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q77" s="1" t="str">
+        <f>LOOKUP(N77,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <f t="shared" si="4"/>
         <v>76</v>
@@ -4385,8 +5747,23 @@
       <c r="M78" s="1" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N78" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O78" s="1" t="str">
+        <f>LOOKUP(N78,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P78" s="1" t="str">
+        <f>LOOKUP(N78,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q78" s="1" t="str">
+        <f>LOOKUP(N78,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <f t="shared" si="4"/>
         <v>77</v>
@@ -4418,8 +5795,23 @@
       <c r="M79" s="1" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N79" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O79" s="1" t="str">
+        <f>LOOKUP(N79,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P79" s="1" t="str">
+        <f>LOOKUP(N79,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q79" s="1" t="str">
+        <f>LOOKUP(N79,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <f t="shared" si="4"/>
         <v>78</v>
@@ -4454,8 +5846,23 @@
       <c r="M80" s="1" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N80" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O80" s="1" t="str">
+        <f>LOOKUP(N80,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P80" s="1" t="str">
+        <f>LOOKUP(N80,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q80" s="1" t="str">
+        <f>LOOKUP(N80,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <f t="shared" si="4"/>
         <v>79</v>
@@ -4496,8 +5903,23 @@
       <c r="M81" s="1" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N81" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O81" s="1" t="str">
+        <f>LOOKUP(N81,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P81" s="1" t="str">
+        <f>LOOKUP(N81,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q81" s="1" t="str">
+        <f>LOOKUP(N81,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <f t="shared" si="4"/>
         <v>80</v>
@@ -4532,8 +5954,23 @@
       <c r="M82" s="1" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N82" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O82" s="1" t="str">
+        <f>LOOKUP(N82,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P82" s="1" t="str">
+        <f>LOOKUP(N82,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q82" s="1" t="str">
+        <f>LOOKUP(N82,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <f t="shared" si="4"/>
         <v>81</v>
@@ -4568,8 +6005,23 @@
       <c r="M83" s="27" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N83" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O83" s="1" t="str">
+        <f>LOOKUP(N83,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P83" s="1" t="str">
+        <f>LOOKUP(N83,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q83" s="1" t="str">
+        <f>LOOKUP(N83,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <f t="shared" si="4"/>
         <v>82</v>
@@ -4604,8 +6056,23 @@
       <c r="M84" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N84" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O84" s="1" t="str">
+        <f>LOOKUP(N84,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P84" s="1" t="str">
+        <f>LOOKUP(N84,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q84" s="1" t="str">
+        <f>LOOKUP(N84,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <f t="shared" si="4"/>
         <v>83</v>
@@ -4640,8 +6107,23 @@
       <c r="M85" s="1" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N85" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O85" s="1" t="str">
+        <f>LOOKUP(N85,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P85" s="1" t="str">
+        <f>LOOKUP(N85,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q85" s="1" t="str">
+        <f>LOOKUP(N85,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <f t="shared" si="4"/>
         <v>84</v>
@@ -4676,8 +6158,23 @@
       <c r="M86" s="1" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N86" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O86" s="1" t="str">
+        <f>LOOKUP(N86,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P86" s="1" t="str">
+        <f>LOOKUP(N86,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q86" s="1" t="str">
+        <f>LOOKUP(N86,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <f t="shared" si="4"/>
         <v>85</v>
@@ -4712,8 +6209,23 @@
       <c r="M87" s="1" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N87" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O87" s="1" t="str">
+        <f>LOOKUP(N87,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P87" s="1" t="str">
+        <f>LOOKUP(N87,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q87" s="1" t="str">
+        <f>LOOKUP(N87,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <f t="shared" si="4"/>
         <v>86</v>
@@ -4748,8 +6260,23 @@
       <c r="M88" s="1" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="89" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N88" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O88" s="1" t="str">
+        <f>LOOKUP(N88,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P88" s="1" t="str">
+        <f>LOOKUP(N88,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q88" s="1" t="str">
+        <f>LOOKUP(N88,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <f t="shared" si="4"/>
         <v>87</v>
@@ -4783,8 +6310,23 @@
       <c r="M89" s="1" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N89" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O89" s="1" t="str">
+        <f>LOOKUP(N89,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P89" s="1" t="str">
+        <f>LOOKUP(N89,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q89" s="1" t="str">
+        <f>LOOKUP(N89,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <f t="shared" si="4"/>
         <v>88</v>
@@ -4816,8 +6358,23 @@
       <c r="M90" s="27" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N90" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O90" s="1" t="str">
+        <f>LOOKUP(N90,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P90" s="1" t="str">
+        <f>LOOKUP(N90,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q90" s="1" t="str">
+        <f>LOOKUP(N90,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <f t="shared" si="4"/>
         <v>89</v>
@@ -4855,8 +6412,23 @@
       <c r="M91" s="1" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N91" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O91" s="1" t="str">
+        <f>LOOKUP(N91,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P91" s="1" t="str">
+        <f>LOOKUP(N91,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q91" s="1" t="str">
+        <f>LOOKUP(N91,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <f t="shared" si="4"/>
         <v>90</v>
@@ -4891,8 +6463,23 @@
       <c r="M92" s="1" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N92" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O92" s="1" t="str">
+        <f>LOOKUP(N92,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P92" s="1" t="str">
+        <f>LOOKUP(N92,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q92" s="1" t="str">
+        <f>LOOKUP(N92,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <f t="shared" si="4"/>
         <v>91</v>
@@ -4929,8 +6516,23 @@
       <c r="M93" s="27" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N93" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O93" s="1" t="str">
+        <f>LOOKUP(N93,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P93" s="1" t="str">
+        <f>LOOKUP(N93,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q93" s="1" t="str">
+        <f>LOOKUP(N93,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <f t="shared" si="4"/>
         <v>92</v>
@@ -4965,8 +6567,23 @@
       <c r="M94" s="1" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N94" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O94" s="1" t="str">
+        <f>LOOKUP(N94,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P94" s="1" t="str">
+        <f>LOOKUP(N94,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q94" s="1" t="str">
+        <f>LOOKUP(N94,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <f t="shared" si="4"/>
         <v>93</v>
@@ -4998,8 +6615,23 @@
       <c r="M95" s="1" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N95" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O95" s="1" t="str">
+        <f>LOOKUP(N95,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P95" s="1" t="str">
+        <f>LOOKUP(N95,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q95" s="1" t="str">
+        <f>LOOKUP(N95,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <f t="shared" si="4"/>
         <v>94</v>
@@ -5031,8 +6663,23 @@
       <c r="M96" s="1" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N96" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O96" s="1" t="str">
+        <f>LOOKUP(N96,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P96" s="1" t="str">
+        <f>LOOKUP(N96,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q96" s="1" t="str">
+        <f>LOOKUP(N96,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <f t="shared" si="4"/>
         <v>95</v>
@@ -5064,8 +6711,23 @@
       <c r="M97" s="27" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N97" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O97" s="1" t="str">
+        <f>LOOKUP(N97,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P97" s="1" t="str">
+        <f>LOOKUP(N97,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q97" s="1" t="str">
+        <f>LOOKUP(N97,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <f t="shared" ref="A98:A121" si="6">A97+1</f>
         <v>96</v>
@@ -5097,8 +6759,23 @@
       <c r="M98" s="1" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N98" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O98" s="1" t="str">
+        <f>LOOKUP(N98,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P98" s="1" t="str">
+        <f>LOOKUP(N98,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q98" s="1" t="str">
+        <f>LOOKUP(N98,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <f t="shared" si="6"/>
         <v>97</v>
@@ -5133,8 +6810,23 @@
       <c r="M99" s="1" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N99" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O99" s="1" t="str">
+        <f>LOOKUP(N99,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P99" s="1" t="str">
+        <f>LOOKUP(N99,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q99" s="1" t="str">
+        <f>LOOKUP(N99,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <f t="shared" si="6"/>
         <v>98</v>
@@ -5169,8 +6861,23 @@
       <c r="M100" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N100" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O100" s="1" t="str">
+        <f>LOOKUP(N100,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P100" s="1" t="str">
+        <f>LOOKUP(N100,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q100" s="1" t="str">
+        <f>LOOKUP(N100,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <f t="shared" si="6"/>
         <v>99</v>
@@ -5205,8 +6912,23 @@
       <c r="M101" s="1" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N101" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O101" s="1" t="str">
+        <f>LOOKUP(N101,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P101" s="1" t="str">
+        <f>LOOKUP(N101,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q101" s="1" t="str">
+        <f>LOOKUP(N101,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <f t="shared" si="6"/>
         <v>100</v>
@@ -5241,8 +6963,23 @@
       <c r="M102" s="27" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N102" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O102" s="1" t="str">
+        <f>LOOKUP(N102,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P102" s="1" t="str">
+        <f>LOOKUP(N102,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q102" s="1" t="str">
+        <f>LOOKUP(N102,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <f t="shared" si="6"/>
         <v>101</v>
@@ -5277,8 +7014,23 @@
       <c r="M103" s="1" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N103" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O103" s="1" t="str">
+        <f>LOOKUP(N103,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P103" s="1" t="str">
+        <f>LOOKUP(N103,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q103" s="1" t="str">
+        <f>LOOKUP(N103,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <f t="shared" si="6"/>
         <v>102</v>
@@ -5313,8 +7065,23 @@
       <c r="M104" s="1" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N104" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O104" s="1" t="str">
+        <f>LOOKUP(N104,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P104" s="1" t="str">
+        <f>LOOKUP(N104,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q104" s="1" t="str">
+        <f>LOOKUP(N104,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <f t="shared" si="6"/>
         <v>103</v>
@@ -5352,8 +7119,23 @@
       <c r="M105" s="1" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N105" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O105" s="1" t="str">
+        <f>LOOKUP(N105,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P105" s="1" t="str">
+        <f>LOOKUP(N105,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q105" s="1" t="str">
+        <f>LOOKUP(N105,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <f t="shared" si="6"/>
         <v>104</v>
@@ -5385,8 +7167,23 @@
       <c r="M106" s="27" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N106" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O106" s="1" t="str">
+        <f>LOOKUP(N106,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P106" s="1" t="str">
+        <f>LOOKUP(N106,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q106" s="1" t="str">
+        <f>LOOKUP(N106,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <f t="shared" si="6"/>
         <v>105</v>
@@ -5421,8 +7218,23 @@
       <c r="M107" s="1" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N107" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O107" s="1" t="str">
+        <f>LOOKUP(N107,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P107" s="1" t="str">
+        <f>LOOKUP(N107,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q107" s="1" t="str">
+        <f>LOOKUP(N107,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <f t="shared" si="6"/>
         <v>106</v>
@@ -5457,8 +7269,23 @@
       <c r="M108" s="27" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N108" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O108" s="1" t="str">
+        <f>LOOKUP(N108,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P108" s="1" t="str">
+        <f>LOOKUP(N108,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q108" s="1" t="str">
+        <f>LOOKUP(N108,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <f t="shared" si="6"/>
         <v>107</v>
@@ -5493,8 +7320,23 @@
       <c r="M109" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N109" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O109" s="1" t="str">
+        <f>LOOKUP(N109,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P109" s="1" t="str">
+        <f>LOOKUP(N109,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q109" s="1" t="str">
+        <f>LOOKUP(N109,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <f t="shared" si="6"/>
         <v>108</v>
@@ -5532,8 +7374,23 @@
       <c r="M110" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N110" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O110" s="1" t="str">
+        <f>LOOKUP(N110,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P110" s="1" t="str">
+        <f>LOOKUP(N110,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q110" s="1" t="str">
+        <f>LOOKUP(N110,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <f t="shared" si="6"/>
         <v>109</v>
@@ -5565,8 +7422,23 @@
       <c r="M111" s="1" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N111" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O111" s="1" t="str">
+        <f>LOOKUP(N111,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P111" s="1" t="str">
+        <f>LOOKUP(N111,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q111" s="1" t="str">
+        <f>LOOKUP(N111,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <f t="shared" si="6"/>
         <v>110</v>
@@ -5598,8 +7470,23 @@
       <c r="M112" s="27" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N112" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O112" s="1" t="str">
+        <f>LOOKUP(N112,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P112" s="1" t="str">
+        <f>LOOKUP(N112,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q112" s="1" t="str">
+        <f>LOOKUP(N112,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <f t="shared" si="6"/>
         <v>111</v>
@@ -5631,8 +7518,23 @@
       <c r="M113" s="1" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N113" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O113" s="1" t="str">
+        <f>LOOKUP(N113,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P113" s="1" t="str">
+        <f>LOOKUP(N113,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q113" s="1" t="str">
+        <f>LOOKUP(N113,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <f t="shared" si="6"/>
         <v>112</v>
@@ -5665,8 +7567,23 @@
       <c r="M114" s="27" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N114" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O114" s="1" t="str">
+        <f>LOOKUP(N114,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P114" s="1" t="str">
+        <f>LOOKUP(N114,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q114" s="1" t="str">
+        <f>LOOKUP(N114,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <f t="shared" si="6"/>
         <v>113</v>
@@ -5701,8 +7618,23 @@
       <c r="M115" s="1" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N115" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O115" s="1" t="str">
+        <f>LOOKUP(N115,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P115" s="1" t="str">
+        <f>LOOKUP(N115,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q115" s="1" t="str">
+        <f>LOOKUP(N115,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <f t="shared" si="6"/>
         <v>114</v>
@@ -5734,8 +7666,23 @@
       <c r="M116" s="1" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N116" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O116" s="1" t="str">
+        <f>LOOKUP(N116,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P116" s="1" t="str">
+        <f>LOOKUP(N116,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q116" s="1" t="str">
+        <f>LOOKUP(N116,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <f t="shared" si="6"/>
         <v>115</v>
@@ -5770,8 +7717,23 @@
       <c r="M117" s="1" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="118" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N117" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O117" s="1" t="str">
+        <f>LOOKUP(N117,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P117" s="1" t="str">
+        <f>LOOKUP(N117,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q117" s="1" t="str">
+        <f>LOOKUP(N117,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="118" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <f t="shared" si="6"/>
         <v>116</v>
@@ -5805,8 +7767,23 @@
       <c r="M118" s="1" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="119" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N118" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O118" s="1" t="str">
+        <f>LOOKUP(N118,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P118" s="1" t="str">
+        <f>LOOKUP(N118,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q118" s="1" t="str">
+        <f>LOOKUP(N118,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="119" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <f t="shared" si="6"/>
         <v>117</v>
@@ -5840,8 +7817,23 @@
       <c r="M119" s="1" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="120" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N119" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O119" s="1" t="str">
+        <f>LOOKUP(N119,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P119" s="1" t="str">
+        <f>LOOKUP(N119,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q119" s="1" t="str">
+        <f>LOOKUP(N119,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="120" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <f t="shared" si="6"/>
         <v>118</v>
@@ -5875,8 +7867,23 @@
       <c r="M120" s="1" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N120" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O120" s="1" t="str">
+        <f>LOOKUP(N120,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P120" s="1" t="str">
+        <f>LOOKUP(N120,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q120" s="1" t="str">
+        <f>LOOKUP(N120,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <f t="shared" si="6"/>
         <v>119</v>
@@ -5907,6 +7914,21 @@
       <c r="L121" s="5"/>
       <c r="M121" s="1" t="s">
         <v>286</v>
+      </c>
+      <c r="N121" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="O121" s="1" t="str">
+        <f>LOOKUP(N121,Climate!A:A,Climate!B:B)</f>
+        <v>Data Pending</v>
+      </c>
+      <c r="P121" s="1" t="str">
+        <f>LOOKUP(N121,Climate!A:A,Climate!D:D)</f>
+        <v>-</v>
+      </c>
+      <c r="Q121" s="1" t="str">
+        <f>LOOKUP(N121,Climate!A:A,Climate!C:C)</f>
+        <v>-</v>
       </c>
     </row>
   </sheetData>
@@ -5919,6 +7941,493 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{567ACFC2-334E-D34F-85FB-0289015A229A}">
+  <dimension ref="A1:D33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>417</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>417</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>417</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>408</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>408</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>408</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>408</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D30" s="29" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>408</v>
+      </c>
+      <c r="D31" s="29" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C32" s="29" t="s">
+        <v>408</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="C33" s="29" t="s">
+        <v>401</v>
+      </c>
+      <c r="D33" s="29" t="s">
+        <v>401</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C32">
+    <sortCondition ref="A2:A32"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A76F5DF-B7AB-FD4F-8B65-5F9CF6278BAF}">
   <dimension ref="A1:H53"/>
   <sheetViews>
@@ -7133,7 +9642,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80AB13DC-0E22-5540-A84A-EF51CCCABDEE}">
   <dimension ref="A1:O16"/>
   <sheetViews>

</xml_diff>

<commit_message>
Overhaul dendrogram module to improve UX and accuracy
</commit_message>
<xml_diff>
--- a/io_in/city_list.xlsx
+++ b/io_in/city_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Coding/roadtrips/io_in/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FA3764-7EAC-BE45-BC13-A42C6D031F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE174D1-C979-1E44-A0C9-E11B798345BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13500" yWindow="500" windowWidth="30020" windowHeight="21900" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
+    <workbookView xWindow="17520" yWindow="500" windowWidth="13020" windowHeight="21900" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="9" r:id="rId1"/>
@@ -1517,10 +1517,10 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1838,8 +1838,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418BD67C-5132-6942-B406-D98F46E6A0BD}">
   <dimension ref="A1:Q121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2035,7 +2038,9 @@
       <c r="E4" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="F4" s="23"/>
+      <c r="F4" s="23">
+        <v>3.8</v>
+      </c>
       <c r="G4" s="5" t="s">
         <v>128</v>
       </c>
@@ -2086,7 +2091,9 @@
       <c r="E5" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="F5" s="23"/>
+      <c r="F5" s="23">
+        <v>4</v>
+      </c>
       <c r="G5" s="5" t="s">
         <v>125</v>
       </c>
@@ -2896,7 +2903,9 @@
       <c r="E21" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F21" s="23"/>
+      <c r="F21" s="23">
+        <v>2.1</v>
+      </c>
       <c r="G21" s="5" t="s">
         <v>125</v>
       </c>
@@ -2947,7 +2956,9 @@
       <c r="E22" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F22" s="23"/>
+      <c r="F22" s="23">
+        <v>4.5999999999999996</v>
+      </c>
       <c r="G22" s="1" t="s">
         <v>128</v>
       </c>
@@ -2995,7 +3006,9 @@
       <c r="E23" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="F23" s="23"/>
+      <c r="F23" s="23">
+        <v>99.9</v>
+      </c>
       <c r="G23" s="5" t="s">
         <v>125</v>
       </c>
@@ -3048,7 +3061,9 @@
       <c r="E24" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="F24" s="23"/>
+      <c r="F24" s="23">
+        <v>1.8</v>
+      </c>
       <c r="G24" s="5" t="s">
         <v>125</v>
       </c>
@@ -3418,7 +3433,10 @@
       <c r="E31" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="F31" s="23"/>
+      <c r="F31" s="23">
+        <f>5.2+5.3</f>
+        <v>10.5</v>
+      </c>
       <c r="G31" s="5" t="s">
         <v>125</v>
       </c>
@@ -3469,7 +3487,9 @@
       <c r="E32" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="F32" s="23"/>
+      <c r="F32" s="23">
+        <v>8.6</v>
+      </c>
       <c r="G32" s="5" t="s">
         <v>128</v>
       </c>
@@ -5357,19 +5377,19 @@
         <v>273</v>
       </c>
       <c r="N70" s="2" t="s">
-        <v>403</v>
+        <v>371</v>
       </c>
       <c r="O70" s="1" t="str">
         <f>LOOKUP(N70,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Continental</v>
       </c>
       <c r="P70" s="1" t="str">
         <f>LOOKUP(N70,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q70" s="1" t="str">
         <f>LOOKUP(N70,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Warm, Wet</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
@@ -5405,19 +5425,19 @@
         <v>345</v>
       </c>
       <c r="N71" s="2" t="s">
-        <v>403</v>
+        <v>367</v>
       </c>
       <c r="O71" s="1" t="str">
         <f>LOOKUP(N71,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Continental</v>
       </c>
       <c r="P71" s="1" t="str">
         <f>LOOKUP(N71,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q71" s="1" t="str">
         <f>LOOKUP(N71,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="72" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -5455,19 +5475,19 @@
         <v>321</v>
       </c>
       <c r="N72" s="2" t="s">
-        <v>403</v>
+        <v>361</v>
       </c>
       <c r="O72" s="1" t="str">
         <f>LOOKUP(N72,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Temperate</v>
       </c>
       <c r="P72" s="1" t="str">
         <f>LOOKUP(N72,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q72" s="1" t="str">
         <f>LOOKUP(N72,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
@@ -5503,19 +5523,19 @@
         <v>353</v>
       </c>
       <c r="N73" s="2" t="s">
-        <v>403</v>
+        <v>361</v>
       </c>
       <c r="O73" s="1" t="str">
         <f>LOOKUP(N73,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Temperate</v>
       </c>
       <c r="P73" s="1" t="str">
         <f>LOOKUP(N73,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q73" s="1" t="str">
         <f>LOOKUP(N73,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="74" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -5553,19 +5573,19 @@
         <v>334</v>
       </c>
       <c r="N74" s="2" t="s">
-        <v>403</v>
+        <v>362</v>
       </c>
       <c r="O74" s="1" t="str">
         <f>LOOKUP(N74,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Arid Cold</v>
       </c>
       <c r="P74" s="1" t="str">
         <f>LOOKUP(N74,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Dry</v>
       </c>
       <c r="Q74" s="1" t="str">
         <f>LOOKUP(N74,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Dry</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
@@ -5601,19 +5621,19 @@
         <v>334</v>
       </c>
       <c r="N75" s="2" t="s">
-        <v>403</v>
+        <v>371</v>
       </c>
       <c r="O75" s="1" t="str">
         <f>LOOKUP(N75,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Continental</v>
       </c>
       <c r="P75" s="1" t="str">
         <f>LOOKUP(N75,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q75" s="1" t="str">
         <f>LOOKUP(N75,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Warm, Wet</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
@@ -5649,19 +5669,19 @@
         <v>334</v>
       </c>
       <c r="N76" s="2" t="s">
-        <v>403</v>
+        <v>371</v>
       </c>
       <c r="O76" s="1" t="str">
         <f>LOOKUP(N76,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Continental</v>
       </c>
       <c r="P76" s="1" t="str">
         <f>LOOKUP(N76,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q76" s="1" t="str">
         <f>LOOKUP(N76,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Warm, Wet</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
@@ -5697,19 +5717,19 @@
         <v>322</v>
       </c>
       <c r="N77" s="2" t="s">
-        <v>403</v>
+        <v>362</v>
       </c>
       <c r="O77" s="1" t="str">
         <f>LOOKUP(N77,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Arid Cold</v>
       </c>
       <c r="P77" s="1" t="str">
         <f>LOOKUP(N77,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Dry</v>
       </c>
       <c r="Q77" s="1" t="str">
         <f>LOOKUP(N77,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Dry</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
@@ -5748,19 +5768,19 @@
         <v>291</v>
       </c>
       <c r="N78" s="2" t="s">
-        <v>403</v>
+        <v>363</v>
       </c>
       <c r="O78" s="1" t="str">
         <f>LOOKUP(N78,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Desert Hot</v>
       </c>
       <c r="P78" s="1" t="str">
         <f>LOOKUP(N78,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Dry</v>
       </c>
       <c r="Q78" s="1" t="str">
         <f>LOOKUP(N78,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Dry</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
@@ -5796,19 +5816,19 @@
         <v>274</v>
       </c>
       <c r="N79" s="2" t="s">
-        <v>403</v>
+        <v>367</v>
       </c>
       <c r="O79" s="1" t="str">
         <f>LOOKUP(N79,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Continental</v>
       </c>
       <c r="P79" s="1" t="str">
         <f>LOOKUP(N79,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q79" s="1" t="str">
         <f>LOOKUP(N79,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
@@ -5847,19 +5867,19 @@
         <v>315</v>
       </c>
       <c r="N80" s="2" t="s">
-        <v>403</v>
+        <v>371</v>
       </c>
       <c r="O80" s="1" t="str">
         <f>LOOKUP(N80,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Continental</v>
       </c>
       <c r="P80" s="1" t="str">
         <f>LOOKUP(N80,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q80" s="1" t="str">
         <f>LOOKUP(N80,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Warm, Wet</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
@@ -5904,19 +5924,19 @@
         <v>292</v>
       </c>
       <c r="N81" s="2" t="s">
-        <v>403</v>
+        <v>361</v>
       </c>
       <c r="O81" s="1" t="str">
         <f>LOOKUP(N81,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Temperate</v>
       </c>
       <c r="P81" s="1" t="str">
         <f>LOOKUP(N81,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q81" s="1" t="str">
         <f>LOOKUP(N81,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
@@ -5955,19 +5975,19 @@
         <v>317</v>
       </c>
       <c r="N82" s="2" t="s">
-        <v>403</v>
+        <v>367</v>
       </c>
       <c r="O82" s="1" t="str">
         <f>LOOKUP(N82,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Continental</v>
       </c>
       <c r="P82" s="1" t="str">
         <f>LOOKUP(N82,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q82" s="1" t="str">
         <f>LOOKUP(N82,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
@@ -6006,19 +6026,19 @@
         <v>347</v>
       </c>
       <c r="N83" s="2" t="s">
-        <v>403</v>
+        <v>367</v>
       </c>
       <c r="O83" s="1" t="str">
         <f>LOOKUP(N83,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Continental</v>
       </c>
       <c r="P83" s="1" t="str">
         <f>LOOKUP(N83,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q83" s="1" t="str">
         <f>LOOKUP(N83,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
@@ -6057,19 +6077,19 @@
         <v>309</v>
       </c>
       <c r="N84" s="2" t="s">
-        <v>403</v>
+        <v>367</v>
       </c>
       <c r="O84" s="1" t="str">
         <f>LOOKUP(N84,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Continental</v>
       </c>
       <c r="P84" s="1" t="str">
         <f>LOOKUP(N84,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q84" s="1" t="str">
         <f>LOOKUP(N84,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
@@ -6108,19 +6128,19 @@
         <v>275</v>
       </c>
       <c r="N85" s="2" t="s">
-        <v>403</v>
+        <v>367</v>
       </c>
       <c r="O85" s="1" t="str">
         <f>LOOKUP(N85,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Continental</v>
       </c>
       <c r="P85" s="1" t="str">
         <f>LOOKUP(N85,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q85" s="1" t="str">
         <f>LOOKUP(N85,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
@@ -6159,19 +6179,19 @@
         <v>276</v>
       </c>
       <c r="N86" s="2" t="s">
-        <v>403</v>
+        <v>361</v>
       </c>
       <c r="O86" s="1" t="str">
         <f>LOOKUP(N86,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Temperate</v>
       </c>
       <c r="P86" s="1" t="str">
         <f>LOOKUP(N86,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q86" s="1" t="str">
         <f>LOOKUP(N86,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
@@ -6210,19 +6230,19 @@
         <v>318</v>
       </c>
       <c r="N87" s="2" t="s">
-        <v>403</v>
+        <v>361</v>
       </c>
       <c r="O87" s="1" t="str">
         <f>LOOKUP(N87,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Temperate</v>
       </c>
       <c r="P87" s="1" t="str">
         <f>LOOKUP(N87,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q87" s="1" t="str">
         <f>LOOKUP(N87,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
@@ -6261,19 +6281,19 @@
         <v>306</v>
       </c>
       <c r="N88" s="2" t="s">
-        <v>403</v>
+        <v>364</v>
       </c>
       <c r="O88" s="1" t="str">
         <f>LOOKUP(N88,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Temperate</v>
       </c>
       <c r="P88" s="1" t="str">
         <f>LOOKUP(N88,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q88" s="1" t="str">
         <f>LOOKUP(N88,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v xml:space="preserve">Dry, Warm </v>
       </c>
     </row>
     <row r="89" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -6311,19 +6331,19 @@
         <v>277</v>
       </c>
       <c r="N89" s="2" t="s">
-        <v>403</v>
+        <v>364</v>
       </c>
       <c r="O89" s="1" t="str">
         <f>LOOKUP(N89,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Temperate</v>
       </c>
       <c r="P89" s="1" t="str">
         <f>LOOKUP(N89,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q89" s="1" t="str">
         <f>LOOKUP(N89,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v xml:space="preserve">Dry, Warm </v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.2">
@@ -6359,19 +6379,19 @@
         <v>350</v>
       </c>
       <c r="N90" s="2" t="s">
-        <v>403</v>
+        <v>361</v>
       </c>
       <c r="O90" s="1" t="str">
         <f>LOOKUP(N90,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Temperate</v>
       </c>
       <c r="P90" s="1" t="str">
         <f>LOOKUP(N90,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q90" s="1" t="str">
         <f>LOOKUP(N90,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.2">
@@ -6413,19 +6433,19 @@
         <v>293</v>
       </c>
       <c r="N91" s="2" t="s">
-        <v>403</v>
+        <v>361</v>
       </c>
       <c r="O91" s="1" t="str">
         <f>LOOKUP(N91,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Temperate</v>
       </c>
       <c r="P91" s="1" t="str">
         <f>LOOKUP(N91,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q91" s="1" t="str">
         <f>LOOKUP(N91,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.2">
@@ -6464,19 +6484,19 @@
         <v>307</v>
       </c>
       <c r="N92" s="2" t="s">
-        <v>403</v>
+        <v>367</v>
       </c>
       <c r="O92" s="1" t="str">
         <f>LOOKUP(N92,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Continental</v>
       </c>
       <c r="P92" s="1" t="str">
         <f>LOOKUP(N92,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q92" s="1" t="str">
         <f>LOOKUP(N92,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.2">
@@ -6517,19 +6537,19 @@
         <v>340</v>
       </c>
       <c r="N93" s="2" t="s">
-        <v>403</v>
+        <v>369</v>
       </c>
       <c r="O93" s="1" t="str">
         <f>LOOKUP(N93,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Tropical Monsoon</v>
       </c>
       <c r="P93" s="1" t="str">
         <f>LOOKUP(N93,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q93" s="1" t="str">
         <f>LOOKUP(N93,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
@@ -6568,19 +6588,19 @@
         <v>278</v>
       </c>
       <c r="N94" s="2" t="s">
-        <v>403</v>
+        <v>367</v>
       </c>
       <c r="O94" s="1" t="str">
         <f>LOOKUP(N94,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Continental</v>
       </c>
       <c r="P94" s="1" t="str">
         <f>LOOKUP(N94,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q94" s="1" t="str">
         <f>LOOKUP(N94,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
@@ -6616,19 +6636,19 @@
         <v>335</v>
       </c>
       <c r="N95" s="2" t="s">
-        <v>403</v>
+        <v>361</v>
       </c>
       <c r="O95" s="1" t="str">
         <f>LOOKUP(N95,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Temperate</v>
       </c>
       <c r="P95" s="1" t="str">
         <f>LOOKUP(N95,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q95" s="1" t="str">
         <f>LOOKUP(N95,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.2">
@@ -6664,19 +6684,19 @@
         <v>279</v>
       </c>
       <c r="N96" s="2" t="s">
-        <v>403</v>
+        <v>361</v>
       </c>
       <c r="O96" s="1" t="str">
         <f>LOOKUP(N96,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Temperate</v>
       </c>
       <c r="P96" s="1" t="str">
         <f>LOOKUP(N96,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q96" s="1" t="str">
         <f>LOOKUP(N96,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.2">
@@ -6712,19 +6732,19 @@
         <v>346</v>
       </c>
       <c r="N97" s="2" t="s">
-        <v>403</v>
+        <v>367</v>
       </c>
       <c r="O97" s="1" t="str">
         <f>LOOKUP(N97,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Continental</v>
       </c>
       <c r="P97" s="1" t="str">
         <f>LOOKUP(N97,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q97" s="1" t="str">
         <f>LOOKUP(N97,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
@@ -6760,19 +6780,19 @@
         <v>324</v>
       </c>
       <c r="N98" s="2" t="s">
-        <v>403</v>
+        <v>367</v>
       </c>
       <c r="O98" s="1" t="str">
         <f>LOOKUP(N98,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Continental</v>
       </c>
       <c r="P98" s="1" t="str">
         <f>LOOKUP(N98,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q98" s="1" t="str">
         <f>LOOKUP(N98,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.2">
@@ -6811,19 +6831,19 @@
         <v>323</v>
       </c>
       <c r="N99" s="2" t="s">
-        <v>403</v>
+        <v>361</v>
       </c>
       <c r="O99" s="1" t="str">
         <f>LOOKUP(N99,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Temperate</v>
       </c>
       <c r="P99" s="1" t="str">
         <f>LOOKUP(N99,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q99" s="1" t="str">
         <f>LOOKUP(N99,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.2">
@@ -6862,19 +6882,19 @@
         <v>314</v>
       </c>
       <c r="N100" s="2" t="s">
-        <v>403</v>
+        <v>361</v>
       </c>
       <c r="O100" s="1" t="str">
         <f>LOOKUP(N100,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Temperate</v>
       </c>
       <c r="P100" s="1" t="str">
         <f>LOOKUP(N100,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q100" s="1" t="str">
         <f>LOOKUP(N100,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.2">
@@ -6913,19 +6933,19 @@
         <v>280</v>
       </c>
       <c r="N101" s="2" t="s">
-        <v>403</v>
+        <v>361</v>
       </c>
       <c r="O101" s="1" t="str">
         <f>LOOKUP(N101,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Temperate</v>
       </c>
       <c r="P101" s="1" t="str">
         <f>LOOKUP(N101,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q101" s="1" t="str">
         <f>LOOKUP(N101,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.2">
@@ -6964,19 +6984,19 @@
         <v>305</v>
       </c>
       <c r="N102" s="2" t="s">
-        <v>403</v>
+        <v>361</v>
       </c>
       <c r="O102" s="1" t="str">
         <f>LOOKUP(N102,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Temperate</v>
       </c>
       <c r="P102" s="1" t="str">
         <f>LOOKUP(N102,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q102" s="1" t="str">
         <f>LOOKUP(N102,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.2">
@@ -7015,19 +7035,19 @@
         <v>295</v>
       </c>
       <c r="N103" s="2" t="s">
-        <v>403</v>
+        <v>361</v>
       </c>
       <c r="O103" s="1" t="str">
         <f>LOOKUP(N103,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Temperate</v>
       </c>
       <c r="P103" s="1" t="str">
         <f>LOOKUP(N103,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q103" s="1" t="str">
         <f>LOOKUP(N103,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
@@ -7066,19 +7086,19 @@
         <v>296</v>
       </c>
       <c r="N104" s="2" t="s">
-        <v>403</v>
+        <v>361</v>
       </c>
       <c r="O104" s="1" t="str">
         <f>LOOKUP(N104,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Temperate</v>
       </c>
       <c r="P104" s="1" t="str">
         <f>LOOKUP(N104,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q104" s="1" t="str">
         <f>LOOKUP(N104,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
@@ -7120,19 +7140,19 @@
         <v>305</v>
       </c>
       <c r="N105" s="2" t="s">
-        <v>403</v>
+        <v>361</v>
       </c>
       <c r="O105" s="1" t="str">
         <f>LOOKUP(N105,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Temperate</v>
       </c>
       <c r="P105" s="1" t="str">
         <f>LOOKUP(N105,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q105" s="1" t="str">
         <f>LOOKUP(N105,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.2">
@@ -7168,19 +7188,19 @@
         <v>281</v>
       </c>
       <c r="N106" s="2" t="s">
-        <v>403</v>
+        <v>366</v>
       </c>
       <c r="O106" s="1" t="str">
         <f>LOOKUP(N106,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Temperate</v>
       </c>
       <c r="P106" s="1" t="str">
         <f>LOOKUP(N106,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q106" s="1" t="str">
         <f>LOOKUP(N106,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v xml:space="preserve">Dry, Hot </v>
       </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.2">
@@ -7219,19 +7239,19 @@
         <v>281</v>
       </c>
       <c r="N107" s="2" t="s">
-        <v>403</v>
+        <v>382</v>
       </c>
       <c r="O107" s="1" t="str">
         <f>LOOKUP(N107,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Continental</v>
       </c>
       <c r="P107" s="1" t="str">
         <f>LOOKUP(N107,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q107" s="1" t="str">
         <f>LOOKUP(N107,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v xml:space="preserve">Dry, Hot </v>
       </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.2">
@@ -7270,19 +7290,19 @@
         <v>352</v>
       </c>
       <c r="N108" s="2" t="s">
-        <v>403</v>
+        <v>361</v>
       </c>
       <c r="O108" s="1" t="str">
         <f>LOOKUP(N108,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Temperate</v>
       </c>
       <c r="P108" s="1" t="str">
         <f>LOOKUP(N108,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q108" s="1" t="str">
         <f>LOOKUP(N108,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.2">
@@ -7321,19 +7341,19 @@
         <v>310</v>
       </c>
       <c r="N109" s="2" t="s">
-        <v>403</v>
+        <v>361</v>
       </c>
       <c r="O109" s="1" t="str">
         <f>LOOKUP(N109,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Temperate</v>
       </c>
       <c r="P109" s="1" t="str">
         <f>LOOKUP(N109,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q109" s="1" t="str">
         <f>LOOKUP(N109,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.2">
@@ -7375,19 +7395,19 @@
         <v>282</v>
       </c>
       <c r="N110" s="2" t="s">
-        <v>403</v>
+        <v>361</v>
       </c>
       <c r="O110" s="1" t="str">
         <f>LOOKUP(N110,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Temperate</v>
       </c>
       <c r="P110" s="1" t="str">
         <f>LOOKUP(N110,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q110" s="1" t="str">
         <f>LOOKUP(N110,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.2">
@@ -7423,19 +7443,19 @@
         <v>325</v>
       </c>
       <c r="N111" s="2" t="s">
-        <v>403</v>
+        <v>367</v>
       </c>
       <c r="O111" s="1" t="str">
         <f>LOOKUP(N111,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Continental</v>
       </c>
       <c r="P111" s="1" t="str">
         <f>LOOKUP(N111,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q111" s="1" t="str">
         <f>LOOKUP(N111,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.2">
@@ -7471,19 +7491,19 @@
         <v>325</v>
       </c>
       <c r="N112" s="2" t="s">
-        <v>403</v>
+        <v>371</v>
       </c>
       <c r="O112" s="1" t="str">
         <f>LOOKUP(N112,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Continental</v>
       </c>
       <c r="P112" s="1" t="str">
         <f>LOOKUP(N112,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q112" s="1" t="str">
         <f>LOOKUP(N112,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Warm, Wet</v>
       </c>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.2">
@@ -7519,19 +7539,19 @@
         <v>283</v>
       </c>
       <c r="N113" s="2" t="s">
-        <v>403</v>
+        <v>364</v>
       </c>
       <c r="O113" s="1" t="str">
         <f>LOOKUP(N113,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Temperate</v>
       </c>
       <c r="P113" s="1" t="str">
         <f>LOOKUP(N113,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q113" s="1" t="str">
         <f>LOOKUP(N113,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v xml:space="preserve">Dry, Warm </v>
       </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.2">
@@ -7568,19 +7588,19 @@
         <v>299</v>
       </c>
       <c r="N114" s="2" t="s">
-        <v>403</v>
+        <v>364</v>
       </c>
       <c r="O114" s="1" t="str">
         <f>LOOKUP(N114,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Temperate</v>
       </c>
       <c r="P114" s="1" t="str">
         <f>LOOKUP(N114,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q114" s="1" t="str">
         <f>LOOKUP(N114,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v xml:space="preserve">Dry, Warm </v>
       </c>
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.2">
@@ -7619,19 +7639,19 @@
         <v>299</v>
       </c>
       <c r="N115" s="2" t="s">
-        <v>403</v>
+        <v>364</v>
       </c>
       <c r="O115" s="1" t="str">
         <f>LOOKUP(N115,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Temperate</v>
       </c>
       <c r="P115" s="1" t="str">
         <f>LOOKUP(N115,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q115" s="1" t="str">
         <f>LOOKUP(N115,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v xml:space="preserve">Dry, Warm </v>
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.2">
@@ -7667,19 +7687,19 @@
         <v>284</v>
       </c>
       <c r="N116" s="2" t="s">
-        <v>403</v>
+        <v>367</v>
       </c>
       <c r="O116" s="1" t="str">
         <f>LOOKUP(N116,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Continental</v>
       </c>
       <c r="P116" s="1" t="str">
         <f>LOOKUP(N116,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q116" s="1" t="str">
         <f>LOOKUP(N116,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.2">
@@ -7718,19 +7738,19 @@
         <v>312</v>
       </c>
       <c r="N117" s="2" t="s">
-        <v>403</v>
+        <v>367</v>
       </c>
       <c r="O117" s="1" t="str">
         <f>LOOKUP(N117,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Continental</v>
       </c>
       <c r="P117" s="1" t="str">
         <f>LOOKUP(N117,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q117" s="1" t="str">
         <f>LOOKUP(N117,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="118" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -7768,19 +7788,19 @@
         <v>285</v>
       </c>
       <c r="N118" s="2" t="s">
-        <v>403</v>
+        <v>361</v>
       </c>
       <c r="O118" s="1" t="str">
         <f>LOOKUP(N118,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Temperate</v>
       </c>
       <c r="P118" s="1" t="str">
         <f>LOOKUP(N118,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q118" s="1" t="str">
         <f>LOOKUP(N118,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="119" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -7818,19 +7838,19 @@
         <v>336</v>
       </c>
       <c r="N119" s="2" t="s">
-        <v>403</v>
+        <v>361</v>
       </c>
       <c r="O119" s="1" t="str">
         <f>LOOKUP(N119,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Temperate</v>
       </c>
       <c r="P119" s="1" t="str">
         <f>LOOKUP(N119,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Wet</v>
       </c>
       <c r="Q119" s="1" t="str">
         <f>LOOKUP(N119,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Hot, Wet</v>
       </c>
     </row>
     <row r="120" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -7868,19 +7888,19 @@
         <v>326</v>
       </c>
       <c r="N120" s="2" t="s">
-        <v>403</v>
+        <v>362</v>
       </c>
       <c r="O120" s="1" t="str">
         <f>LOOKUP(N120,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Arid Cold</v>
       </c>
       <c r="P120" s="1" t="str">
         <f>LOOKUP(N120,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Dry</v>
       </c>
       <c r="Q120" s="1" t="str">
         <f>LOOKUP(N120,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Dry</v>
       </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.2">
@@ -7916,19 +7936,19 @@
         <v>286</v>
       </c>
       <c r="N121" s="2" t="s">
-        <v>403</v>
+        <v>362</v>
       </c>
       <c r="O121" s="1" t="str">
         <f>LOOKUP(N121,Climate!A:A,Climate!B:B)</f>
-        <v>Data Pending</v>
+        <v>Arid Cold</v>
       </c>
       <c r="P121" s="1" t="str">
         <f>LOOKUP(N121,Climate!A:A,Climate!D:D)</f>
-        <v>-</v>
+        <v>Dry</v>
       </c>
       <c r="Q121" s="1" t="str">
         <f>LOOKUP(N121,Climate!A:A,Climate!C:C)</f>
-        <v>-</v>
+        <v>Dry</v>
       </c>
     </row>
   </sheetData>
@@ -7978,10 +7998,10 @@
       <c r="B2" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="28" t="s">
         <v>417</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="28" t="s">
         <v>417</v>
       </c>
     </row>
@@ -7992,10 +8012,10 @@
       <c r="B3" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="28" t="s">
         <v>417</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="28" t="s">
         <v>417</v>
       </c>
     </row>
@@ -8009,7 +8029,7 @@
       <c r="C4" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="28" t="s">
         <v>417</v>
       </c>
     </row>
@@ -8020,7 +8040,7 @@
       <c r="B5" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="28" t="s">
         <v>417</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -8034,10 +8054,10 @@
       <c r="B6" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="28" t="s">
         <v>408</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="28" t="s">
         <v>408</v>
       </c>
     </row>
@@ -8048,10 +8068,10 @@
       <c r="B7" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="28" t="s">
         <v>408</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="28" t="s">
         <v>408</v>
       </c>
     </row>
@@ -8062,10 +8082,10 @@
       <c r="B8" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="28" t="s">
         <v>408</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="28" t="s">
         <v>408</v>
       </c>
     </row>
@@ -8076,10 +8096,10 @@
       <c r="B9" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="28" t="s">
         <v>408</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="28" t="s">
         <v>408</v>
       </c>
     </row>
@@ -8093,7 +8113,7 @@
       <c r="C10" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="28" t="s">
         <v>417</v>
       </c>
     </row>
@@ -8107,7 +8127,7 @@
       <c r="C11" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="28" t="s">
         <v>417</v>
       </c>
     </row>
@@ -8121,7 +8141,7 @@
       <c r="C12" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="28" t="s">
         <v>417</v>
       </c>
     </row>
@@ -8135,7 +8155,7 @@
       <c r="C13" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="28" t="s">
         <v>417</v>
       </c>
     </row>
@@ -8149,7 +8169,7 @@
       <c r="C14" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="28" t="s">
         <v>417</v>
       </c>
     </row>
@@ -8163,7 +8183,7 @@
       <c r="C15" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="28" t="s">
         <v>417</v>
       </c>
     </row>
@@ -8177,7 +8197,7 @@
       <c r="C16" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="D16" s="28" t="s">
         <v>408</v>
       </c>
     </row>
@@ -8191,7 +8211,7 @@
       <c r="C17" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="28" t="s">
         <v>408</v>
       </c>
     </row>
@@ -8205,7 +8225,7 @@
       <c r="C18" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D18" s="29" t="s">
+      <c r="D18" s="28" t="s">
         <v>408</v>
       </c>
     </row>
@@ -8219,7 +8239,7 @@
       <c r="C19" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="28" t="s">
         <v>417</v>
       </c>
     </row>
@@ -8233,7 +8253,7 @@
       <c r="C20" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="D20" s="28" t="s">
         <v>417</v>
       </c>
     </row>
@@ -8247,7 +8267,7 @@
       <c r="C21" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="D21" s="29" t="s">
+      <c r="D21" s="28" t="s">
         <v>417</v>
       </c>
     </row>
@@ -8261,7 +8281,7 @@
       <c r="C22" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="D22" s="29" t="s">
+      <c r="D22" s="28" t="s">
         <v>417</v>
       </c>
     </row>
@@ -8275,7 +8295,7 @@
       <c r="C23" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="D23" s="29" t="s">
+      <c r="D23" s="28" t="s">
         <v>417</v>
       </c>
     </row>
@@ -8289,7 +8309,7 @@
       <c r="C24" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="D24" s="29" t="s">
+      <c r="D24" s="28" t="s">
         <v>417</v>
       </c>
     </row>
@@ -8303,7 +8323,7 @@
       <c r="C25" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="D25" s="29" t="s">
+      <c r="D25" s="28" t="s">
         <v>417</v>
       </c>
     </row>
@@ -8317,7 +8337,7 @@
       <c r="C26" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="D26" s="29" t="s">
+      <c r="D26" s="28" t="s">
         <v>417</v>
       </c>
     </row>
@@ -8331,7 +8351,7 @@
       <c r="C27" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="D27" s="29" t="s">
+      <c r="D27" s="28" t="s">
         <v>408</v>
       </c>
     </row>
@@ -8345,7 +8365,7 @@
       <c r="C28" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="D28" s="29" t="s">
+      <c r="D28" s="28" t="s">
         <v>408</v>
       </c>
     </row>
@@ -8359,7 +8379,7 @@
       <c r="C29" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="D29" s="29" t="s">
+      <c r="D29" s="28" t="s">
         <v>408</v>
       </c>
     </row>
@@ -8373,7 +8393,7 @@
       <c r="C30" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="D30" s="29" t="s">
+      <c r="D30" s="28" t="s">
         <v>408</v>
       </c>
     </row>
@@ -8384,10 +8404,10 @@
       <c r="B31" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="C31" s="29" t="s">
+      <c r="C31" s="28" t="s">
         <v>408</v>
       </c>
-      <c r="D31" s="29" t="s">
+      <c r="D31" s="28" t="s">
         <v>408</v>
       </c>
     </row>
@@ -8398,10 +8418,10 @@
       <c r="B32" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="C32" s="29" t="s">
+      <c r="C32" s="28" t="s">
         <v>408</v>
       </c>
-      <c r="D32" s="29" t="s">
+      <c r="D32" s="28" t="s">
         <v>408</v>
       </c>
     </row>
@@ -8412,10 +8432,10 @@
       <c r="B33" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="C33" s="29" t="s">
+      <c r="C33" s="28" t="s">
         <v>401</v>
       </c>
-      <c r="D33" s="29" t="s">
+      <c r="D33" s="28" t="s">
         <v>401</v>
       </c>
     </row>
@@ -9662,12 +9682,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
@@ -9732,12 +9752,12 @@
       <c r="L6" s="20"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="29" t="s">
         <v>219</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
@@ -9750,12 +9770,12 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="29" t="s">
         <v>241</v>
       </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">

</xml_diff>

<commit_message>
Add module doc strings and improve README
</commit_message>
<xml_diff>
--- a/io_in/city_list.xlsx
+++ b/io_in/city_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Coding/roadtrips/io_in/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE174D1-C979-1E44-A0C9-E11B798345BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D5B179-02EC-0F47-81BE-74E224F758A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17520" yWindow="500" windowWidth="13020" windowHeight="21900" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
+    <workbookView xWindow="22480" yWindow="500" windowWidth="13020" windowHeight="21900" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="9" r:id="rId1"/>
@@ -1839,10 +1839,10 @@
   <dimension ref="A1:Q121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5508,7 +5508,9 @@
       <c r="E73" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F73" s="23"/>
+      <c r="F73" s="23">
+        <v>3.6</v>
+      </c>
       <c r="G73" s="5" t="s">
         <v>125</v>
       </c>
@@ -5556,7 +5558,9 @@
       <c r="E74" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="F74" s="23"/>
+      <c r="F74" s="23">
+        <v>8.6</v>
+      </c>
       <c r="G74" s="5" t="s">
         <v>128</v>
       </c>
@@ -5606,7 +5610,9 @@
       <c r="E75" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="F75" s="23"/>
+      <c r="F75" s="23">
+        <v>10.3</v>
+      </c>
       <c r="G75" s="5" t="s">
         <v>125</v>
       </c>
@@ -5654,7 +5660,9 @@
       <c r="E76" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="F76" s="23"/>
+      <c r="F76" s="23">
+        <v>3.5</v>
+      </c>
       <c r="G76" s="1" t="s">
         <v>240</v>
       </c>

</xml_diff>

<commit_message>
Squash line overrun; update travels
</commit_message>
<xml_diff>
--- a/io_in/city_list.xlsx
+++ b/io_in/city_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Coding/roadtrips/io_in/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3155B17A-4E60-EF4C-ABE5-45B3B7774DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB949BCD-4986-824E-81EA-7E894E010841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22480" yWindow="500" windowWidth="13020" windowHeight="21900" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
   </bookViews>
@@ -1839,10 +1839,10 @@
   <dimension ref="A1:Q121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C89" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H112" sqref="H112"/>
+      <selection pane="bottomRight" activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3590,7 +3590,9 @@
       <c r="E34" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="F34" s="25"/>
+      <c r="F34" s="25">
+        <v>1.8</v>
+      </c>
       <c r="G34" s="5" t="s">
         <v>128</v>
       </c>
@@ -3638,7 +3640,9 @@
       <c r="E35" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F35" s="23"/>
+      <c r="F35" s="23">
+        <v>8.1</v>
+      </c>
       <c r="G35" s="5" t="s">
         <v>125</v>
       </c>
@@ -3782,7 +3786,9 @@
       <c r="E38" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="F38" s="23"/>
+      <c r="F38" s="23">
+        <v>22.7</v>
+      </c>
       <c r="G38" s="5" t="s">
         <v>128</v>
       </c>
@@ -3833,7 +3839,9 @@
       <c r="E39" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F39" s="23"/>
+      <c r="F39" s="23">
+        <v>6.6</v>
+      </c>
       <c r="G39" s="5" t="s">
         <v>125</v>
       </c>
@@ -3881,7 +3889,9 @@
       <c r="E40" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F40" s="23"/>
+      <c r="F40" s="23">
+        <v>4.9000000000000004</v>
+      </c>
       <c r="G40" s="5" t="s">
         <v>125</v>
       </c>
@@ -3933,7 +3943,9 @@
       <c r="E41" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F41" s="23"/>
+      <c r="F41" s="23">
+        <v>2.6</v>
+      </c>
       <c r="G41" s="5" t="s">
         <v>125</v>
       </c>
@@ -4029,7 +4041,9 @@
       <c r="E43" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F43" s="23"/>
+      <c r="F43" s="23">
+        <v>2.2999999999999998</v>
+      </c>
       <c r="G43" s="5" t="s">
         <v>125</v>
       </c>
@@ -4077,7 +4091,9 @@
       <c r="E44" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F44" s="23"/>
+      <c r="F44" s="23">
+        <v>7.6</v>
+      </c>
       <c r="G44" s="5" t="s">
         <v>128</v>
       </c>
@@ -4377,7 +4393,9 @@
       <c r="E50" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F50" s="23"/>
+      <c r="F50" s="23">
+        <v>3.2</v>
+      </c>
       <c r="G50" s="5" t="s">
         <v>125</v>
       </c>
@@ -4425,7 +4443,9 @@
       <c r="E51" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F51" s="23"/>
+      <c r="F51" s="23">
+        <v>5.2</v>
+      </c>
       <c r="G51" s="5" t="s">
         <v>128</v>
       </c>
@@ -7442,7 +7462,9 @@
       <c r="E111" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F111" s="23"/>
+      <c r="F111" s="23">
+        <v>4.8</v>
+      </c>
       <c r="G111" s="5" t="s">
         <v>128</v>
       </c>
@@ -7490,7 +7512,9 @@
       <c r="E112" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F112" s="23"/>
+      <c r="F112" s="23">
+        <v>2.7</v>
+      </c>
       <c r="G112" s="5" t="s">
         <v>125</v>
       </c>

</xml_diff>

<commit_message>
Finish waffle plots and tie into slider
</commit_message>
<xml_diff>
--- a/io_in/city_list.xlsx
+++ b/io_in/city_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Coding/roadtrips/io_in/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AA7247-2B17-4046-94F2-1285E3A0439B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A82317-D58A-614C-A7DF-BD3B32D1732A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="500" windowWidth="26920" windowHeight="21900" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
+    <workbookView xWindow="3060" yWindow="500" windowWidth="26920" windowHeight="21900" activeTab="3" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="9" r:id="rId1"/>
@@ -1952,7 +1952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418BD67C-5132-6942-B406-D98F46E6A0BD}">
   <dimension ref="A1:R121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -9238,8 +9238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1D4776-82C5-A549-993A-3BE59A636F7D}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9306,52 +9306,52 @@
         <v>80</v>
       </c>
       <c r="C2" s="3" t="str">
-        <f>"hsva("&amp;C$1&amp;",50,"&amp;$B2&amp;",100)"</f>
-        <v>hsva(0,50,80,100)</v>
+        <f>"hsva("&amp;C$1&amp;",40,"&amp;$B2&amp;",100)"</f>
+        <v>hsva(0,40,80,100)</v>
       </c>
       <c r="D2" s="3" t="str">
-        <f t="shared" ref="D2:N2" si="0">"hsva("&amp;D$1&amp;",50,"&amp;$B2&amp;",100)"</f>
-        <v>hsva(30,50,80,100)</v>
+        <f>"hsva("&amp;D$1&amp;",40,"&amp;$B2&amp;",100)"</f>
+        <v>hsva(30,40,80,100)</v>
       </c>
       <c r="E2" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>hsva(60,50,80,100)</v>
+        <f t="shared" ref="E2:N2" si="0">"hsva("&amp;E$1&amp;",40,"&amp;$B2&amp;",100)"</f>
+        <v>hsva(60,40,80,100)</v>
       </c>
       <c r="F2" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>hsva(90,50,80,100)</v>
+        <v>hsva(90,40,80,100)</v>
       </c>
       <c r="G2" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>hsva(120,50,80,100)</v>
+        <v>hsva(120,40,80,100)</v>
       </c>
       <c r="H2" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>hsva(150,50,80,100)</v>
+        <v>hsva(150,40,80,100)</v>
       </c>
       <c r="I2" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>hsva(180,50,80,100)</v>
+        <v>hsva(180,40,80,100)</v>
       </c>
       <c r="J2" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>hsva(210,50,80,100)</v>
+        <v>hsva(210,40,80,100)</v>
       </c>
       <c r="K2" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>hsva(240,50,80,100)</v>
+        <v>hsva(240,40,80,100)</v>
       </c>
       <c r="L2" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>hsva(270,50,80,100)</v>
+        <v>hsva(270,40,80,100)</v>
       </c>
       <c r="M2" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>hsva(300,50,80,100)</v>
+        <v>hsva(300,40,80,100)</v>
       </c>
       <c r="N2" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>hsva(330,50,80,100)</v>
+        <v>hsva(330,40,80,100)</v>
       </c>
       <c r="O2" s="3" t="str">
         <f>"hsv(0,0,"&amp;$B2&amp;")"</f>
@@ -9366,52 +9366,52 @@
         <v>50</v>
       </c>
       <c r="C3" s="3" t="str">
-        <f t="shared" ref="C3:N6" si="1">"hsva("&amp;C$1&amp;",50,"&amp;$B3&amp;",100)"</f>
-        <v>hsva(0,50,50,100)</v>
+        <f t="shared" ref="C3:N6" si="1">"hsva("&amp;C$1&amp;",40,"&amp;$B3&amp;",100)"</f>
+        <v>hsva(0,40,50,100)</v>
       </c>
       <c r="D3" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(30,50,50,100)</v>
+        <v>hsva(30,40,50,100)</v>
       </c>
       <c r="E3" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(60,50,50,100)</v>
+        <v>hsva(60,40,50,100)</v>
       </c>
       <c r="F3" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(90,50,50,100)</v>
+        <v>hsva(90,40,50,100)</v>
       </c>
       <c r="G3" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(120,50,50,100)</v>
+        <v>hsva(120,40,50,100)</v>
       </c>
       <c r="H3" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(150,50,50,100)</v>
+        <v>hsva(150,40,50,100)</v>
       </c>
       <c r="I3" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(180,50,50,100)</v>
+        <v>hsva(180,40,50,100)</v>
       </c>
       <c r="J3" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(210,50,50,100)</v>
+        <v>hsva(210,40,50,100)</v>
       </c>
       <c r="K3" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(240,50,50,100)</v>
+        <v>hsva(240,40,50,100)</v>
       </c>
       <c r="L3" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(270,50,50,100)</v>
+        <v>hsva(270,40,50,100)</v>
       </c>
       <c r="M3" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(300,50,50,100)</v>
+        <v>hsva(300,40,50,100)</v>
       </c>
       <c r="N3" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(330,50,50,100)</v>
+        <v>hsva(330,40,50,100)</v>
       </c>
       <c r="O3" s="3" t="str">
         <f t="shared" ref="O3:O6" si="2">"hsv(0,0,"&amp;$B3&amp;")"</f>
@@ -9427,51 +9427,51 @@
       </c>
       <c r="C4" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(0,50,31,100)</v>
+        <v>hsva(0,40,31,100)</v>
       </c>
       <c r="D4" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(30,50,31,100)</v>
+        <v>hsva(30,40,31,100)</v>
       </c>
       <c r="E4" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(60,50,31,100)</v>
+        <v>hsva(60,40,31,100)</v>
       </c>
       <c r="F4" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(90,50,31,100)</v>
+        <v>hsva(90,40,31,100)</v>
       </c>
       <c r="G4" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(120,50,31,100)</v>
+        <v>hsva(120,40,31,100)</v>
       </c>
       <c r="H4" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(150,50,31,100)</v>
+        <v>hsva(150,40,31,100)</v>
       </c>
       <c r="I4" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(180,50,31,100)</v>
+        <v>hsva(180,40,31,100)</v>
       </c>
       <c r="J4" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(210,50,31,100)</v>
+        <v>hsva(210,40,31,100)</v>
       </c>
       <c r="K4" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(240,50,31,100)</v>
+        <v>hsva(240,40,31,100)</v>
       </c>
       <c r="L4" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(270,50,31,100)</v>
+        <v>hsva(270,40,31,100)</v>
       </c>
       <c r="M4" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(300,50,31,100)</v>
+        <v>hsva(300,40,31,100)</v>
       </c>
       <c r="N4" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(330,50,31,100)</v>
+        <v>hsva(330,40,31,100)</v>
       </c>
       <c r="O4" s="3" t="str">
         <f t="shared" si="2"/>
@@ -9487,51 +9487,51 @@
       </c>
       <c r="C5" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(0,50,19,100)</v>
+        <v>hsva(0,40,19,100)</v>
       </c>
       <c r="D5" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(30,50,19,100)</v>
+        <v>hsva(30,40,19,100)</v>
       </c>
       <c r="E5" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(60,50,19,100)</v>
+        <v>hsva(60,40,19,100)</v>
       </c>
       <c r="F5" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(90,50,19,100)</v>
+        <v>hsva(90,40,19,100)</v>
       </c>
       <c r="G5" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(120,50,19,100)</v>
+        <v>hsva(120,40,19,100)</v>
       </c>
       <c r="H5" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(150,50,19,100)</v>
+        <v>hsva(150,40,19,100)</v>
       </c>
       <c r="I5" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(180,50,19,100)</v>
+        <v>hsva(180,40,19,100)</v>
       </c>
       <c r="J5" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(210,50,19,100)</v>
+        <v>hsva(210,40,19,100)</v>
       </c>
       <c r="K5" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(240,50,19,100)</v>
+        <v>hsva(240,40,19,100)</v>
       </c>
       <c r="L5" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(270,50,19,100)</v>
+        <v>hsva(270,40,19,100)</v>
       </c>
       <c r="M5" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(300,50,19,100)</v>
+        <v>hsva(300,40,19,100)</v>
       </c>
       <c r="N5" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(330,50,19,100)</v>
+        <v>hsva(330,40,19,100)</v>
       </c>
       <c r="O5" s="3" t="str">
         <f t="shared" si="2"/>
@@ -9547,51 +9547,51 @@
       </c>
       <c r="C6" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(0,50,0,100)</v>
+        <v>hsva(0,40,0,100)</v>
       </c>
       <c r="D6" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(30,50,0,100)</v>
+        <v>hsva(30,40,0,100)</v>
       </c>
       <c r="E6" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(60,50,0,100)</v>
+        <v>hsva(60,40,0,100)</v>
       </c>
       <c r="F6" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(90,50,0,100)</v>
+        <v>hsva(90,40,0,100)</v>
       </c>
       <c r="G6" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(120,50,0,100)</v>
+        <v>hsva(120,40,0,100)</v>
       </c>
       <c r="H6" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(150,50,0,100)</v>
+        <v>hsva(150,40,0,100)</v>
       </c>
       <c r="I6" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(180,50,0,100)</v>
+        <v>hsva(180,40,0,100)</v>
       </c>
       <c r="J6" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(210,50,0,100)</v>
+        <v>hsva(210,40,0,100)</v>
       </c>
       <c r="K6" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(240,50,0,100)</v>
+        <v>hsva(240,40,0,100)</v>
       </c>
       <c r="L6" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(270,50,0,100)</v>
+        <v>hsva(270,40,0,100)</v>
       </c>
       <c r="M6" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(300,50,0,100)</v>
+        <v>hsva(300,40,0,100)</v>
       </c>
       <c r="N6" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(330,50,0,100)</v>
+        <v>hsva(330,40,0,100)</v>
       </c>
       <c r="O6" s="3" t="str">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
Improve waffle plot coloring and ordering
</commit_message>
<xml_diff>
--- a/io_in/city_list.xlsx
+++ b/io_in/city_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Coding/roadtrips/io_in/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/code/roadtrips/io_in/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A82317-D58A-614C-A7DF-BD3B32D1732A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CF378E-CFD8-954E-8E16-4DCCCD6A20A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="500" windowWidth="26920" windowHeight="21900" activeTab="3" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
+    <workbookView xWindow="-19720" yWindow="500" windowWidth="19640" windowHeight="18360" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="9" r:id="rId1"/>
@@ -1654,9 +1654,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1694,7 +1694,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1800,7 +1800,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1942,7 +1942,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1952,11 +1952,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418BD67C-5132-6942-B406-D98F46E6A0BD}">
   <dimension ref="A1:R121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E32" sqref="E32"/>
+      <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9238,8 +9238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1D4776-82C5-A549-993A-3BE59A636F7D}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9306,52 +9306,52 @@
         <v>80</v>
       </c>
       <c r="C2" s="3" t="str">
-        <f>"hsva("&amp;C$1&amp;",40,"&amp;$B2&amp;",100)"</f>
-        <v>hsva(0,40,80,100)</v>
+        <f t="shared" ref="C2:E6" si="0">"hsva("&amp;C$1&amp;",50,"&amp;$B2&amp;",100)"</f>
+        <v>hsva(0,50,80,100)</v>
       </c>
       <c r="D2" s="3" t="str">
-        <f>"hsva("&amp;D$1&amp;",40,"&amp;$B2&amp;",100)"</f>
-        <v>hsva(30,40,80,100)</v>
+        <f t="shared" si="0"/>
+        <v>hsva(30,50,80,100)</v>
       </c>
       <c r="E2" s="3" t="str">
-        <f t="shared" ref="E2:N2" si="0">"hsva("&amp;E$1&amp;",40,"&amp;$B2&amp;",100)"</f>
-        <v>hsva(60,40,80,100)</v>
+        <f t="shared" si="0"/>
+        <v>hsva(60,50,80,100)</v>
       </c>
       <c r="F2" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>hsva(90,40,80,100)</v>
+        <f t="shared" ref="F2:I6" si="1">"hsva("&amp;F$1&amp;",50,"&amp;$B2&amp;",100)"</f>
+        <v>hsva(90,50,80,100)</v>
       </c>
       <c r="G2" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>hsva(120,40,80,100)</v>
+        <f t="shared" si="1"/>
+        <v>hsva(120,50,80,100)</v>
       </c>
       <c r="H2" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>hsva(150,40,80,100)</v>
+        <f t="shared" si="1"/>
+        <v>hsva(150,50,80,100)</v>
       </c>
       <c r="I2" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>hsva(180,40,80,100)</v>
+        <f t="shared" si="1"/>
+        <v>hsva(180,50,80,100)</v>
       </c>
       <c r="J2" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>hsva(210,40,80,100)</v>
+        <f t="shared" ref="J2:L6" si="2">"hsva("&amp;J$1&amp;",50,"&amp;$B2&amp;",100)"</f>
+        <v>hsva(210,50,80,100)</v>
       </c>
       <c r="K2" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>hsva(240,40,80,100)</v>
+        <f t="shared" si="2"/>
+        <v>hsva(240,50,80,100)</v>
       </c>
       <c r="L2" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>hsva(270,40,80,100)</v>
+        <f t="shared" si="2"/>
+        <v>hsva(270,50,80,100)</v>
       </c>
       <c r="M2" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>hsva(300,40,80,100)</v>
+        <f t="shared" ref="M2:N6" si="3">"hsva("&amp;M$1&amp;",50,"&amp;$B2&amp;",100)"</f>
+        <v>hsva(300,50,80,100)</v>
       </c>
       <c r="N2" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>hsva(330,40,80,100)</v>
+        <f t="shared" si="3"/>
+        <v>hsva(330,50,80,100)</v>
       </c>
       <c r="O2" s="3" t="str">
         <f>"hsv(0,0,"&amp;$B2&amp;")"</f>
@@ -9366,55 +9366,55 @@
         <v>50</v>
       </c>
       <c r="C3" s="3" t="str">
-        <f t="shared" ref="C3:N6" si="1">"hsva("&amp;C$1&amp;",40,"&amp;$B3&amp;",100)"</f>
-        <v>hsva(0,40,50,100)</v>
+        <f t="shared" si="0"/>
+        <v>hsva(0,50,50,100)</v>
       </c>
       <c r="D3" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(30,40,50,100)</v>
+        <f t="shared" si="0"/>
+        <v>hsva(30,50,50,100)</v>
       </c>
       <c r="E3" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(60,40,50,100)</v>
+        <f t="shared" si="0"/>
+        <v>hsva(60,50,50,100)</v>
       </c>
       <c r="F3" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(90,40,50,100)</v>
+        <v>hsva(90,50,50,100)</v>
       </c>
       <c r="G3" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(120,40,50,100)</v>
+        <v>hsva(120,50,50,100)</v>
       </c>
       <c r="H3" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(150,40,50,100)</v>
+        <v>hsva(150,50,50,100)</v>
       </c>
       <c r="I3" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(180,40,50,100)</v>
+        <v>hsva(180,50,50,100)</v>
       </c>
       <c r="J3" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(210,40,50,100)</v>
+        <f t="shared" si="2"/>
+        <v>hsva(210,50,50,100)</v>
       </c>
       <c r="K3" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(240,40,50,100)</v>
+        <f t="shared" si="2"/>
+        <v>hsva(240,50,50,100)</v>
       </c>
       <c r="L3" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(270,40,50,100)</v>
+        <f t="shared" si="2"/>
+        <v>hsva(270,50,50,100)</v>
       </c>
       <c r="M3" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(300,40,50,100)</v>
+        <f t="shared" si="3"/>
+        <v>hsva(300,50,50,100)</v>
       </c>
       <c r="N3" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(330,40,50,100)</v>
+        <f t="shared" si="3"/>
+        <v>hsva(330,50,50,100)</v>
       </c>
       <c r="O3" s="3" t="str">
-        <f t="shared" ref="O3:O6" si="2">"hsv(0,0,"&amp;$B3&amp;")"</f>
+        <f t="shared" ref="O3:O6" si="4">"hsv(0,0,"&amp;$B3&amp;")"</f>
         <v>hsv(0,0,50)</v>
       </c>
     </row>
@@ -9426,55 +9426,55 @@
         <v>31</v>
       </c>
       <c r="C4" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(0,40,31,100)</v>
+        <f t="shared" si="0"/>
+        <v>hsva(0,50,31,100)</v>
       </c>
       <c r="D4" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(30,40,31,100)</v>
+        <f t="shared" si="0"/>
+        <v>hsva(30,50,31,100)</v>
       </c>
       <c r="E4" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(60,40,31,100)</v>
+        <f t="shared" si="0"/>
+        <v>hsva(60,50,31,100)</v>
       </c>
       <c r="F4" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(90,40,31,100)</v>
+        <v>hsva(90,50,31,100)</v>
       </c>
       <c r="G4" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(120,40,31,100)</v>
+        <v>hsva(120,50,31,100)</v>
       </c>
       <c r="H4" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(150,40,31,100)</v>
+        <v>hsva(150,50,31,100)</v>
       </c>
       <c r="I4" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(180,40,31,100)</v>
+        <v>hsva(180,50,31,100)</v>
       </c>
       <c r="J4" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(210,40,31,100)</v>
+        <f t="shared" si="2"/>
+        <v>hsva(210,50,31,100)</v>
       </c>
       <c r="K4" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(240,40,31,100)</v>
+        <f t="shared" si="2"/>
+        <v>hsva(240,50,31,100)</v>
       </c>
       <c r="L4" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(270,40,31,100)</v>
+        <f t="shared" si="2"/>
+        <v>hsva(270,50,31,100)</v>
       </c>
       <c r="M4" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(300,40,31,100)</v>
+        <f t="shared" si="3"/>
+        <v>hsva(300,50,31,100)</v>
       </c>
       <c r="N4" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(330,40,31,100)</v>
+        <f t="shared" si="3"/>
+        <v>hsva(330,50,31,100)</v>
       </c>
       <c r="O4" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>hsv(0,0,31)</v>
       </c>
     </row>
@@ -9486,55 +9486,55 @@
         <v>19</v>
       </c>
       <c r="C5" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(0,40,19,100)</v>
+        <f t="shared" si="0"/>
+        <v>hsva(0,50,19,100)</v>
       </c>
       <c r="D5" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(30,40,19,100)</v>
+        <f t="shared" si="0"/>
+        <v>hsva(30,50,19,100)</v>
       </c>
       <c r="E5" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(60,40,19,100)</v>
+        <f t="shared" si="0"/>
+        <v>hsva(60,50,19,100)</v>
       </c>
       <c r="F5" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(90,40,19,100)</v>
+        <v>hsva(90,50,19,100)</v>
       </c>
       <c r="G5" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(120,40,19,100)</v>
+        <v>hsva(120,50,19,100)</v>
       </c>
       <c r="H5" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(150,40,19,100)</v>
+        <v>hsva(150,50,19,100)</v>
       </c>
       <c r="I5" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(180,40,19,100)</v>
+        <v>hsva(180,50,19,100)</v>
       </c>
       <c r="J5" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(210,40,19,100)</v>
+        <f t="shared" si="2"/>
+        <v>hsva(210,50,19,100)</v>
       </c>
       <c r="K5" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(240,40,19,100)</v>
+        <f t="shared" si="2"/>
+        <v>hsva(240,50,19,100)</v>
       </c>
       <c r="L5" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(270,40,19,100)</v>
+        <f t="shared" si="2"/>
+        <v>hsva(270,50,19,100)</v>
       </c>
       <c r="M5" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(300,40,19,100)</v>
+        <f t="shared" si="3"/>
+        <v>hsva(300,50,19,100)</v>
       </c>
       <c r="N5" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(330,40,19,100)</v>
+        <f t="shared" si="3"/>
+        <v>hsva(330,50,19,100)</v>
       </c>
       <c r="O5" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>hsv(0,0,19)</v>
       </c>
     </row>
@@ -9546,55 +9546,55 @@
         <v>0</v>
       </c>
       <c r="C6" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(0,40,0,100)</v>
+        <f t="shared" si="0"/>
+        <v>hsva(0,50,0,100)</v>
       </c>
       <c r="D6" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(30,40,0,100)</v>
+        <f t="shared" si="0"/>
+        <v>hsva(30,50,0,100)</v>
       </c>
       <c r="E6" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(60,40,0,100)</v>
+        <f t="shared" si="0"/>
+        <v>hsva(60,50,0,100)</v>
       </c>
       <c r="F6" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(90,40,0,100)</v>
+        <v>hsva(90,50,0,100)</v>
       </c>
       <c r="G6" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(120,40,0,100)</v>
+        <v>hsva(120,50,0,100)</v>
       </c>
       <c r="H6" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(150,40,0,100)</v>
+        <v>hsva(150,50,0,100)</v>
       </c>
       <c r="I6" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>hsva(180,40,0,100)</v>
+        <v>hsva(180,50,0,100)</v>
       </c>
       <c r="J6" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(210,40,0,100)</v>
+        <f t="shared" si="2"/>
+        <v>hsva(210,50,0,100)</v>
       </c>
       <c r="K6" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(240,40,0,100)</v>
+        <f t="shared" si="2"/>
+        <v>hsva(240,50,0,100)</v>
       </c>
       <c r="L6" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(270,40,0,100)</v>
+        <f t="shared" si="2"/>
+        <v>hsva(270,50,0,100)</v>
       </c>
       <c r="M6" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(300,40,0,100)</v>
+        <f t="shared" si="3"/>
+        <v>hsva(300,50,0,100)</v>
       </c>
       <c r="N6" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>hsva(330,40,0,100)</v>
+        <f t="shared" si="3"/>
+        <v>hsva(330,50,0,100)</v>
       </c>
       <c r="O6" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>hsv(0,0,0)</v>
       </c>
     </row>
@@ -9652,10 +9652,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{777FE5C5-9298-4A44-8C2F-DF5EF8BB8EFF}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9674,164 +9674,114 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>426</v>
+        <v>439</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>423</v>
+        <v>440</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>424</v>
+        <v>459</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>427</v>
+        <v>456</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>120</v>
+        <v>180</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>150</v>
+        <v>210</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>440</v>
+        <v>457</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>439</v>
+        <v>458</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>210</v>
+        <v>120</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>240</v>
+        <v>150</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>229</v>
+        <v>424</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>300</v>
+        <v>210</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>425</v>
+        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>330</v>
+        <v>240</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>420</v>
+        <v>426</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>0</v>
+        <v>270</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
-        <v>180</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
-        <v>210</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
-        <v>240</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
-        <v>270</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
         <v>300</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
-        <v>330</v>
+      <c r="B15" s="2" t="s">
+        <v>427</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve weather data code (issue 27
</commit_message>
<xml_diff>
--- a/io_in/city_list.xlsx
+++ b/io_in/city_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/code/roadtrips/io_in/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CF378E-CFD8-954E-8E16-4DCCCD6A20A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF963BC0-124D-E54A-8E5A-36C8D5CDA553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19720" yWindow="500" windowWidth="19640" windowHeight="18360" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
+    <workbookView xWindow="12520" yWindow="500" windowWidth="22620" windowHeight="21900" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="9" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="458">
   <si>
     <t>Boston MA</t>
   </si>
@@ -927,9 +927,6 @@
     <t>USW00023234</t>
   </si>
   <si>
-    <t>USW00094847</t>
-  </si>
-  <si>
     <t>USW00024233</t>
   </si>
   <si>
@@ -978,15 +975,9 @@
     <t>USW00013893</t>
   </si>
   <si>
-    <t>USW00014733</t>
-  </si>
-  <si>
     <t>USW00094860</t>
   </si>
   <si>
-    <t>USW00014768</t>
-  </si>
-  <si>
     <t>USW00013968</t>
   </si>
   <si>
@@ -1065,9 +1056,6 @@
     <t>USW00003945</t>
   </si>
   <si>
-    <t>USW00024132</t>
-  </si>
-  <si>
     <t>USW00014710</t>
   </si>
   <si>
@@ -1420,6 +1408,12 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>USW00014822</t>
+  </si>
+  <si>
+    <t>USW00004724</t>
   </si>
 </sst>
 </file>
@@ -1953,10 +1947,10 @@
   <dimension ref="A1:R121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C73" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
+      <selection pane="bottomRight" activeCell="H86" sqref="H86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2022,16 +2016,16 @@
         <v>216</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>397</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>401</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>177</v>
@@ -2057,7 +2051,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="J2" s="13">
         <v>-149.9002778</v>
@@ -2072,7 +2066,7 @@
         <v>244</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="O2" s="1" t="str">
         <f>LOOKUP(N2,Climate!A:A,Climate!B:B)</f>
@@ -2087,7 +2081,7 @@
         <v>Cold, Wet</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
@@ -2110,7 +2104,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J3" s="13">
         <v>-134.42161300000001</v>
@@ -2125,7 +2119,7 @@
         <v>245</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="O3" s="1" t="str">
         <f>LOOKUP(N3,Climate!A:A,Climate!B:B)</f>
@@ -2140,7 +2134,7 @@
         <v>Cold, Wet</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
@@ -2165,7 +2159,7 @@
         <v>3.8</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H4" s="4">
         <v>1181196</v>
@@ -2181,7 +2175,7 @@
         <v>246</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O4" s="1" t="str">
         <f>LOOKUP(N4,Climate!A:A,Climate!B:B)</f>
@@ -2196,7 +2190,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
@@ -2221,7 +2215,7 @@
         <v>4</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J5" s="13">
         <v>-86.307736800000001</v>
@@ -2234,7 +2228,7 @@
         <v>247</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O5" s="1" t="str">
         <f>LOOKUP(N5,Climate!A:A,Climate!B:B)</f>
@@ -2249,7 +2243,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -2272,7 +2266,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J6" s="13">
         <v>-92.289594800000003</v>
@@ -2285,7 +2279,7 @@
         <v>248</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O6" s="1" t="str">
         <f>LOOKUP(N6,Climate!A:A,Climate!B:B)</f>
@@ -2300,7 +2294,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="7" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2323,7 +2317,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="1" t="s">
@@ -2340,7 +2334,7 @@
         <v>249</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="O7" s="1" t="str">
         <f>LOOKUP(N7,Climate!A:A,Climate!B:B)</f>
@@ -2378,7 +2372,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="H8" s="4">
         <v>5015678</v>
@@ -2394,7 +2388,7 @@
         <v>249</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="O8" s="1" t="str">
         <f>LOOKUP(N8,Climate!A:A,Climate!B:B)</f>
@@ -2432,7 +2426,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H9" s="4">
         <v>1057597</v>
@@ -2448,7 +2442,7 @@
         <v>250</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="O9" s="1" t="str">
         <f>LOOKUP(N9,Climate!A:A,Climate!B:B)</f>
@@ -2485,7 +2479,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>196</v>
@@ -2497,10 +2491,10 @@
         <v>40.801943999999999</v>
       </c>
       <c r="M10" s="27" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="O10" s="1" t="str">
         <f>LOOKUP(N10,Climate!A:A,Climate!B:B)</f>
@@ -2515,7 +2509,7 @@
         <v xml:space="preserve">Dry, Warm </v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
@@ -2538,7 +2532,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="H11" s="4">
         <v>1175446</v>
@@ -2554,7 +2548,7 @@
         <v>251</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="O11" s="1" t="str">
         <f>LOOKUP(N11,Climate!A:A,Climate!B:B)</f>
@@ -2595,7 +2589,7 @@
         <v>27</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H12" s="4">
         <v>12872322</v>
@@ -2611,7 +2605,7 @@
         <v>284</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="O12" s="1" t="str">
         <f>LOOKUP(N12,Climate!A:A,Climate!B:B)</f>
@@ -2651,7 +2645,7 @@
         <v>3</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="H13" s="4">
         <v>4667558</v>
@@ -2667,7 +2661,7 @@
         <v>284</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="O13" s="1" t="str">
         <f>LOOKUP(N13,Climate!A:A,Climate!B:B)</f>
@@ -2705,7 +2699,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="H14" s="4">
         <v>2416702</v>
@@ -2721,7 +2715,7 @@
         <v>252</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="O14" s="1" t="str">
         <f>LOOKUP(N14,Climate!A:A,Climate!B:B)</f>
@@ -2736,7 +2730,7 @@
         <v xml:space="preserve">Dry, Hot </v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
@@ -2762,7 +2756,7 @@
         <v>31.1</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="H15" s="4">
         <v>3276208</v>
@@ -2775,10 +2769,10 @@
       </c>
       <c r="L15" s="5"/>
       <c r="M15" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="O15" s="1" t="str">
         <f>LOOKUP(N15,Climate!A:A,Climate!B:B)</f>
@@ -2816,7 +2810,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="H16" s="4">
         <v>4579599</v>
@@ -2832,7 +2826,7 @@
         <v>294</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="O16" s="1" t="str">
         <f>LOOKUP(N16,Climate!A:A,Climate!B:B)</f>
@@ -2847,7 +2841,7 @@
         <v xml:space="preserve">Dry, Warm </v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
@@ -2870,7 +2864,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="H17" s="4">
         <v>1938524</v>
@@ -2886,7 +2880,7 @@
         <v>294</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="O17" s="1" t="str">
         <f>LOOKUP(N17,Climate!A:A,Climate!B:B)</f>
@@ -2901,7 +2895,7 @@
         <v xml:space="preserve">Dry, Hot </v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
@@ -2923,7 +2917,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>201</v>
@@ -2935,10 +2929,10 @@
         <v>37.984444000000003</v>
       </c>
       <c r="M18" s="27" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="O18" s="1" t="str">
         <f>LOOKUP(N18,Climate!A:A,Climate!B:B)</f>
@@ -2953,7 +2947,7 @@
         <v xml:space="preserve">Dry, Hot </v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
@@ -2975,7 +2969,7 @@
         <v>0</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="J19" s="14">
         <v>-104.825278</v>
@@ -2984,10 +2978,10 @@
         <v>38.833888999999999</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="O19" s="1" t="str">
         <f>LOOKUP(N19,Climate!A:A,Climate!B:B)</f>
@@ -3002,7 +2996,7 @@
         <v>Dry</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
@@ -3025,7 +3019,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="H20" s="4">
         <v>2985871</v>
@@ -3041,7 +3035,7 @@
         <v>253</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="O20" s="1" t="str">
         <f>LOOKUP(N20,Climate!A:A,Climate!B:B)</f>
@@ -3056,7 +3050,7 @@
         <v>Dry</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
@@ -3081,7 +3075,7 @@
         <v>2.1</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="H21" s="4">
         <v>1158069</v>
@@ -3097,7 +3091,7 @@
         <v>254</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="O21" s="1" t="str">
         <f>LOOKUP(N21,Climate!A:A,Climate!B:B)</f>
@@ -3112,7 +3106,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
@@ -3137,7 +3131,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="J22" s="13">
         <v>-72.923610999999994</v>
@@ -3150,7 +3144,7 @@
         <v>254</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O22" s="1" t="str">
         <f>LOOKUP(N22,Climate!A:A,Climate!B:B)</f>
@@ -3165,7 +3159,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
@@ -3190,7 +3184,7 @@
         <v>99.9</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="H23" s="4">
         <v>6265183</v>
@@ -3205,10 +3199,10 @@
         <v>126</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O23" s="1" t="str">
         <f>LOOKUP(N23,Climate!A:A,Climate!B:B)</f>
@@ -3223,7 +3217,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
@@ -3248,7 +3242,7 @@
         <v>1.8</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J24" s="13">
         <v>-75.524368199999998</v>
@@ -3258,10 +3252,10 @@
       </c>
       <c r="L24" s="5"/>
       <c r="M24" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O24" s="1" t="str">
         <f>LOOKUP(N24,Climate!A:A,Climate!B:B)</f>
@@ -3276,7 +3270,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
@@ -3301,7 +3295,7 @@
         <v>11.5</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="H25" s="4">
         <v>1675668</v>
@@ -3317,10 +3311,10 @@
       </c>
       <c r="L25" s="5"/>
       <c r="M25" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O25" s="1" t="str">
         <f>LOOKUP(N25,Climate!A:A,Climate!B:B)</f>
@@ -3335,7 +3329,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
@@ -3361,7 +3355,7 @@
         <v>8.9</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>204</v>
@@ -3374,10 +3368,10 @@
       </c>
       <c r="L26" s="5"/>
       <c r="M26" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="O26" s="1" t="str">
         <f>LOOKUP(N26,Climate!A:A,Climate!B:B)</f>
@@ -3392,7 +3386,7 @@
         <v>Wet</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
@@ -3417,7 +3411,7 @@
         <v>14.3</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H27" s="4">
         <v>6139340</v>
@@ -3433,7 +3427,7 @@
         <v>285</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="O27" s="1" t="str">
         <f>LOOKUP(N27,Climate!A:A,Climate!B:B)</f>
@@ -3448,7 +3442,7 @@
         <v>Wet</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
@@ -3473,7 +3467,7 @@
         <v>6.1</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="H28" s="4">
         <v>2764182</v>
@@ -3486,10 +3480,10 @@
       </c>
       <c r="L28" s="5"/>
       <c r="M28" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O28" s="1" t="str">
         <f>LOOKUP(N28,Climate!A:A,Climate!B:B)</f>
@@ -3504,7 +3498,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="29" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -3529,7 +3523,7 @@
         <v>5</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="H29" s="4"/>
       <c r="I29" s="1"/>
@@ -3541,10 +3535,10 @@
       </c>
       <c r="L29" s="5"/>
       <c r="M29" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O29" s="1" t="str">
         <f>LOOKUP(N29,Climate!A:A,Climate!B:B)</f>
@@ -3559,7 +3553,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="30" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -3584,7 +3578,7 @@
         <v>7.4</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="H30" s="4">
         <v>3290730</v>
@@ -3598,10 +3592,10 @@
       </c>
       <c r="L30" s="5"/>
       <c r="M30" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O30" s="1" t="str">
         <f>LOOKUP(N30,Climate!A:A,Climate!B:B)</f>
@@ -3616,7 +3610,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
@@ -3642,7 +3636,7 @@
         <v>10.5</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="H31" s="4">
         <v>6237435</v>
@@ -3658,7 +3652,7 @@
         <v>255</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O31" s="1" t="str">
         <f>LOOKUP(N31,Climate!A:A,Climate!B:B)</f>
@@ -3673,7 +3667,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
@@ -3698,7 +3692,7 @@
         <v>8.6</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="J32" s="13">
         <v>-81.091202999999993</v>
@@ -3708,10 +3702,10 @@
       </c>
       <c r="L32" s="5"/>
       <c r="M32" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O32" s="1" t="str">
         <f>LOOKUP(N32,Climate!A:A,Climate!B:B)</f>
@@ -3726,7 +3720,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
@@ -3749,7 +3743,7 @@
         <v>0</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="H33" s="4">
         <v>995638</v>
@@ -3767,7 +3761,7 @@
         <v>256</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="O33" s="1" t="str">
         <f>LOOKUP(N33,Climate!A:A,Climate!B:B)</f>
@@ -3782,7 +3776,7 @@
         <v>Dry</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.2">
@@ -3807,7 +3801,7 @@
         <v>1.8</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="J34" s="13">
         <v>-90.577636699999999</v>
@@ -3817,10 +3811,10 @@
       </c>
       <c r="L34" s="5"/>
       <c r="M34" s="27" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="O34" s="1" t="str">
         <f>LOOKUP(N34,Climate!A:A,Climate!B:B)</f>
@@ -3835,7 +3829,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.2">
@@ -3860,7 +3854,7 @@
         <v>8.1</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J35" s="13">
         <v>-93.6249593</v>
@@ -3873,7 +3867,7 @@
         <v>257</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="O35" s="1" t="str">
         <f>LOOKUP(N35,Climate!A:A,Climate!B:B)</f>
@@ -3888,7 +3882,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R35" s="1" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
@@ -3911,7 +3905,7 @@
         <v>0</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J36" s="13">
         <v>-116.2023137</v>
@@ -3924,7 +3918,7 @@
         <v>258</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="O36" s="1" t="str">
         <f>LOOKUP(N36,Climate!A:A,Climate!B:B)</f>
@@ -3939,7 +3933,7 @@
         <v>Dry</v>
       </c>
       <c r="R36" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.2">
@@ -3962,7 +3956,7 @@
         <v>0</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="J37" s="13">
         <v>-116.78</v>
@@ -3972,10 +3966,10 @@
       </c>
       <c r="L37" s="5"/>
       <c r="M37" s="27" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="O37" s="1" t="str">
         <f>LOOKUP(N37,Climate!A:A,Climate!B:B)</f>
@@ -3990,7 +3984,7 @@
         <v xml:space="preserve">Dry, Warm </v>
       </c>
       <c r="R37" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
@@ -4015,7 +4009,7 @@
         <v>22.7</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H38" s="4">
         <v>9274140</v>
@@ -4031,7 +4025,7 @@
         <v>286</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="O38" s="1" t="str">
         <f>LOOKUP(N38,Climate!A:A,Climate!B:B)</f>
@@ -4046,7 +4040,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R38" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
@@ -4071,7 +4065,7 @@
         <v>6.6</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J39" s="13">
         <v>-89.650148099999996</v>
@@ -4084,7 +4078,7 @@
         <v>259</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="O39" s="1" t="str">
         <f>LOOKUP(N39,Climate!A:A,Climate!B:B)</f>
@@ -4099,7 +4093,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R39" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="40" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -4124,7 +4118,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="H40" s="4">
         <v>2119839</v>
@@ -4138,10 +4132,10 @@
       </c>
       <c r="L40" s="5"/>
       <c r="M40" s="1" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="O40" s="1" t="str">
         <f>LOOKUP(N40,Climate!A:A,Climate!B:B)</f>
@@ -4156,7 +4150,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R40" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.2">
@@ -4181,7 +4175,7 @@
         <v>2.6</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J41" s="13">
         <v>-95.675157600000006</v>
@@ -4194,7 +4188,7 @@
         <v>260</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="O41" s="1" t="str">
         <f>LOOKUP(N41,Climate!A:A,Climate!B:B)</f>
@@ -4209,7 +4203,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R41" s="1" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.2">
@@ -4232,7 +4226,7 @@
         <v>0</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="J42" s="13">
         <v>-97.330053000000007</v>
@@ -4242,10 +4236,10 @@
       </c>
       <c r="L42" s="5"/>
       <c r="M42" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O42" s="1" t="str">
         <f>LOOKUP(N42,Climate!A:A,Climate!B:B)</f>
@@ -4260,7 +4254,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R42" s="1" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.2">
@@ -4285,7 +4279,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J43" s="13">
         <v>-84.873283499999999</v>
@@ -4295,10 +4289,10 @@
       </c>
       <c r="L43" s="5"/>
       <c r="M43" s="27" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O43" s="1" t="str">
         <f>LOOKUP(N43,Climate!A:A,Climate!B:B)</f>
@@ -4313,7 +4307,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R43" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.2">
@@ -4338,7 +4332,7 @@
         <v>7.6</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H44" s="4">
         <v>1361946</v>
@@ -4351,10 +4345,10 @@
       </c>
       <c r="L44" s="5"/>
       <c r="M44" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="N44" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O44" s="1" t="str">
         <f>LOOKUP(N44,Climate!A:A,Climate!B:B)</f>
@@ -4369,7 +4363,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R44" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.2">
@@ -4392,7 +4386,7 @@
         <v>0</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J45" s="13">
         <v>-91.187146600000005</v>
@@ -4402,10 +4396,10 @@
       </c>
       <c r="L45" s="5"/>
       <c r="M45" s="27" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O45" s="1" t="str">
         <f>LOOKUP(N45,Climate!A:A,Climate!B:B)</f>
@@ -4420,7 +4414,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R45" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.2">
@@ -4446,7 +4440,7 @@
         <v>23.9</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="J46" s="13">
         <v>-90.071532300000001</v>
@@ -4456,10 +4450,10 @@
       </c>
       <c r="L46" s="5"/>
       <c r="M46" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O46" s="1" t="str">
         <f>LOOKUP(N46,Climate!A:A,Climate!B:B)</f>
@@ -4474,7 +4468,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R46" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.2">
@@ -4497,7 +4491,7 @@
       </c>
       <c r="F47" s="23"/>
       <c r="G47" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="H47" s="4">
         <v>4900550</v>
@@ -4513,7 +4507,7 @@
         <v>261</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="O47" s="1" t="str">
         <f>LOOKUP(N47,Climate!A:A,Climate!B:B)</f>
@@ -4528,7 +4522,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R47" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.2">
@@ -4551,7 +4545,7 @@
       </c>
       <c r="F48" s="23"/>
       <c r="G48" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J48" s="13">
         <v>-76.492182900000003</v>
@@ -4561,10 +4555,10 @@
       </c>
       <c r="L48" s="5"/>
       <c r="M48" s="27" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O48" s="1" t="str">
         <f>LOOKUP(N48,Climate!A:A,Climate!B:B)</f>
@@ -4579,7 +4573,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R48" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.2">
@@ -4602,7 +4596,7 @@
       </c>
       <c r="F49" s="23"/>
       <c r="G49" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H49" s="4">
         <v>2835672</v>
@@ -4615,10 +4609,10 @@
       </c>
       <c r="L49" s="5"/>
       <c r="M49" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="N49" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O49" s="1" t="str">
         <f>LOOKUP(N49,Climate!A:A,Climate!B:B)</f>
@@ -4633,7 +4627,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R49" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.2">
@@ -4658,7 +4652,7 @@
         <v>3.2</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J50" s="13">
         <v>-69.779489699999999</v>
@@ -4671,7 +4665,7 @@
         <v>262</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="O50" s="1" t="str">
         <f>LOOKUP(N50,Climate!A:A,Climate!B:B)</f>
@@ -4686,7 +4680,7 @@
         <v>Warm, Wet</v>
       </c>
       <c r="R50" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.2">
@@ -4711,7 +4705,7 @@
         <v>5.2</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="J51" s="13">
         <v>-70.256818899999999</v>
@@ -4721,10 +4715,10 @@
       </c>
       <c r="L51" s="5"/>
       <c r="M51" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="N51" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="O51" s="1" t="str">
         <f>LOOKUP(N51,Climate!A:A,Climate!B:B)</f>
@@ -4739,7 +4733,7 @@
         <v>Warm, Wet</v>
       </c>
       <c r="R51" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.2">
@@ -4762,7 +4756,7 @@
       </c>
       <c r="F52" s="23"/>
       <c r="G52" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H52" s="4">
         <v>4345761</v>
@@ -4775,10 +4769,10 @@
       </c>
       <c r="L52" s="5"/>
       <c r="M52" s="1" t="s">
-        <v>295</v>
+        <v>456</v>
       </c>
       <c r="N52" s="1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="O52" s="1" t="str">
         <f>LOOKUP(N52,Climate!A:A,Climate!B:B)</f>
@@ -4793,7 +4787,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R52" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.2">
@@ -4816,7 +4810,7 @@
       </c>
       <c r="F53" s="23"/>
       <c r="G53" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="H53" s="4">
         <v>1157752</v>
@@ -4829,10 +4823,10 @@
       </c>
       <c r="L53" s="5"/>
       <c r="M53" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="N53" s="1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="O53" s="1" t="str">
         <f>LOOKUP(N53,Climate!A:A,Climate!B:B)</f>
@@ -4847,7 +4841,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R53" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.2">
@@ -4870,7 +4864,7 @@
       </c>
       <c r="F54" s="23"/>
       <c r="G54" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J54" s="13">
         <v>-84.555534699999995</v>
@@ -4883,7 +4877,7 @@
         <v>263</v>
       </c>
       <c r="N54" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="O54" s="1" t="str">
         <f>LOOKUP(N54,Climate!A:A,Climate!B:B)</f>
@@ -4898,7 +4892,7 @@
         <v>Warm, Wet</v>
       </c>
       <c r="R54" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.2">
@@ -4920,7 +4914,7 @@
         <v>0</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="J55" s="14">
         <v>-92.098056</v>
@@ -4929,10 +4923,10 @@
         <v>46.786943999999998</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="N55" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="O55" s="1" t="str">
         <f>LOOKUP(N55,Climate!A:A,Climate!B:B)</f>
@@ -4947,7 +4941,7 @@
         <v>Warm, Wet</v>
       </c>
       <c r="R55" s="1" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="56" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -4970,7 +4964,7 @@
         <v>0</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="H56" s="4">
         <v>3693729</v>
@@ -4987,7 +4981,7 @@
         <v>264</v>
       </c>
       <c r="N56" s="1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="O56" s="1" t="str">
         <f>LOOKUP(N56,Climate!A:A,Climate!B:B)</f>
@@ -5002,7 +4996,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R56" s="1" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.2">
@@ -5025,7 +5019,7 @@
       </c>
       <c r="F57" s="23"/>
       <c r="G57" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J57" s="13">
         <v>-92.173516399999997</v>
@@ -5035,10 +5029,10 @@
       </c>
       <c r="L57" s="5"/>
       <c r="M57" s="27" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="N57" s="1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="O57" s="1" t="str">
         <f>LOOKUP(N57,Climate!A:A,Climate!B:B)</f>
@@ -5053,7 +5047,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R57" s="1" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.2">
@@ -5076,7 +5070,7 @@
       </c>
       <c r="F58" s="23"/>
       <c r="G58" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="H58" s="4">
         <v>2209494</v>
@@ -5089,10 +5083,10 @@
       </c>
       <c r="L58" s="5"/>
       <c r="M58" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="N58" s="1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="O58" s="1" t="str">
         <f>LOOKUP(N58,Climate!A:A,Climate!B:B)</f>
@@ -5107,7 +5101,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R58" s="1" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.2">
@@ -5130,7 +5124,7 @@
       </c>
       <c r="F59" s="26"/>
       <c r="G59" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H59" s="4">
         <v>2801319</v>
@@ -5149,7 +5143,7 @@
         <v>291</v>
       </c>
       <c r="N59" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O59" s="1" t="str">
         <f>LOOKUP(N59,Climate!A:A,Climate!B:B)</f>
@@ -5164,7 +5158,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R59" s="1" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.2">
@@ -5187,7 +5181,7 @@
         <v>0</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J60" s="13">
         <v>-90.184810299999995</v>
@@ -5200,7 +5194,7 @@
         <v>265</v>
       </c>
       <c r="N60" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O60" s="1" t="str">
         <f>LOOKUP(N60,Climate!A:A,Climate!B:B)</f>
@@ -5215,7 +5209,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R60" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.2">
@@ -5238,7 +5232,7 @@
         <v>0</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="J61" s="13">
         <v>-108.5006904</v>
@@ -5251,7 +5245,7 @@
         <v>287</v>
       </c>
       <c r="N61" s="1" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="O61" s="1" t="str">
         <f>LOOKUP(N61,Climate!A:A,Climate!B:B)</f>
@@ -5266,7 +5260,7 @@
         <v>Dry</v>
       </c>
       <c r="R61" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.2">
@@ -5288,7 +5282,7 @@
         <v>0</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="I62" s="1" t="s">
         <v>200</v>
@@ -5299,11 +5293,11 @@
       <c r="K62" s="14">
         <v>45.677778000000004</v>
       </c>
-      <c r="M62" s="1" t="s">
-        <v>341</v>
+      <c r="M62" s="27" t="s">
+        <v>266</v>
       </c>
       <c r="N62" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="O62" s="1" t="str">
         <f>LOOKUP(N62,Climate!A:A,Climate!B:B)</f>
@@ -5318,7 +5312,7 @@
         <v>Warm, Wet</v>
       </c>
       <c r="R62" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.2">
@@ -5341,7 +5335,7 @@
         <v>0</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J63" s="13">
         <v>-112.03910569999999</v>
@@ -5354,7 +5348,7 @@
         <v>266</v>
       </c>
       <c r="N63" s="1" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="O63" s="1" t="str">
         <f>LOOKUP(N63,Climate!A:A,Climate!B:B)</f>
@@ -5369,7 +5363,7 @@
         <v>Dry</v>
       </c>
       <c r="R63" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.2">
@@ -5392,7 +5386,7 @@
       </c>
       <c r="F64" s="23"/>
       <c r="G64" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H64" s="4">
         <v>2756069</v>
@@ -5405,10 +5399,10 @@
       </c>
       <c r="L64" s="5"/>
       <c r="M64" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N64" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O64" s="1" t="str">
         <f>LOOKUP(N64,Climate!A:A,Climate!B:B)</f>
@@ -5423,7 +5417,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R64" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="65" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -5446,7 +5440,7 @@
       </c>
       <c r="F65" s="23"/>
       <c r="G65" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="H65" s="4">
         <v>1484338</v>
@@ -5463,7 +5457,7 @@
         <v>267</v>
       </c>
       <c r="N65" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O65" s="1" t="str">
         <f>LOOKUP(N65,Climate!A:A,Climate!B:B)</f>
@@ -5478,7 +5472,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R65" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.2">
@@ -5501,7 +5495,7 @@
         <v>0</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J66" s="13">
         <v>-100.7837392</v>
@@ -5514,7 +5508,7 @@
         <v>268</v>
       </c>
       <c r="N66" s="1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="O66" s="1" t="str">
         <f>LOOKUP(N66,Climate!A:A,Climate!B:B)</f>
@@ -5529,7 +5523,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R66" s="1" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.2">
@@ -5552,7 +5546,7 @@
         <v>0</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="J67" s="13">
         <v>-96.789803399999997</v>
@@ -5562,10 +5556,10 @@
       </c>
       <c r="L67" s="5"/>
       <c r="M67" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="N67" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="O67" s="1" t="str">
         <f>LOOKUP(N67,Climate!A:A,Climate!B:B)</f>
@@ -5580,7 +5574,7 @@
         <v>Warm, Wet</v>
       </c>
       <c r="R67" s="1" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.2">
@@ -5603,7 +5597,7 @@
       </c>
       <c r="F68" s="23"/>
       <c r="G68" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J68" s="13">
         <v>-96.702595500000001</v>
@@ -5616,7 +5610,7 @@
         <v>269</v>
       </c>
       <c r="N68" s="1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="O68" s="1" t="str">
         <f>LOOKUP(N68,Climate!A:A,Climate!B:B)</f>
@@ -5631,7 +5625,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R68" s="1" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.2">
@@ -5654,7 +5648,7 @@
       </c>
       <c r="F69" s="23"/>
       <c r="G69" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="J69" s="13">
         <v>-95.934503399999997</v>
@@ -5664,10 +5658,10 @@
       </c>
       <c r="L69" s="5"/>
       <c r="M69" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="N69" s="1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="O69" s="1" t="str">
         <f>LOOKUP(N69,Climate!A:A,Climate!B:B)</f>
@@ -5682,7 +5676,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R69" s="1" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.2">
@@ -5705,7 +5699,7 @@
       </c>
       <c r="F70" s="23"/>
       <c r="G70" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J70" s="13">
         <v>-71.537571799999995</v>
@@ -5718,7 +5712,7 @@
         <v>270</v>
       </c>
       <c r="N70" s="2" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="O70" s="1" t="str">
         <f>LOOKUP(N70,Climate!A:A,Climate!B:B)</f>
@@ -5733,7 +5727,7 @@
         <v>Warm, Wet</v>
       </c>
       <c r="R70" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.2">
@@ -5756,7 +5750,7 @@
       </c>
       <c r="F71" s="23"/>
       <c r="G71" s="1" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="J71" s="13">
         <v>-71.463611</v>
@@ -5766,10 +5760,10 @@
       </c>
       <c r="L71" s="5"/>
       <c r="M71" s="1" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="N71" s="2" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="O71" s="1" t="str">
         <f>LOOKUP(N71,Climate!A:A,Climate!B:B)</f>
@@ -5784,7 +5778,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R71" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="72" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -5807,7 +5801,7 @@
         <v>0</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H72" s="4"/>
       <c r="I72" s="1"/>
@@ -5819,10 +5813,10 @@
       </c>
       <c r="L72" s="5"/>
       <c r="M72" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="N72" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O72" s="1" t="str">
         <f>LOOKUP(N72,Climate!A:A,Climate!B:B)</f>
@@ -5837,7 +5831,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R72" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.2">
@@ -5862,7 +5856,7 @@
         <v>3.6</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J73" s="13">
         <v>-74.759716999999995</v>
@@ -5872,10 +5866,10 @@
       </c>
       <c r="L73" s="5"/>
       <c r="M73" s="27" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="N73" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O73" s="1" t="str">
         <f>LOOKUP(N73,Climate!A:A,Climate!B:B)</f>
@@ -5890,7 +5884,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R73" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="74" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -5915,7 +5909,7 @@
         <v>8.6</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H74" s="4"/>
       <c r="I74" s="1"/>
@@ -5927,10 +5921,10 @@
       </c>
       <c r="L74" s="5"/>
       <c r="M74" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="N74" s="2" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="O74" s="1" t="str">
         <f>LOOKUP(N74,Climate!A:A,Climate!B:B)</f>
@@ -5970,7 +5964,7 @@
         <v>10.3</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J75" s="13">
         <v>-105.937799</v>
@@ -5980,10 +5974,10 @@
       </c>
       <c r="L75" s="5"/>
       <c r="M75" s="27" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="N75" s="2" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="O75" s="1" t="str">
         <f>LOOKUP(N75,Climate!A:A,Climate!B:B)</f>
@@ -6023,7 +6017,7 @@
         <v>3.5</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="J76" s="13">
         <v>-105.576667</v>
@@ -6033,10 +6027,10 @@
       </c>
       <c r="L76" s="5"/>
       <c r="M76" s="27" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="N76" s="2" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="O76" s="1" t="str">
         <f>LOOKUP(N76,Climate!A:A,Climate!B:B)</f>
@@ -6074,7 +6068,7 @@
         <v>0</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J77" s="13">
         <v>-119.76740340000001</v>
@@ -6084,10 +6078,10 @@
       </c>
       <c r="L77" s="5"/>
       <c r="M77" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="N77" s="2" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="O77" s="1" t="str">
         <f>LOOKUP(N77,Climate!A:A,Climate!B:B)</f>
@@ -6102,7 +6096,7 @@
         <v>Dry</v>
       </c>
       <c r="R77" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.2">
@@ -6127,7 +6121,7 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H78" s="4">
         <v>2322985</v>
@@ -6143,7 +6137,7 @@
         <v>288</v>
       </c>
       <c r="N78" s="2" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="O78" s="1" t="str">
         <f>LOOKUP(N78,Climate!A:A,Climate!B:B)</f>
@@ -6181,7 +6175,7 @@
       </c>
       <c r="F79" s="23"/>
       <c r="G79" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J79" s="13">
         <v>-73.756231700000001</v>
@@ -6194,7 +6188,7 @@
         <v>271</v>
       </c>
       <c r="N79" s="2" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="O79" s="1" t="str">
         <f>LOOKUP(N79,Climate!A:A,Climate!B:B)</f>
@@ -6209,7 +6203,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R79" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.2">
@@ -6232,7 +6226,7 @@
       </c>
       <c r="F80" s="23"/>
       <c r="G80" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="H80" s="4">
         <v>1161192</v>
@@ -6245,10 +6239,10 @@
       </c>
       <c r="L80" s="5"/>
       <c r="M80" s="1" t="s">
-        <v>312</v>
+        <v>457</v>
       </c>
       <c r="N80" s="2" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="O80" s="1" t="str">
         <f>LOOKUP(N80,Climate!A:A,Climate!B:B)</f>
@@ -6263,7 +6257,7 @@
         <v>Warm, Wet</v>
       </c>
       <c r="R80" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.2">
@@ -6289,7 +6283,7 @@
         <v>56.900000000000006</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H81" s="4">
         <v>19557311</v>
@@ -6308,7 +6302,7 @@
         <v>289</v>
       </c>
       <c r="N81" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O81" s="1" t="str">
         <f>LOOKUP(N81,Climate!A:A,Climate!B:B)</f>
@@ -6323,7 +6317,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R81" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.2">
@@ -6346,7 +6340,7 @@
       </c>
       <c r="F82" s="23"/>
       <c r="G82" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="H82" s="4">
         <v>1056701</v>
@@ -6358,11 +6352,11 @@
         <v>43.156577900000002</v>
       </c>
       <c r="L82" s="5"/>
-      <c r="M82" s="1" t="s">
-        <v>314</v>
+      <c r="M82" s="27" t="s">
+        <v>457</v>
       </c>
       <c r="N82" s="2" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="O82" s="1" t="str">
         <f>LOOKUP(N82,Climate!A:A,Climate!B:B)</f>
@@ -6377,7 +6371,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R82" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.2">
@@ -6400,7 +6394,7 @@
       </c>
       <c r="F83" s="23"/>
       <c r="G83" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H83" s="4">
         <v>2258099</v>
@@ -6413,10 +6407,10 @@
       </c>
       <c r="L83" s="5"/>
       <c r="M83" s="27" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="N83" s="2" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="O83" s="1" t="str">
         <f>LOOKUP(N83,Climate!A:A,Climate!B:B)</f>
@@ -6431,7 +6425,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R83" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.2">
@@ -6454,7 +6448,7 @@
       </c>
       <c r="F84" s="23"/>
       <c r="G84" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="H84" s="4">
         <v>2160146</v>
@@ -6467,10 +6461,10 @@
       </c>
       <c r="L84" s="5"/>
       <c r="M84" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="N84" s="2" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="O84" s="1" t="str">
         <f>LOOKUP(N84,Climate!A:A,Climate!B:B)</f>
@@ -6485,7 +6479,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R84" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.2">
@@ -6508,7 +6502,7 @@
       </c>
       <c r="F85" s="23"/>
       <c r="G85" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="H85" s="4">
         <v>2161511</v>
@@ -6524,7 +6518,7 @@
         <v>272</v>
       </c>
       <c r="N85" s="2" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="O85" s="1" t="str">
         <f>LOOKUP(N85,Climate!A:A,Climate!B:B)</f>
@@ -6539,7 +6533,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R85" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.2">
@@ -6562,7 +6556,7 @@
         <v>0</v>
       </c>
       <c r="G86" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="H86" s="4">
         <v>1459380</v>
@@ -6578,7 +6572,7 @@
         <v>273</v>
       </c>
       <c r="N86" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O86" s="1" t="str">
         <f>LOOKUP(N86,Climate!A:A,Climate!B:B)</f>
@@ -6616,7 +6610,7 @@
         <v>0</v>
       </c>
       <c r="G87" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H87" s="4">
         <v>1034123</v>
@@ -6629,10 +6623,10 @@
       </c>
       <c r="L87" s="5"/>
       <c r="M87" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="N87" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O87" s="1" t="str">
         <f>LOOKUP(N87,Climate!A:A,Climate!B:B)</f>
@@ -6670,7 +6664,7 @@
         <v>0</v>
       </c>
       <c r="G88" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H88" s="4">
         <v>2509489</v>
@@ -6683,10 +6677,10 @@
       </c>
       <c r="L88" s="5"/>
       <c r="M88" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="N88" s="2" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="O88" s="1" t="str">
         <f>LOOKUP(N88,Climate!A:A,Climate!B:B)</f>
@@ -6701,7 +6695,7 @@
         <v xml:space="preserve">Dry, Warm </v>
       </c>
       <c r="R88" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="89" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -6724,7 +6718,7 @@
         <v>0</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="H89" s="4"/>
       <c r="I89" s="1"/>
@@ -6739,7 +6733,7 @@
         <v>274</v>
       </c>
       <c r="N89" s="2" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="O89" s="1" t="str">
         <f>LOOKUP(N89,Climate!A:A,Climate!B:B)</f>
@@ -6754,7 +6748,7 @@
         <v xml:space="preserve">Dry, Warm </v>
       </c>
       <c r="R89" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.2">
@@ -6777,7 +6771,7 @@
       </c>
       <c r="F90" s="23"/>
       <c r="G90" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J90" s="13">
         <v>-76.8867008</v>
@@ -6787,10 +6781,10 @@
       </c>
       <c r="L90" s="5"/>
       <c r="M90" s="27" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="N90" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O90" s="1" t="str">
         <f>LOOKUP(N90,Climate!A:A,Climate!B:B)</f>
@@ -6805,7 +6799,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R90" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.2">
@@ -6828,7 +6822,7 @@
       </c>
       <c r="F91" s="23"/>
       <c r="G91" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H91" s="4">
         <v>6241164</v>
@@ -6847,7 +6841,7 @@
         <v>290</v>
       </c>
       <c r="N91" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O91" s="1" t="str">
         <f>LOOKUP(N91,Climate!A:A,Climate!B:B)</f>
@@ -6862,7 +6856,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R91" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.2">
@@ -6885,7 +6879,7 @@
       </c>
       <c r="F92" s="23"/>
       <c r="G92" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="H92" s="4">
         <v>2434021</v>
@@ -6898,10 +6892,10 @@
       </c>
       <c r="L92" s="5"/>
       <c r="M92" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="N92" s="2" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="O92" s="1" t="str">
         <f>LOOKUP(N92,Climate!A:A,Climate!B:B)</f>
@@ -6916,7 +6910,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R92" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.2">
@@ -6939,7 +6933,7 @@
         <v>0</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="I93" s="1" t="s">
         <v>203</v>
@@ -6954,10 +6948,10 @@
         <v>237</v>
       </c>
       <c r="M93" s="27" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="N93" s="2" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="O93" s="1" t="str">
         <f>LOOKUP(N93,Climate!A:A,Climate!B:B)</f>
@@ -6972,7 +6966,7 @@
         <v>Wet</v>
       </c>
       <c r="R93" s="1" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.2">
@@ -6995,7 +6989,7 @@
       </c>
       <c r="F94" s="23"/>
       <c r="G94" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="H94" s="4">
         <v>1673802</v>
@@ -7011,7 +7005,7 @@
         <v>275</v>
       </c>
       <c r="N94" s="2" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="O94" s="1" t="str">
         <f>LOOKUP(N94,Climate!A:A,Climate!B:B)</f>
@@ -7026,7 +7020,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R94" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.2">
@@ -7049,7 +7043,7 @@
       </c>
       <c r="F95" s="23"/>
       <c r="G95" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="J95" s="13">
         <v>-79.931051199999999</v>
@@ -7059,10 +7053,10 @@
       </c>
       <c r="L95" s="5"/>
       <c r="M95" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="N95" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O95" s="1" t="str">
         <f>LOOKUP(N95,Climate!A:A,Climate!B:B)</f>
@@ -7077,7 +7071,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R95" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.2">
@@ -7100,7 +7094,7 @@
       </c>
       <c r="F96" s="23"/>
       <c r="G96" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J96" s="13">
         <v>-81.034814400000002</v>
@@ -7113,7 +7107,7 @@
         <v>276</v>
       </c>
       <c r="N96" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O96" s="1" t="str">
         <f>LOOKUP(N96,Climate!A:A,Climate!B:B)</f>
@@ -7128,7 +7122,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R96" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.2">
@@ -7151,7 +7145,7 @@
         <v>0</v>
       </c>
       <c r="G97" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J97" s="13">
         <v>-100.3537522</v>
@@ -7161,10 +7155,10 @@
       </c>
       <c r="L97" s="5"/>
       <c r="M97" s="27" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="N97" s="2" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="O97" s="1" t="str">
         <f>LOOKUP(N97,Climate!A:A,Climate!B:B)</f>
@@ -7179,7 +7173,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R97" s="1" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.2">
@@ -7202,7 +7196,7 @@
         <v>0</v>
       </c>
       <c r="G98" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="J98" s="13">
         <v>-96.731264999999993</v>
@@ -7212,10 +7206,10 @@
       </c>
       <c r="L98" s="5"/>
       <c r="M98" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="N98" s="2" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="O98" s="1" t="str">
         <f>LOOKUP(N98,Climate!A:A,Climate!B:B)</f>
@@ -7230,7 +7224,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R98" s="1" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.2">
@@ -7255,7 +7249,7 @@
         <v>9.4</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="I99" s="1" t="s">
         <v>192</v>
@@ -7268,10 +7262,10 @@
       </c>
       <c r="L99" s="5"/>
       <c r="M99" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="N99" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O99" s="1" t="str">
         <f>LOOKUP(N99,Climate!A:A,Climate!B:B)</f>
@@ -7286,7 +7280,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R99" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.2">
@@ -7309,7 +7303,7 @@
         <v>0</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H100" s="4">
         <v>1339855</v>
@@ -7322,10 +7316,10 @@
       </c>
       <c r="L100" s="5"/>
       <c r="M100" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="N100" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O100" s="1" t="str">
         <f>LOOKUP(N100,Climate!A:A,Climate!B:B)</f>
@@ -7340,7 +7334,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R100" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.2">
@@ -7365,7 +7359,7 @@
         <v>5.7</v>
       </c>
       <c r="G101" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="H101" s="4">
         <v>2072283</v>
@@ -7381,7 +7375,7 @@
         <v>277</v>
       </c>
       <c r="N101" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O101" s="1" t="str">
         <f>LOOKUP(N101,Climate!A:A,Climate!B:B)</f>
@@ -7396,7 +7390,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R101" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.2">
@@ -7419,7 +7413,7 @@
         <v>0</v>
       </c>
       <c r="G102" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="H102" s="4">
         <v>2421115</v>
@@ -7432,10 +7426,10 @@
       </c>
       <c r="L102" s="5"/>
       <c r="M102" s="27" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="N102" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O102" s="1" t="str">
         <f>LOOKUP(N102,Climate!A:A,Climate!B:B)</f>
@@ -7473,7 +7467,7 @@
         <v>0</v>
       </c>
       <c r="G103" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H103" s="4">
         <v>7943685</v>
@@ -7489,7 +7483,7 @@
         <v>292</v>
       </c>
       <c r="N103" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O103" s="1" t="str">
         <f>LOOKUP(N103,Climate!A:A,Climate!B:B)</f>
@@ -7527,7 +7521,7 @@
         <v>0</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="H104" s="4">
         <v>7368466</v>
@@ -7543,7 +7537,7 @@
         <v>293</v>
       </c>
       <c r="N104" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O104" s="1" t="str">
         <f>LOOKUP(N104,Climate!A:A,Climate!B:B)</f>
@@ -7581,7 +7575,7 @@
         <v>0</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="H105" s="4">
         <v>2655342</v>
@@ -7597,10 +7591,10 @@
       </c>
       <c r="L105" s="5"/>
       <c r="M105" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="N105" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O105" s="1" t="str">
         <f>LOOKUP(N105,Climate!A:A,Climate!B:B)</f>
@@ -7638,7 +7632,7 @@
         <v>0</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="J106" s="13">
         <v>-111.660833</v>
@@ -7651,7 +7645,7 @@
         <v>278</v>
       </c>
       <c r="N106" s="2" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="O106" s="1" t="str">
         <f>LOOKUP(N106,Climate!A:A,Climate!B:B)</f>
@@ -7666,7 +7660,7 @@
         <v xml:space="preserve">Dry, Hot </v>
       </c>
       <c r="R106" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.2">
@@ -7689,7 +7683,7 @@
         <v>0</v>
       </c>
       <c r="G107" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="H107" s="4">
         <v>1266191</v>
@@ -7705,7 +7699,7 @@
         <v>278</v>
       </c>
       <c r="N107" s="2" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="O107" s="1" t="str">
         <f>LOOKUP(N107,Climate!A:A,Climate!B:B)</f>
@@ -7720,7 +7714,7 @@
         <v xml:space="preserve">Dry, Hot </v>
       </c>
       <c r="R107" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.2">
@@ -7743,7 +7737,7 @@
       </c>
       <c r="F108" s="23"/>
       <c r="G108" s="1" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="I108" s="1" t="s">
         <v>202</v>
@@ -7756,10 +7750,10 @@
       </c>
       <c r="L108" s="5"/>
       <c r="M108" s="27" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="N108" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O108" s="1" t="str">
         <f>LOOKUP(N108,Climate!A:A,Climate!B:B)</f>
@@ -7774,7 +7768,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R108" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.2">
@@ -7797,7 +7791,7 @@
       </c>
       <c r="F109" s="23"/>
       <c r="G109" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H109" s="4">
         <v>1787188</v>
@@ -7810,10 +7804,10 @@
       </c>
       <c r="L109" s="5"/>
       <c r="M109" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="N109" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O109" s="1" t="str">
         <f>LOOKUP(N109,Climate!A:A,Climate!B:B)</f>
@@ -7828,7 +7822,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R109" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.2">
@@ -7851,7 +7845,7 @@
       </c>
       <c r="F110" s="23"/>
       <c r="G110" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="H110" s="4">
         <v>1339182</v>
@@ -7870,7 +7864,7 @@
         <v>279</v>
       </c>
       <c r="N110" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O110" s="1" t="str">
         <f>LOOKUP(N110,Climate!A:A,Climate!B:B)</f>
@@ -7885,7 +7879,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R110" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.2">
@@ -7910,7 +7904,7 @@
         <v>4.8</v>
       </c>
       <c r="G111" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="J111" s="13">
         <v>-73.212072000000006</v>
@@ -7920,10 +7914,10 @@
       </c>
       <c r="L111" s="5"/>
       <c r="M111" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="N111" s="2" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="O111" s="1" t="str">
         <f>LOOKUP(N111,Climate!A:A,Climate!B:B)</f>
@@ -7938,7 +7932,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R111" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.2">
@@ -7963,7 +7957,7 @@
         <v>2.7</v>
       </c>
       <c r="G112" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J112" s="13">
         <v>-72.575386899999998</v>
@@ -7973,10 +7967,10 @@
       </c>
       <c r="L112" s="5"/>
       <c r="M112" s="27" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="N112" s="2" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="O112" s="1" t="str">
         <f>LOOKUP(N112,Climate!A:A,Climate!B:B)</f>
@@ -7991,7 +7985,7 @@
         <v>Warm, Wet</v>
       </c>
       <c r="R112" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.2">
@@ -8014,7 +8008,7 @@
         <v>0</v>
       </c>
       <c r="G113" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J113" s="13">
         <v>-122.90069509999999</v>
@@ -8027,7 +8021,7 @@
         <v>280</v>
       </c>
       <c r="N113" s="2" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="O113" s="1" t="str">
         <f>LOOKUP(N113,Climate!A:A,Climate!B:B)</f>
@@ -8042,7 +8036,7 @@
         <v xml:space="preserve">Dry, Warm </v>
       </c>
       <c r="R113" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="114" spans="1:18" x14ac:dyDescent="0.2">
@@ -8064,7 +8058,7 @@
         <v>0</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="I114" s="1" t="s">
         <v>195</v>
@@ -8076,10 +8070,10 @@
         <v>48.113056</v>
       </c>
       <c r="M114" s="27" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="N114" s="2" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="O114" s="1" t="str">
         <f>LOOKUP(N114,Climate!A:A,Climate!B:B)</f>
@@ -8094,7 +8088,7 @@
         <v xml:space="preserve">Dry, Warm </v>
       </c>
       <c r="R114" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="115" spans="1:18" x14ac:dyDescent="0.2">
@@ -8117,7 +8111,7 @@
         <v>0</v>
       </c>
       <c r="G115" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H115" s="4">
         <v>4034248</v>
@@ -8130,10 +8124,10 @@
       </c>
       <c r="L115" s="5"/>
       <c r="M115" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="N115" s="2" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="O115" s="1" t="str">
         <f>LOOKUP(N115,Climate!A:A,Climate!B:B)</f>
@@ -8148,7 +8142,7 @@
         <v xml:space="preserve">Dry, Warm </v>
       </c>
       <c r="R115" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.2">
@@ -8171,7 +8165,7 @@
       </c>
       <c r="F116" s="23"/>
       <c r="G116" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J116" s="13">
         <v>-89.401230200000001</v>
@@ -8184,7 +8178,7 @@
         <v>281</v>
       </c>
       <c r="N116" s="2" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="O116" s="1" t="str">
         <f>LOOKUP(N116,Climate!A:A,Climate!B:B)</f>
@@ -8199,7 +8193,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R116" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.2">
@@ -8222,7 +8216,7 @@
       </c>
       <c r="F117" s="23"/>
       <c r="G117" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H117" s="4">
         <v>1559792</v>
@@ -8235,10 +8229,10 @@
       </c>
       <c r="L117" s="5"/>
       <c r="M117" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="N117" s="2" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="O117" s="1" t="str">
         <f>LOOKUP(N117,Climate!A:A,Climate!B:B)</f>
@@ -8253,7 +8247,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R117" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="118" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -8276,7 +8270,7 @@
       </c>
       <c r="F118" s="23"/>
       <c r="G118" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="H118" s="4"/>
       <c r="I118" s="1"/>
@@ -8291,7 +8285,7 @@
         <v>282</v>
       </c>
       <c r="N118" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O118" s="1" t="str">
         <f>LOOKUP(N118,Climate!A:A,Climate!B:B)</f>
@@ -8306,7 +8300,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R118" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="119" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -8329,7 +8323,7 @@
       </c>
       <c r="F119" s="23"/>
       <c r="G119" s="1" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H119" s="4"/>
       <c r="I119" s="1"/>
@@ -8341,10 +8335,10 @@
       </c>
       <c r="L119" s="5"/>
       <c r="M119" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="N119" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O119" s="1" t="str">
         <f>LOOKUP(N119,Climate!A:A,Climate!B:B)</f>
@@ -8359,7 +8353,7 @@
         <v>Hot, Wet</v>
       </c>
       <c r="R119" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="120" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -8382,7 +8376,7 @@
         <v>0</v>
       </c>
       <c r="G120" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H120" s="4"/>
       <c r="I120" s="1"/>
@@ -8394,10 +8388,10 @@
       </c>
       <c r="L120" s="5"/>
       <c r="M120" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="N120" s="2" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="O120" s="1" t="str">
         <f>LOOKUP(N120,Climate!A:A,Climate!B:B)</f>
@@ -8412,7 +8406,7 @@
         <v>Dry</v>
       </c>
       <c r="R120" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="121" spans="1:18" x14ac:dyDescent="0.2">
@@ -8435,7 +8429,7 @@
         <v>0</v>
       </c>
       <c r="G121" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J121" s="13">
         <v>-104.8202462</v>
@@ -8448,7 +8442,7 @@
         <v>283</v>
       </c>
       <c r="N121" s="2" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="O121" s="1" t="str">
         <f>LOOKUP(N121,Climate!A:A,Climate!B:B)</f>
@@ -8463,7 +8457,7 @@
         <v>Dry</v>
       </c>
       <c r="R121" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
   </sheetData>
@@ -8494,464 +8488,464 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="D13" s="28" t="s">
         <v>410</v>
-      </c>
-      <c r="D13" s="28" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="D18" s="28" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D21" s="28" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="D23" s="28" t="s">
         <v>410</v>
-      </c>
-      <c r="D23" s="28" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D24" s="28" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="D25" s="28" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D26" s="28" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="D27" s="28" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D29" s="28" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="D30" s="28" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="D31" s="28" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="D32" s="28" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D33" s="28" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
   </sheetData>
@@ -9123,17 +9117,17 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="29" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="29" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -9177,7 +9171,7 @@
         <v>240</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -9199,7 +9193,7 @@
         <v>240</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -9210,7 +9204,7 @@
         <v>240</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -9256,7 +9250,7 @@
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="C1" s="3">
         <v>0</v>
@@ -9295,12 +9289,12 @@
         <v>330</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B2" s="3">
         <v>80</v>
@@ -9360,7 +9354,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="B3" s="3">
         <v>50</v>
@@ -9420,7 +9414,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="B4" s="3">
         <v>31</v>
@@ -9540,7 +9534,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -9600,49 +9594,49 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B7" s="3">
         <v>0</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="K7" s="2" t="s">
         <v>443</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="L7" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="F7" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>451</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>449</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>448</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>454</v>
-      </c>
       <c r="O7" s="2" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
   </sheetData>
@@ -9666,10 +9660,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -9677,7 +9671,7 @@
         <v>180</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -9685,7 +9679,7 @@
         <v>150</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -9693,7 +9687,7 @@
         <v>180</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -9701,7 +9695,7 @@
         <v>150</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -9709,7 +9703,7 @@
         <v>180</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -9717,7 +9711,7 @@
         <v>210</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -9725,7 +9719,7 @@
         <v>240</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -9733,7 +9727,7 @@
         <v>120</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -9741,7 +9735,7 @@
         <v>150</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -9749,7 +9743,7 @@
         <v>180</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -9765,7 +9759,7 @@
         <v>240</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -9773,7 +9767,7 @@
         <v>270</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -9781,7 +9775,7 @@
         <v>300</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add weather slider to dendrogram
</commit_message>
<xml_diff>
--- a/io_in/city_list.xlsx
+++ b/io_in/city_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/code/roadtrips/io_in/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE70FB35-A5BE-6042-83FA-C2C71FE264D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7025A200-09B0-0040-8CA1-66EC61F7700C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38640" yWindow="500" windowWidth="24340" windowHeight="21100" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
+    <workbookView xWindow="-23020" yWindow="500" windowWidth="17020" windowHeight="21100" activeTab="3" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="9" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="458">
   <si>
     <t>Boston MA</t>
   </si>
@@ -1946,11 +1946,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418BD67C-5132-6942-B406-D98F46E6A0BD}">
   <dimension ref="A1:R121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C73" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C80" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H87" sqref="H87"/>
+      <selection pane="bottomRight" activeCell="F107" sqref="F107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4062,7 +4062,7 @@
         <v>114</v>
       </c>
       <c r="F39" s="23">
-        <v>6.6</v>
+        <v>7.3</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>452</v>
@@ -4115,7 +4115,7 @@
         <v>114</v>
       </c>
       <c r="F40" s="23">
-        <v>4.9000000000000004</v>
+        <v>10.6</v>
       </c>
       <c r="G40" s="5" t="s">
         <v>452</v>
@@ -5022,7 +5022,9 @@
       <c r="E57" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F57" s="23"/>
+      <c r="F57" s="23">
+        <v>3.9</v>
+      </c>
       <c r="G57" s="5" t="s">
         <v>452</v>
       </c>
@@ -5073,7 +5075,9 @@
       <c r="E58" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F58" s="23"/>
+      <c r="F58" s="23">
+        <v>7.9</v>
+      </c>
       <c r="G58" s="1" t="s">
         <v>453</v>
       </c>
@@ -5127,7 +5131,9 @@
       <c r="E59" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="F59" s="26"/>
+      <c r="F59" s="26">
+        <v>12.4</v>
+      </c>
       <c r="G59" s="5" t="s">
         <v>451</v>
       </c>
@@ -5600,7 +5606,9 @@
       <c r="E68" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F68" s="23"/>
+      <c r="F68" s="23">
+        <v>3.2</v>
+      </c>
       <c r="G68" s="5" t="s">
         <v>452</v>
       </c>
@@ -5651,7 +5659,9 @@
       <c r="E69" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F69" s="23"/>
+      <c r="F69" s="23">
+        <v>4.2</v>
+      </c>
       <c r="G69" s="5" t="s">
         <v>451</v>
       </c>
@@ -6397,7 +6407,9 @@
       <c r="E83" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F83" s="23"/>
+      <c r="F83" s="23">
+        <v>4.7</v>
+      </c>
       <c r="G83" s="5" t="s">
         <v>451</v>
       </c>
@@ -6505,7 +6517,9 @@
       <c r="E85" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F85" s="23"/>
+      <c r="F85" s="23">
+        <v>10.6</v>
+      </c>
       <c r="G85" s="5" t="s">
         <v>452</v>
       </c>
@@ -7048,7 +7062,9 @@
       <c r="E95" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="F95" s="23"/>
+      <c r="F95" s="23">
+        <v>5</v>
+      </c>
       <c r="G95" s="5" t="s">
         <v>451</v>
       </c>
@@ -7099,7 +7115,9 @@
       <c r="E96" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="F96" s="23"/>
+      <c r="F96" s="23">
+        <v>2.6</v>
+      </c>
       <c r="G96" s="5" t="s">
         <v>452</v>
       </c>
@@ -7742,7 +7760,10 @@
       <c r="E108" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F108" s="23"/>
+      <c r="F108" s="23">
+        <f>2.5+3.6</f>
+        <v>6.1</v>
+      </c>
       <c r="G108" s="1" t="s">
         <v>454</v>
       </c>
@@ -7796,7 +7817,9 @@
       <c r="E109" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="F109" s="23"/>
+      <c r="F109" s="23">
+        <v>4.7</v>
+      </c>
       <c r="G109" s="5" t="s">
         <v>451</v>
       </c>
@@ -7850,7 +7873,10 @@
       <c r="E110" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F110" s="23"/>
+      <c r="F110" s="23">
+        <f>7.5+1.5</f>
+        <v>9</v>
+      </c>
       <c r="G110" s="5" t="s">
         <v>452</v>
       </c>
@@ -8275,7 +8301,9 @@
       <c r="E118" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F118" s="23"/>
+      <c r="F118" s="23">
+        <v>3.4</v>
+      </c>
       <c r="G118" s="5" t="s">
         <v>452</v>
       </c>
@@ -8328,7 +8356,9 @@
       <c r="E119" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F119" s="23"/>
+      <c r="F119" s="23">
+        <v>3.3</v>
+      </c>
       <c r="G119" s="1" t="s">
         <v>451</v>
       </c>
@@ -9237,10 +9267,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1D4776-82C5-A549-993A-3BE59A636F7D}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9644,6 +9674,66 @@
       </c>
       <c r="O7" s="2" t="s">
         <v>429</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2" t="str">
+        <f>""&amp;C1</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="str">
+        <f t="shared" ref="D8:O8" si="5">""&amp;D1</f>
+        <v>30</v>
+      </c>
+      <c r="E8" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>60</v>
+      </c>
+      <c r="F8" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>90</v>
+      </c>
+      <c r="G8" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>120</v>
+      </c>
+      <c r="H8" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>150</v>
+      </c>
+      <c r="I8" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>180</v>
+      </c>
+      <c r="J8" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>210</v>
+      </c>
+      <c r="K8" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>240</v>
+      </c>
+      <c r="L8" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>270</v>
+      </c>
+      <c r="M8" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>300</v>
+      </c>
+      <c r="N8" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>330</v>
+      </c>
+      <c r="O8" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>grey</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete High Plains trip
</commit_message>
<xml_diff>
--- a/io_in/city_list.xlsx
+++ b/io_in/city_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/code/roadtrips/io_in/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A49D59-771C-4843-B6CB-12D315D29714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0018478-B901-3B46-9A9F-5E555D78B453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13880" yWindow="500" windowWidth="21960" windowHeight="21900" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1251,7 +1251,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1291,13 +1291,6 @@
       <u/>
       <sz val="12"/>
       <color theme="9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="5"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1411,7 +1404,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1489,65 +1482,26 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <border>
         <bottom style="thin">
@@ -4071,7 +4025,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3A57F64D-E116-4E44-9D34-EEF2E49FD5BA}" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3A57F64D-E116-4E44-9D34-EEF2E49FD5BA}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:C8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>
@@ -4145,13 +4099,13 @@
     <dataField name="Count of photo_date" fld="4" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="4">
-    <format dxfId="7">
+    <format dxfId="3">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="6">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="5">
+    <format dxfId="1">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="17" count="1">
@@ -4160,7 +4114,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="17" count="1">
@@ -4482,10 +4436,10 @@
   <dimension ref="A1:R121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E61" sqref="E61"/>
+      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4582,7 +4536,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="6"/>
-      <c r="F2" s="21">
+      <c r="F2" s="39">
         <v>0</v>
       </c>
       <c r="G2" s="5" t="s">
@@ -4634,7 +4588,7 @@
       <c r="D3" s="12">
         <v>0</v>
       </c>
-      <c r="F3" s="22">
+      <c r="F3" s="40">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -4690,7 +4644,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="6"/>
-      <c r="F4" s="21">
+      <c r="F4" s="39">
         <v>0</v>
       </c>
       <c r="G4" s="5" t="s">
@@ -4852,7 +4806,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="21">
+      <c r="F7" s="39">
         <v>0</v>
       </c>
       <c r="G7" s="5" t="s">
@@ -4904,7 +4858,7 @@
       <c r="D8" s="12">
         <v>0</v>
       </c>
-      <c r="F8" s="22">
+      <c r="F8" s="40">
         <v>0</v>
       </c>
       <c r="G8" s="1" t="s">
@@ -4957,7 +4911,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="6"/>
-      <c r="F9" s="21">
+      <c r="F9" s="39">
         <v>0</v>
       </c>
       <c r="G9" s="5" t="s">
@@ -5011,7 +4965,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="6"/>
-      <c r="F10" s="21">
+      <c r="F10" s="39">
         <v>0</v>
       </c>
       <c r="G10" s="5" t="s">
@@ -5064,7 +5018,7 @@
       <c r="D11" s="12">
         <v>1</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="40">
         <v>0</v>
       </c>
       <c r="G11" s="1" t="s">
@@ -5117,7 +5071,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="6"/>
-      <c r="F12" s="21">
+      <c r="F12" s="39">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -5284,7 +5238,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="6"/>
-      <c r="F15" s="21">
+      <c r="F15" s="39">
         <v>0</v>
       </c>
       <c r="G15" s="5" t="s">
@@ -5395,7 +5349,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="6"/>
-      <c r="F17" s="21">
+      <c r="F17" s="39">
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
@@ -5449,7 +5403,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="6"/>
-      <c r="F18" s="21">
+      <c r="F18" s="39">
         <v>0</v>
       </c>
       <c r="G18" s="1" t="s">
@@ -5502,7 +5456,7 @@
       <c r="D19" s="12">
         <v>0</v>
       </c>
-      <c r="F19" s="22">
+      <c r="F19" s="40">
         <v>0</v>
       </c>
       <c r="G19" s="1" t="s">
@@ -5554,7 +5508,7 @@
       <c r="D20" s="12">
         <v>0</v>
       </c>
-      <c r="F20" s="22">
+      <c r="F20" s="40">
         <v>0</v>
       </c>
       <c r="G20" s="1" t="s">
@@ -5604,7 +5558,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="6"/>
-      <c r="F21" s="21">
+      <c r="F21" s="39">
         <v>0</v>
       </c>
       <c r="G21" s="5" t="s">
@@ -6328,7 +6282,7 @@
         <v>0</v>
       </c>
       <c r="E34" s="15"/>
-      <c r="F34" s="21">
+      <c r="F34" s="39">
         <v>0</v>
       </c>
       <c r="G34" s="5" t="s">
@@ -6490,7 +6444,7 @@
         <v>0</v>
       </c>
       <c r="E37" s="6"/>
-      <c r="F37" s="21">
+      <c r="F37" s="39">
         <v>0</v>
       </c>
       <c r="G37" s="5" t="s">
@@ -6541,7 +6495,7 @@
         <v>0</v>
       </c>
       <c r="E38" s="6"/>
-      <c r="F38" s="21">
+      <c r="F38" s="39">
         <v>0</v>
       </c>
       <c r="G38" s="1" t="s">
@@ -6812,7 +6766,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="6"/>
-      <c r="F43" s="21">
+      <c r="F43" s="39">
         <v>0</v>
       </c>
       <c r="G43" s="5" t="s">
@@ -6972,7 +6926,7 @@
         <v>1</v>
       </c>
       <c r="E46" s="6"/>
-      <c r="F46" s="21">
+      <c r="F46" s="39">
         <v>0</v>
       </c>
       <c r="G46" s="5" t="s">
@@ -7136,7 +7090,9 @@
       <c r="E49" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F49" s="21"/>
+      <c r="F49" s="21">
+        <v>7.3</v>
+      </c>
       <c r="G49" s="5" t="s">
         <v>382</v>
       </c>
@@ -7187,7 +7143,9 @@
       <c r="E50" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="F50" s="21"/>
+      <c r="F50" s="21">
+        <v>7.5</v>
+      </c>
       <c r="G50" s="5" t="s">
         <v>381</v>
       </c>
@@ -7498,18 +7456,18 @@
       <c r="B56" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C56" s="39" t="str">
+      <c r="C56" s="1" t="str">
         <f t="shared" si="3"/>
         <v>MN</v>
       </c>
-      <c r="D56" s="36">
+      <c r="D56" s="5">
         <v>1</v>
       </c>
-      <c r="E56" s="37" t="s">
+      <c r="E56" s="15" t="s">
         <v>398</v>
       </c>
-      <c r="F56" s="38">
-        <v>0</v>
+      <c r="F56" s="21">
+        <v>18.100000000000001</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>382</v>
@@ -7731,7 +7689,7 @@
         <v>1</v>
       </c>
       <c r="E60" s="6"/>
-      <c r="F60" s="21">
+      <c r="F60" s="39">
         <v>0</v>
       </c>
       <c r="G60" s="5" t="s">
@@ -7782,7 +7740,7 @@
         <v>0</v>
       </c>
       <c r="E61" s="6"/>
-      <c r="F61" s="21">
+      <c r="F61" s="39">
         <v>0</v>
       </c>
       <c r="G61" s="5" t="s">
@@ -7832,7 +7790,7 @@
       <c r="D62" s="12">
         <v>0</v>
       </c>
-      <c r="F62" s="22">
+      <c r="F62" s="40">
         <v>0</v>
       </c>
       <c r="G62" s="1" t="s">
@@ -7885,7 +7843,7 @@
         <v>0</v>
       </c>
       <c r="E63" s="6"/>
-      <c r="F63" s="21">
+      <c r="F63" s="39">
         <v>0</v>
       </c>
       <c r="G63" s="5" t="s">
@@ -8037,18 +7995,18 @@
       <c r="B66" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C66" s="39" t="str">
+      <c r="C66" s="1" t="str">
         <f t="shared" ref="C66:C97" si="5">RIGHT(B66,2)</f>
         <v>ND</v>
       </c>
-      <c r="D66" s="36">
+      <c r="D66" s="5">
         <v>1</v>
       </c>
-      <c r="E66" s="37" t="s">
+      <c r="E66" s="15" t="s">
         <v>398</v>
       </c>
-      <c r="F66" s="38">
-        <v>0</v>
+      <c r="F66" s="21">
+        <v>5.6</v>
       </c>
       <c r="G66" s="5" t="s">
         <v>382</v>
@@ -8090,18 +8048,18 @@
       <c r="B67" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C67" s="39" t="str">
+      <c r="C67" s="1" t="str">
         <f t="shared" si="5"/>
         <v>ND</v>
       </c>
-      <c r="D67" s="36">
+      <c r="D67" s="5">
         <v>1</v>
       </c>
-      <c r="E67" s="37" t="s">
+      <c r="E67" s="15" t="s">
         <v>398</v>
       </c>
-      <c r="F67" s="38">
-        <v>0</v>
+      <c r="F67" s="21">
+        <v>4</v>
       </c>
       <c r="G67" s="5" t="s">
         <v>381</v>
@@ -8207,7 +8165,8 @@
         <v>110</v>
       </c>
       <c r="F69" s="21">
-        <v>4.2</v>
+        <f>4.2+2.4</f>
+        <v>6.6</v>
       </c>
       <c r="G69" s="5" t="s">
         <v>381</v>
@@ -8573,7 +8532,7 @@
         <v>0</v>
       </c>
       <c r="E76" s="6"/>
-      <c r="F76" s="21">
+      <c r="F76" s="39">
         <v>0</v>
       </c>
       <c r="G76" s="5" t="s">
@@ -9065,7 +9024,7 @@
         <v>0</v>
       </c>
       <c r="E85" s="6"/>
-      <c r="F85" s="21">
+      <c r="F85" s="39">
         <v>0</v>
       </c>
       <c r="G85" s="5" t="s">
@@ -9119,7 +9078,7 @@
         <v>0</v>
       </c>
       <c r="E86" s="6"/>
-      <c r="F86" s="21">
+      <c r="F86" s="39">
         <v>0</v>
       </c>
       <c r="G86" s="5" t="s">
@@ -9173,7 +9132,7 @@
         <v>1</v>
       </c>
       <c r="E87" s="6"/>
-      <c r="F87" s="21">
+      <c r="F87" s="39">
         <v>0</v>
       </c>
       <c r="G87" s="5" t="s">
@@ -9227,7 +9186,7 @@
         <v>0</v>
       </c>
       <c r="E88" s="6"/>
-      <c r="F88" s="21">
+      <c r="F88" s="39">
         <v>0</v>
       </c>
       <c r="G88" s="5" t="s">
@@ -9442,7 +9401,7 @@
         <v>1</v>
       </c>
       <c r="E92" s="6"/>
-      <c r="F92" s="21">
+      <c r="F92" s="39">
         <v>0</v>
       </c>
       <c r="G92" s="5" t="s">
@@ -9652,18 +9611,18 @@
       <c r="B96" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C96" s="39" t="str">
+      <c r="C96" s="1" t="str">
         <f t="shared" si="5"/>
         <v>SD</v>
       </c>
-      <c r="D96" s="36">
+      <c r="D96" s="5">
         <v>1</v>
       </c>
-      <c r="E96" s="37" t="s">
+      <c r="E96" s="15" t="s">
         <v>398</v>
       </c>
-      <c r="F96" s="38">
-        <v>0</v>
+      <c r="F96" s="21">
+        <v>3.3</v>
       </c>
       <c r="G96" s="5" t="s">
         <v>382</v>
@@ -9705,18 +9664,18 @@
       <c r="B97" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C97" s="39" t="str">
+      <c r="C97" s="1" t="str">
         <f t="shared" si="5"/>
         <v>SD</v>
       </c>
-      <c r="D97" s="40">
+      <c r="D97" s="12">
         <v>1</v>
       </c>
-      <c r="E97" s="37" t="s">
+      <c r="E97" s="15" t="s">
         <v>398</v>
       </c>
-      <c r="F97" s="41">
-        <v>0</v>
+      <c r="F97" s="22">
+        <v>7.1</v>
       </c>
       <c r="G97" s="1" t="s">
         <v>384</v>
@@ -9760,18 +9719,18 @@
       <c r="B98" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C98" s="39" t="str">
-        <f t="shared" ref="C98:C129" si="7">RIGHT(B98,2)</f>
+      <c r="C98" s="1" t="str">
+        <f t="shared" ref="C98:C121" si="7">RIGHT(B98,2)</f>
         <v>SD</v>
       </c>
-      <c r="D98" s="36">
+      <c r="D98" s="5">
         <v>1</v>
       </c>
-      <c r="E98" s="37" t="s">
+      <c r="E98" s="15" t="s">
         <v>398</v>
       </c>
-      <c r="F98" s="38">
-        <v>0</v>
+      <c r="F98" s="21">
+        <v>2.1</v>
       </c>
       <c r="G98" s="5" t="s">
         <v>381</v>
@@ -9877,7 +9836,7 @@
         <v>0</v>
       </c>
       <c r="E100" s="6"/>
-      <c r="F100" s="21">
+      <c r="F100" s="39">
         <v>0</v>
       </c>
       <c r="G100" s="1" t="s">
@@ -9987,7 +9946,7 @@
         <v>1</v>
       </c>
       <c r="E102" s="6"/>
-      <c r="F102" s="21">
+      <c r="F102" s="39">
         <v>0</v>
       </c>
       <c r="G102" s="5" t="s">
@@ -10041,7 +10000,7 @@
         <v>1</v>
       </c>
       <c r="E103" s="6"/>
-      <c r="F103" s="21">
+      <c r="F103" s="39">
         <v>0</v>
       </c>
       <c r="G103" s="5" t="s">
@@ -10095,7 +10054,7 @@
         <v>1</v>
       </c>
       <c r="E104" s="6"/>
-      <c r="F104" s="21">
+      <c r="F104" s="39">
         <v>0</v>
       </c>
       <c r="G104" s="1" t="s">
@@ -10149,7 +10108,7 @@
         <v>1</v>
       </c>
       <c r="E105" s="6"/>
-      <c r="F105" s="21">
+      <c r="F105" s="39">
         <v>0</v>
       </c>
       <c r="G105" s="1" t="s">
@@ -10206,7 +10165,7 @@
         <v>0</v>
       </c>
       <c r="E106" s="6"/>
-      <c r="F106" s="21">
+      <c r="F106" s="39">
         <v>0</v>
       </c>
       <c r="G106" s="1" t="s">
@@ -10257,7 +10216,7 @@
         <v>0</v>
       </c>
       <c r="E107" s="6"/>
-      <c r="F107" s="21">
+      <c r="F107" s="39">
         <v>0</v>
       </c>
       <c r="G107" s="5" t="s">
@@ -10590,7 +10549,7 @@
         <v>0</v>
       </c>
       <c r="E113" s="6"/>
-      <c r="F113" s="21">
+      <c r="F113" s="39">
         <v>0</v>
       </c>
       <c r="G113" s="5" t="s">
@@ -10640,7 +10599,7 @@
       <c r="D114" s="12">
         <v>0</v>
       </c>
-      <c r="F114" s="22">
+      <c r="F114" s="40">
         <v>0</v>
       </c>
       <c r="G114" s="1" t="s">
@@ -10693,7 +10652,7 @@
         <v>1</v>
       </c>
       <c r="E115" s="6"/>
-      <c r="F115" s="21">
+      <c r="F115" s="39">
         <v>0</v>
       </c>
       <c r="G115" s="5" t="s">
@@ -10963,7 +10922,7 @@
         <v>0</v>
       </c>
       <c r="E120" s="6"/>
-      <c r="F120" s="21">
+      <c r="F120" s="39">
         <v>0</v>
       </c>
       <c r="G120" s="5" t="s">
@@ -11014,7 +10973,7 @@
         <v>0</v>
       </c>
       <c r="E121" s="6"/>
-      <c r="F121" s="21">
+      <c r="F121" s="39">
         <v>0</v>
       </c>
       <c r="G121" s="5" t="s">
@@ -11565,12 +11524,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="38" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
@@ -11645,12 +11604,12 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="38" t="s">
         <v>166</v>
       </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
@@ -11663,12 +11622,12 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="38" t="s">
         <v>173</v>
       </c>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
@@ -12490,10 +12449,10 @@
       <c r="A2" s="30" t="s">
         <v>389</v>
       </c>
-      <c r="B2" s="42">
+      <c r="B2">
         <v>26</v>
       </c>
-      <c r="C2" s="42">
+      <c r="C2">
         <v>25</v>
       </c>
       <c r="D2" s="2">
@@ -12505,10 +12464,10 @@
       <c r="A3" s="30" t="s">
         <v>349</v>
       </c>
-      <c r="B3" s="42">
+      <c r="B3">
         <v>22</v>
       </c>
-      <c r="C3" s="42">
+      <c r="C3">
         <v>22</v>
       </c>
       <c r="D3" s="2">
@@ -12520,10 +12479,10 @@
       <c r="A4" s="30" t="s">
         <v>353</v>
       </c>
-      <c r="B4" s="42">
+      <c r="B4">
         <v>5</v>
       </c>
-      <c r="C4" s="42"/>
+      <c r="C4"/>
       <c r="D4" s="2">
         <f>GETPIVOTDATA("Count of region",$A$1,"region","Oconus")-GETPIVOTDATA("Count of photo_date",$A$1,"region","Oconus")</f>
         <v>5</v>
@@ -12533,10 +12492,10 @@
       <c r="A5" s="30" t="s">
         <v>352</v>
       </c>
-      <c r="B5" s="42">
+      <c r="B5">
         <v>25</v>
       </c>
-      <c r="C5" s="42">
+      <c r="C5">
         <v>23</v>
       </c>
       <c r="D5" s="2">
@@ -12548,10 +12507,10 @@
       <c r="A6" s="30" t="s">
         <v>171</v>
       </c>
-      <c r="B6" s="42">
+      <c r="B6">
         <v>20</v>
       </c>
-      <c r="C6" s="42">
+      <c r="C6">
         <v>8</v>
       </c>
       <c r="D6" s="2">
@@ -12563,23 +12522,23 @@
       <c r="A7" s="32" t="s">
         <v>388</v>
       </c>
-      <c r="B7" s="45">
+      <c r="B7" s="37">
         <v>22</v>
       </c>
-      <c r="C7" s="45"/>
+      <c r="C7" s="37"/>
       <c r="D7" s="33">
         <f>GETPIVOTDATA("Count of region",$A$1,"region","West")-GETPIVOTDATA("Count of photo_date",$A$1,"region","West")</f>
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="36" t="s">
         <v>394</v>
       </c>
-      <c r="B8" s="43">
+      <c r="B8" s="35">
         <v>120</v>
       </c>
-      <c r="C8" s="43">
+      <c r="C8" s="35">
         <v>78</v>
       </c>
       <c r="D8" s="34">

</xml_diff>

<commit_message>
Add San Juan PR to list of photographed cities
</commit_message>
<xml_diff>
--- a/io_in/city_list.xlsx
+++ b/io_in/city_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/code/roadtrips/io_in/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0018478-B901-3B46-9A9F-5E555D78B453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD9FD14-6B0F-BB4B-B347-4CEC9AC9DF94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13880" yWindow="500" windowWidth="21960" windowHeight="21900" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
+    <workbookView xWindow="7920" yWindow="500" windowWidth="22800" windowHeight="18700" xr2:uid="{724935DA-9DBD-364F-92E1-C441C90E19CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="9" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="400">
   <si>
     <t>Boston MA</t>
   </si>
@@ -1240,6 +1240,9 @@
   </si>
   <si>
     <t>2024-09</t>
+  </si>
+  <si>
+    <t>2025-01</t>
   </si>
 </sst>
 </file>
@@ -1404,7 +1407,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1487,14 +1490,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4436,10 +4442,10 @@
   <dimension ref="A1:R121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C80" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomRight" activeCell="G91" sqref="G91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4536,9 +4542,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="6"/>
-      <c r="F2" s="39">
-        <v>0</v>
-      </c>
+      <c r="F2" s="38"/>
       <c r="G2" s="5" t="s">
         <v>381</v>
       </c>
@@ -4588,9 +4592,7 @@
       <c r="D3" s="12">
         <v>0</v>
       </c>
-      <c r="F3" s="40">
-        <v>0</v>
-      </c>
+      <c r="F3" s="39"/>
       <c r="G3" s="1" t="s">
         <v>384</v>
       </c>
@@ -4644,9 +4646,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="6"/>
-      <c r="F4" s="39">
-        <v>0</v>
-      </c>
+      <c r="F4" s="38"/>
       <c r="G4" s="5" t="s">
         <v>382</v>
       </c>
@@ -4806,9 +4806,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="39">
-        <v>0</v>
-      </c>
+      <c r="F7" s="38"/>
       <c r="G7" s="5" t="s">
         <v>382</v>
       </c>
@@ -4858,9 +4856,7 @@
       <c r="D8" s="12">
         <v>0</v>
       </c>
-      <c r="F8" s="40">
-        <v>0</v>
-      </c>
+      <c r="F8" s="39"/>
       <c r="G8" s="1" t="s">
         <v>384</v>
       </c>
@@ -4911,9 +4907,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="6"/>
-      <c r="F9" s="39">
-        <v>0</v>
-      </c>
+      <c r="F9" s="38"/>
       <c r="G9" s="5" t="s">
         <v>382</v>
       </c>
@@ -4965,9 +4959,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="6"/>
-      <c r="F10" s="39">
-        <v>0</v>
-      </c>
+      <c r="F10" s="38"/>
       <c r="G10" s="5" t="s">
         <v>381</v>
       </c>
@@ -5018,9 +5010,7 @@
       <c r="D11" s="12">
         <v>1</v>
       </c>
-      <c r="F11" s="40">
-        <v>0</v>
-      </c>
+      <c r="F11" s="39"/>
       <c r="G11" s="1" t="s">
         <v>384</v>
       </c>
@@ -5071,9 +5061,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="6"/>
-      <c r="F12" s="39">
-        <v>0</v>
-      </c>
+      <c r="F12" s="38"/>
       <c r="G12" s="1" t="s">
         <v>383</v>
       </c>
@@ -5238,9 +5226,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="6"/>
-      <c r="F15" s="39">
-        <v>0</v>
-      </c>
+      <c r="F15" s="38"/>
       <c r="G15" s="5" t="s">
         <v>382</v>
       </c>
@@ -5349,9 +5335,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="6"/>
-      <c r="F17" s="39">
-        <v>0</v>
-      </c>
+      <c r="F17" s="38"/>
       <c r="G17" s="1" t="s">
         <v>383</v>
       </c>
@@ -5403,9 +5387,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="6"/>
-      <c r="F18" s="39">
-        <v>0</v>
-      </c>
+      <c r="F18" s="38"/>
       <c r="G18" s="1" t="s">
         <v>383</v>
       </c>
@@ -5456,9 +5438,7 @@
       <c r="D19" s="12">
         <v>0</v>
       </c>
-      <c r="F19" s="40">
-        <v>0</v>
-      </c>
+      <c r="F19" s="39"/>
       <c r="G19" s="1" t="s">
         <v>384</v>
       </c>
@@ -5508,9 +5488,7 @@
       <c r="D20" s="12">
         <v>0</v>
       </c>
-      <c r="F20" s="40">
-        <v>0</v>
-      </c>
+      <c r="F20" s="39"/>
       <c r="G20" s="1" t="s">
         <v>381</v>
       </c>
@@ -5558,9 +5536,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="6"/>
-      <c r="F21" s="39">
-        <v>0</v>
-      </c>
+      <c r="F21" s="38"/>
       <c r="G21" s="5" t="s">
         <v>382</v>
       </c>
@@ -6282,9 +6258,7 @@
         <v>0</v>
       </c>
       <c r="E34" s="15"/>
-      <c r="F34" s="39">
-        <v>0</v>
-      </c>
+      <c r="F34" s="38"/>
       <c r="G34" s="5" t="s">
         <v>382</v>
       </c>
@@ -6444,9 +6418,7 @@
         <v>0</v>
       </c>
       <c r="E37" s="6"/>
-      <c r="F37" s="39">
-        <v>0</v>
-      </c>
+      <c r="F37" s="38"/>
       <c r="G37" s="5" t="s">
         <v>382</v>
       </c>
@@ -6495,9 +6467,7 @@
         <v>0</v>
       </c>
       <c r="E38" s="6"/>
-      <c r="F38" s="39">
-        <v>0</v>
-      </c>
+      <c r="F38" s="38"/>
       <c r="G38" s="1" t="s">
         <v>381</v>
       </c>
@@ -6766,9 +6736,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="6"/>
-      <c r="F43" s="39">
-        <v>0</v>
-      </c>
+      <c r="F43" s="38"/>
       <c r="G43" s="5" t="s">
         <v>381</v>
       </c>
@@ -6926,9 +6894,7 @@
         <v>1</v>
       </c>
       <c r="E46" s="6"/>
-      <c r="F46" s="39">
-        <v>0</v>
-      </c>
+      <c r="F46" s="38"/>
       <c r="G46" s="5" t="s">
         <v>382</v>
       </c>
@@ -7361,7 +7327,9 @@
       <c r="E54" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="F54" s="21"/>
+      <c r="F54" s="21">
+        <v>2.8</v>
+      </c>
       <c r="G54" s="1" t="s">
         <v>383</v>
       </c>
@@ -7415,7 +7383,9 @@
       <c r="E55" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="F55" s="21"/>
+      <c r="F55" s="21">
+        <v>3.7</v>
+      </c>
       <c r="G55" s="5" t="s">
         <v>382</v>
       </c>
@@ -7689,9 +7659,7 @@
         <v>1</v>
       </c>
       <c r="E60" s="6"/>
-      <c r="F60" s="39">
-        <v>0</v>
-      </c>
+      <c r="F60" s="38"/>
       <c r="G60" s="5" t="s">
         <v>382</v>
       </c>
@@ -7740,9 +7708,7 @@
         <v>0</v>
       </c>
       <c r="E61" s="6"/>
-      <c r="F61" s="39">
-        <v>0</v>
-      </c>
+      <c r="F61" s="38"/>
       <c r="G61" s="5" t="s">
         <v>381</v>
       </c>
@@ -7790,9 +7756,7 @@
       <c r="D62" s="12">
         <v>0</v>
       </c>
-      <c r="F62" s="40">
-        <v>0</v>
-      </c>
+      <c r="F62" s="39"/>
       <c r="G62" s="1" t="s">
         <v>384</v>
       </c>
@@ -7843,9 +7807,7 @@
         <v>0</v>
       </c>
       <c r="E63" s="6"/>
-      <c r="F63" s="39">
-        <v>0</v>
-      </c>
+      <c r="F63" s="38"/>
       <c r="G63" s="5" t="s">
         <v>382</v>
       </c>
@@ -7896,7 +7858,9 @@
       <c r="E64" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="F64" s="21"/>
+      <c r="F64" s="21">
+        <v>4</v>
+      </c>
       <c r="G64" s="5" t="s">
         <v>381</v>
       </c>
@@ -7950,7 +7914,9 @@
       <c r="E65" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="F65" s="21"/>
+      <c r="F65" s="21">
+        <v>3.1</v>
+      </c>
       <c r="G65" s="5" t="s">
         <v>382</v>
       </c>
@@ -8218,7 +8184,9 @@
       <c r="E70" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="F70" s="21"/>
+      <c r="F70" s="21">
+        <v>1</v>
+      </c>
       <c r="G70" s="5" t="s">
         <v>382</v>
       </c>
@@ -8269,7 +8237,9 @@
       <c r="E71" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="F71" s="21"/>
+      <c r="F71" s="21">
+        <v>1.8</v>
+      </c>
       <c r="G71" s="1" t="s">
         <v>381</v>
       </c>
@@ -8532,9 +8502,7 @@
         <v>0</v>
       </c>
       <c r="E76" s="6"/>
-      <c r="F76" s="39">
-        <v>0</v>
-      </c>
+      <c r="F76" s="38"/>
       <c r="G76" s="5" t="s">
         <v>382</v>
       </c>
@@ -8641,7 +8609,9 @@
       <c r="E78" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="F78" s="21"/>
+      <c r="F78" s="21">
+        <v>5.0999999999999996</v>
+      </c>
       <c r="G78" s="5" t="s">
         <v>382</v>
       </c>
@@ -8692,7 +8662,9 @@
       <c r="E79" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="F79" s="21"/>
+      <c r="F79" s="21">
+        <v>7.3</v>
+      </c>
       <c r="G79" s="1" t="s">
         <v>383</v>
       </c>
@@ -8806,7 +8778,9 @@
       <c r="E81" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="F81" s="21"/>
+      <c r="F81" s="21">
+        <v>3.5</v>
+      </c>
       <c r="G81" s="1" t="s">
         <v>383</v>
       </c>
@@ -8916,7 +8890,9 @@
       <c r="E83" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="F83" s="21"/>
+      <c r="F83" s="21">
+        <v>6.5</v>
+      </c>
       <c r="G83" s="1" t="s">
         <v>383</v>
       </c>
@@ -9024,9 +9000,7 @@
         <v>0</v>
       </c>
       <c r="E85" s="6"/>
-      <c r="F85" s="39">
-        <v>0</v>
-      </c>
+      <c r="F85" s="38"/>
       <c r="G85" s="5" t="s">
         <v>382</v>
       </c>
@@ -9078,9 +9052,7 @@
         <v>0</v>
       </c>
       <c r="E86" s="6"/>
-      <c r="F86" s="39">
-        <v>0</v>
-      </c>
+      <c r="F86" s="38"/>
       <c r="G86" s="5" t="s">
         <v>381</v>
       </c>
@@ -9132,9 +9104,7 @@
         <v>1</v>
       </c>
       <c r="E87" s="6"/>
-      <c r="F87" s="39">
-        <v>0</v>
-      </c>
+      <c r="F87" s="38"/>
       <c r="G87" s="5" t="s">
         <v>381</v>
       </c>
@@ -9186,9 +9156,7 @@
         <v>0</v>
       </c>
       <c r="E88" s="6"/>
-      <c r="F88" s="39">
-        <v>0</v>
-      </c>
+      <c r="F88" s="38"/>
       <c r="G88" s="5" t="s">
         <v>382</v>
       </c>
@@ -9241,7 +9209,9 @@
       <c r="E89" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="F89" s="21"/>
+      <c r="F89" s="21">
+        <v>7.7</v>
+      </c>
       <c r="G89" s="5" t="s">
         <v>382</v>
       </c>
@@ -9292,7 +9262,9 @@
       <c r="E90" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="F90" s="21"/>
+      <c r="F90" s="21">
+        <v>26.2</v>
+      </c>
       <c r="G90" s="5" t="s">
         <v>381</v>
       </c>
@@ -9349,7 +9321,9 @@
       <c r="E91" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="F91" s="21"/>
+      <c r="F91" s="21">
+        <v>7.7</v>
+      </c>
       <c r="G91" s="1" t="s">
         <v>383</v>
       </c>
@@ -9400,9 +9374,11 @@
       <c r="D92" s="5">
         <v>1</v>
       </c>
-      <c r="E92" s="6"/>
-      <c r="F92" s="39">
-        <v>0</v>
+      <c r="E92" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="F92" s="21">
+        <v>32</v>
       </c>
       <c r="G92" s="5" t="s">
         <v>383</v>
@@ -9836,9 +9812,7 @@
         <v>0</v>
       </c>
       <c r="E100" s="6"/>
-      <c r="F100" s="39">
-        <v>0</v>
-      </c>
+      <c r="F100" s="38"/>
       <c r="G100" s="1" t="s">
         <v>381</v>
       </c>
@@ -9946,9 +9920,7 @@
         <v>1</v>
       </c>
       <c r="E102" s="6"/>
-      <c r="F102" s="39">
-        <v>0</v>
-      </c>
+      <c r="F102" s="38"/>
       <c r="G102" s="5" t="s">
         <v>382</v>
       </c>
@@ -10000,9 +9972,7 @@
         <v>1</v>
       </c>
       <c r="E103" s="6"/>
-      <c r="F103" s="39">
-        <v>0</v>
-      </c>
+      <c r="F103" s="38"/>
       <c r="G103" s="5" t="s">
         <v>381</v>
       </c>
@@ -10054,9 +10024,7 @@
         <v>1</v>
       </c>
       <c r="E104" s="6"/>
-      <c r="F104" s="39">
-        <v>0</v>
-      </c>
+      <c r="F104" s="38"/>
       <c r="G104" s="1" t="s">
         <v>383</v>
       </c>
@@ -10108,9 +10076,7 @@
         <v>1</v>
       </c>
       <c r="E105" s="6"/>
-      <c r="F105" s="39">
-        <v>0</v>
-      </c>
+      <c r="F105" s="38"/>
       <c r="G105" s="1" t="s">
         <v>383</v>
       </c>
@@ -10165,9 +10131,7 @@
         <v>0</v>
       </c>
       <c r="E106" s="6"/>
-      <c r="F106" s="39">
-        <v>0</v>
-      </c>
+      <c r="F106" s="38"/>
       <c r="G106" s="1" t="s">
         <v>381</v>
       </c>
@@ -10216,9 +10180,7 @@
         <v>0</v>
       </c>
       <c r="E107" s="6"/>
-      <c r="F107" s="39">
-        <v>0</v>
-      </c>
+      <c r="F107" s="38"/>
       <c r="G107" s="5" t="s">
         <v>382</v>
       </c>
@@ -10549,9 +10511,7 @@
         <v>0</v>
       </c>
       <c r="E113" s="6"/>
-      <c r="F113" s="39">
-        <v>0</v>
-      </c>
+      <c r="F113" s="38"/>
       <c r="G113" s="5" t="s">
         <v>382</v>
       </c>
@@ -10599,9 +10559,7 @@
       <c r="D114" s="12">
         <v>0</v>
       </c>
-      <c r="F114" s="40">
-        <v>0</v>
-      </c>
+      <c r="F114" s="39"/>
       <c r="G114" s="1" t="s">
         <v>384</v>
       </c>
@@ -10652,9 +10610,7 @@
         <v>1</v>
       </c>
       <c r="E115" s="6"/>
-      <c r="F115" s="39">
-        <v>0</v>
-      </c>
+      <c r="F115" s="38"/>
       <c r="G115" s="5" t="s">
         <v>381</v>
       </c>
@@ -10708,7 +10664,9 @@
       <c r="E116" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="F116" s="21"/>
+      <c r="F116" s="21">
+        <v>8.9</v>
+      </c>
       <c r="G116" s="5" t="s">
         <v>382</v>
       </c>
@@ -10759,7 +10717,9 @@
       <c r="E117" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="F117" s="21"/>
+      <c r="F117" s="21">
+        <v>5.6</v>
+      </c>
       <c r="G117" s="5" t="s">
         <v>381</v>
       </c>
@@ -10922,9 +10882,7 @@
         <v>0</v>
       </c>
       <c r="E120" s="6"/>
-      <c r="F120" s="39">
-        <v>0</v>
-      </c>
+      <c r="F120" s="38"/>
       <c r="G120" s="5" t="s">
         <v>381</v>
       </c>
@@ -10969,13 +10927,11 @@
         <f t="shared" si="7"/>
         <v>WY</v>
       </c>
-      <c r="D121" s="5">
+      <c r="D121" s="40">
         <v>0</v>
       </c>
       <c r="E121" s="6"/>
-      <c r="F121" s="39">
-        <v>0</v>
-      </c>
+      <c r="F121" s="38"/>
       <c r="G121" s="5" t="s">
         <v>382</v>
       </c>
@@ -11524,12 +11480,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="41" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
@@ -11604,12 +11560,12 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="41" t="s">
         <v>166</v>
       </c>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
@@ -11622,12 +11578,12 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="41" t="s">
         <v>173</v>
       </c>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">

</xml_diff>